<commit_message>
adds 4.2_Residuals+VIF.R and corresponding R project to calculate the variance inflation factor and create residual plots; adds the residual plots in reports/figures; adds VIF results as new sheet to Model_results.xlsx; adds _index.csv for each crop which are needed for the R calculations
</commit_message>
<xml_diff>
--- a/reports/Model_results.xlsx
+++ b/reports/Model_results.xlsx
@@ -1,44 +1,237 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Model_results" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Model_statistics" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Model_results" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Model_statistics" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Model_VIF" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+  <si>
+    <t>Corn</t>
+  </si>
+  <si>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>Soybean</t>
+  </si>
+  <si>
+    <t>Wheat</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>+-95%Confidence_Interval</t>
+  </si>
+  <si>
+    <t>Odds_ratios</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>C(thz_class)[T.2]</t>
+  </si>
+  <si>
+    <t>C(thz_class)[T.3]</t>
+  </si>
+  <si>
+    <t>C(thz_class)[T.4]</t>
+  </si>
+  <si>
+    <t>C(thz_class)[T.5]</t>
+  </si>
+  <si>
+    <t>C(thz_class)[T.6]</t>
+  </si>
+  <si>
+    <t>C(thz_class)[T.7]</t>
+  </si>
+  <si>
+    <t>C(mst_class)[T.3]</t>
+  </si>
+  <si>
+    <t>C(mst_class)[T.4]</t>
+  </si>
+  <si>
+    <t>C(mst_class)[T.5]</t>
+  </si>
+  <si>
+    <t>C(mst_class)[T.6]</t>
+  </si>
+  <si>
+    <t>C(soil_class)[T.2]</t>
+  </si>
+  <si>
+    <t>C(soil_class)[T.3]</t>
+  </si>
+  <si>
+    <t>C(soil_class)[T.4]</t>
+  </si>
+  <si>
+    <t>C(soil_class)[T.5]</t>
+  </si>
+  <si>
+    <t>C(soil_class)[T.6]</t>
+  </si>
+  <si>
+    <t>n_total</t>
+  </si>
+  <si>
+    <t>p_fertilizer</t>
+  </si>
+  <si>
+    <t>irrigation_tot</t>
+  </si>
+  <si>
+    <t>mechanized</t>
+  </si>
+  <si>
+    <t>pesticides</t>
+  </si>
+  <si>
+    <t>McFaddens_roh</t>
+  </si>
+  <si>
+    <t>RootMeanGammaDeviance</t>
+  </si>
+  <si>
+    <t>AIC</t>
+  </si>
+  <si>
+    <t>BIC</t>
+  </si>
+  <si>
+    <t>Calibration</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">row.names</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corn.GVIF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corn.Df</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corn.GVIF..1..2.Df..</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rice.GVIF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rice.Df</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rice.GVIF..1..2.Df..</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soybean.GVIF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soybean.Df</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soybean.GVIF..1..2.Df..</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wheat.GVIF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wheat.Df</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wheat.GVIF..1..2.Df..</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p_fertilizer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">irrigation_tot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mechanized</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pesticides</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thz_class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mst_class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soil_class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corn.GVIF2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rice.GVIF2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soybean.GVIF2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wheat.GVIF2</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <b/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -47,143 +240,72 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:Q9" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:Q9"/>
+  <tableColumns count="17">
+    <tableColumn id="1" name="row.names"/>
+    <tableColumn id="2" name="Corn.Df"/>
+    <tableColumn id="3" name="Corn.GVIF"/>
+    <tableColumn id="4" name="Corn.GVIF..1..2.Df.."/>
+    <tableColumn id="5" name="Corn.GVIF2"/>
+    <tableColumn id="6" name="Rice.Df"/>
+    <tableColumn id="7" name="Rice.GVIF"/>
+    <tableColumn id="8" name="Rice.GVIF..1..2.Df.."/>
+    <tableColumn id="9" name="Rice.GVIF2"/>
+    <tableColumn id="10" name="Soybean.Df"/>
+    <tableColumn id="11" name="Soybean.GVIF"/>
+    <tableColumn id="12" name="Soybean.GVIF..1..2.Df.."/>
+    <tableColumn id="13" name="Soybean.GVIF2"/>
+    <tableColumn id="14" name="Wheat.Df"/>
+    <tableColumn id="15" name="Wheat.GVIF"/>
+    <tableColumn id="16" name="Wheat.GVIF..1..2.Df.."/>
+    <tableColumn id="17" name="Wheat.GVIF2"/>
+  </tableColumns>
+  <tableStyleInfo name="none" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -470,325 +592,271 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:Q24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr"/>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Wheat</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="n"/>
-      <c r="D1" s="1" t="n"/>
-      <c r="E1" s="1" t="n"/>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Corn</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="n"/>
-      <c r="H1" s="1" t="n"/>
-      <c r="I1" s="1" t="n"/>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Soybean</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="n"/>
-      <c r="L1" s="1" t="n"/>
-      <c r="M1" s="1" t="n"/>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Rice</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="n"/>
-      <c r="P1" s="1" t="n"/>
-      <c r="Q1" s="1" t="n"/>
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr"/>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>Coefficients</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>+-95%Confidence_Interval</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>Odds_ratios</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>p-value</t>
-        </is>
-      </c>
-      <c r="F2" s="1" t="inlineStr">
-        <is>
-          <t>Coefficients</t>
-        </is>
-      </c>
-      <c r="G2" s="1" t="inlineStr">
-        <is>
-          <t>+-95%Confidence_Interval</t>
-        </is>
-      </c>
-      <c r="H2" s="1" t="inlineStr">
-        <is>
-          <t>Odds_ratios</t>
-        </is>
-      </c>
-      <c r="I2" s="1" t="inlineStr">
-        <is>
-          <t>p-value</t>
-        </is>
-      </c>
-      <c r="J2" s="1" t="inlineStr">
-        <is>
-          <t>Coefficients</t>
-        </is>
-      </c>
-      <c r="K2" s="1" t="inlineStr">
-        <is>
-          <t>+-95%Confidence_Interval</t>
-        </is>
-      </c>
-      <c r="L2" s="1" t="inlineStr">
-        <is>
-          <t>Odds_ratios</t>
-        </is>
-      </c>
-      <c r="M2" s="1" t="inlineStr">
-        <is>
-          <t>p-value</t>
-        </is>
-      </c>
-      <c r="N2" s="1" t="inlineStr">
-        <is>
-          <t>Coefficients</t>
-        </is>
-      </c>
-      <c r="O2" s="1" t="inlineStr">
-        <is>
-          <t>+-95%Confidence_Interval</t>
-        </is>
-      </c>
-      <c r="P2" s="1" t="inlineStr">
-        <is>
-          <t>Odds_ratios</t>
-        </is>
-      </c>
-      <c r="Q2" s="1" t="inlineStr">
-        <is>
-          <t>p-value</t>
-        </is>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Intercept</t>
-        </is>
+      <c r="A4" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B4" t="n">
-        <v>6.498038789327854</v>
+        <v>6.4980387893278539</v>
       </c>
       <c r="C4" t="n">
-        <v>0.02521356821630592</v>
+        <v>2.521356821630592E-2</v>
       </c>
       <c r="D4" t="n">
-        <v>663.8384285221698</v>
+        <v>663.83842852216981</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>6.626383191030197</v>
+        <v>6.6263831910301967</v>
       </c>
       <c r="G4" t="n">
-        <v>0.02399145068646372</v>
+        <v>2.399145068646372E-2</v>
       </c>
       <c r="H4" t="n">
-        <v>754.7474507933468</v>
+        <v>754.74745079334684</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>6.406625842951103</v>
+        <v>6.4066258429511027</v>
       </c>
       <c r="K4" t="n">
-        <v>0.04376919664803752</v>
+        <v>4.3769196648037523E-2</v>
       </c>
       <c r="L4" t="n">
-        <v>605.8460088390894</v>
+        <v>605.84600883908945</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>7.401874530574021</v>
+        <v>7.4018745305740206</v>
       </c>
       <c r="O4" t="n">
-        <v>0.02588184745239167</v>
+        <v>2.5881847452391669E-2</v>
       </c>
       <c r="P4" t="n">
-        <v>1639.054008939526</v>
+        <v>1639.0540089395261</v>
       </c>
       <c r="Q4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>C(thz_class)[T.2]</t>
-        </is>
+      <c r="A5" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B5" t="n">
-        <v>0.003131165845131262</v>
+        <v>3.1311658451312618E-3</v>
       </c>
       <c r="C5" t="n">
-        <v>0.02346832751923398</v>
+        <v>2.3468327519233979E-2</v>
       </c>
       <c r="D5" t="n">
-        <v>1.003136073065343</v>
+        <v>1.0031360730653429</v>
       </c>
       <c r="E5" t="n">
-        <v>0.789590938423563</v>
+        <v>0.78959093842356298</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1438897880480912</v>
+        <v>0.14388978804809119</v>
       </c>
       <c r="G5" t="n">
-        <v>0.01320666843727629</v>
+        <v>1.3206668437276289E-2</v>
       </c>
       <c r="H5" t="n">
         <v>1.154756833506827</v>
       </c>
       <c r="I5" t="n">
-        <v>2.856733592169026e-105</v>
+        <v>2.8567335921690261E-105</v>
       </c>
       <c r="J5" t="n">
         <v>0.1633912825627313</v>
       </c>
       <c r="K5" t="n">
-        <v>0.02280184585840695</v>
+        <v>2.2801845858406951E-2</v>
       </c>
       <c r="L5" t="n">
         <v>1.177497333735952</v>
       </c>
       <c r="M5" t="n">
-        <v>1.392673409602758e-46</v>
+        <v>1.392673409602758E-46</v>
       </c>
       <c r="N5" t="n">
-        <v>0.3100000194259448</v>
+        <v>0.31000001942594479</v>
       </c>
       <c r="O5" t="n">
-        <v>0.02760238292084189</v>
+        <v>2.7602382920841891E-2</v>
       </c>
       <c r="P5" t="n">
-        <v>1.363425140617999</v>
+        <v>1.3634251406179989</v>
       </c>
       <c r="Q5" t="n">
-        <v>9.806455545049278e-112</v>
+        <v>9.8064555450492781E-112</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>C(thz_class)[T.3]</t>
-        </is>
+      <c r="A6" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B6" t="n">
-        <v>0.2137759410906344</v>
+        <v>0.21377594109063441</v>
       </c>
       <c r="C6" t="n">
-        <v>0.01735248342823488</v>
+        <v>1.735248342823488E-2</v>
       </c>
       <c r="D6" t="n">
         <v>1.238345161440894</v>
       </c>
       <c r="E6" t="n">
-        <v>4.800544786868342e-134</v>
+        <v>4.8005447868683417E-134</v>
       </c>
       <c r="F6" t="n">
-        <v>0.08975961304354596</v>
+        <v>8.975961304354596E-2</v>
       </c>
       <c r="G6" t="n">
-        <v>0.01264886734401076</v>
+        <v>1.264886734401076E-2</v>
       </c>
       <c r="H6" t="n">
         <v>1.093911290090704</v>
       </c>
       <c r="I6" t="n">
-        <v>1.019378204942127e-45</v>
+        <v>1.019378204942127E-45</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.0406988412384227</v>
+        <v>-4.0698841238422698E-2</v>
       </c>
       <c r="K6" t="n">
-        <v>0.0126285596025383</v>
+        <v>1.26285596025383E-2</v>
       </c>
       <c r="L6" t="n">
-        <v>0.9601182344308888</v>
+        <v>0.96011823443088884</v>
       </c>
       <c r="M6" t="n">
-        <v>1.152017860315702e-10</v>
+        <v>1.152017860315702E-10</v>
       </c>
       <c r="N6" t="n">
         <v>-0.129434953420793</v>
       </c>
       <c r="O6" t="n">
-        <v>0.0113254644901495</v>
+        <v>1.1325464490149499E-2</v>
       </c>
       <c r="P6" t="n">
-        <v>0.8785917359445433</v>
+        <v>0.87859173594454332</v>
       </c>
       <c r="Q6" t="n">
-        <v>1.235523025736801e-115</v>
+        <v>1.2355230257368011E-115</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>C(thz_class)[T.4]</t>
-        </is>
+      <c r="A7" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.1023613020831547</v>
+        <v>-0.10236130208315471</v>
       </c>
       <c r="C7" t="n">
-        <v>0.01737490275791886</v>
+        <v>1.7374902757918861E-2</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9027033441439863</v>
+        <v>0.90270334414398634</v>
       </c>
       <c r="E7" t="n">
-        <v>4.795435350110615e-32</v>
+        <v>4.7954353501106148E-32</v>
       </c>
       <c r="F7" t="n">
-        <v>0.5488077736144407</v>
+        <v>0.54880777361444066</v>
       </c>
       <c r="G7" t="n">
-        <v>0.01201477637240038</v>
+        <v>1.2014776372400379E-2</v>
       </c>
       <c r="H7" t="n">
         <v>1.731187819223424</v>
@@ -797,53 +865,51 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>0.07437815605728687</v>
+        <v>7.4378156057286871E-2</v>
       </c>
       <c r="K7" t="n">
-        <v>0.01239321234839729</v>
+        <v>1.2393212348397291E-2</v>
       </c>
       <c r="L7" t="n">
         <v>1.077214083514717</v>
       </c>
       <c r="M7" t="n">
-        <v>3.424520148944059e-33</v>
+        <v>3.4245201489440592E-33</v>
       </c>
       <c r="N7" t="n">
-        <v>0.2995081967522047</v>
+        <v>0.29950819675220469</v>
       </c>
       <c r="O7" t="n">
-        <v>0.01444585608967676</v>
+        <v>1.4445856089676761E-2</v>
       </c>
       <c r="P7" t="n">
-        <v>1.349195105849082</v>
+        <v>1.3491951058490821</v>
       </c>
       <c r="Q7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>C(thz_class)[T.5]</t>
-        </is>
+      <c r="A8" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B8" t="n">
         <v>-0.1185193741271747</v>
       </c>
       <c r="C8" t="n">
-        <v>0.01783629328238733</v>
+        <v>1.7836293282387328E-2</v>
       </c>
       <c r="D8" t="n">
-        <v>0.8882346067198693</v>
+        <v>0.88823460671986931</v>
       </c>
       <c r="E8" t="n">
-        <v>2.656886049778536e-40</v>
+        <v>2.656886049778536E-40</v>
       </c>
       <c r="F8" t="n">
-        <v>0.6783116131459639</v>
+        <v>0.67831161314596389</v>
       </c>
       <c r="G8" t="n">
-        <v>0.01607716414747894</v>
+        <v>1.607716414747894E-2</v>
       </c>
       <c r="H8" t="n">
         <v>1.97054787485061</v>
@@ -855,74 +921,72 @@
         <v>0.1414323576934178</v>
       </c>
       <c r="K8" t="n">
-        <v>0.02162003775765273</v>
+        <v>2.162003775765273E-2</v>
       </c>
       <c r="L8" t="n">
         <v>1.151922582924936</v>
       </c>
       <c r="M8" t="n">
-        <v>4.094188704041516e-39</v>
+        <v>4.0941887040415162E-39</v>
       </c>
       <c r="N8" t="n">
-        <v>0.270406944401079</v>
+        <v>0.27040694440107899</v>
       </c>
       <c r="O8" t="n">
-        <v>0.022236313839934</v>
+        <v>2.2236313839934001E-2</v>
       </c>
       <c r="P8" t="n">
-        <v>1.310497641914311</v>
+        <v>1.3104976419143111</v>
       </c>
       <c r="Q8" t="n">
-        <v>1.169757516185512e-130</v>
+        <v>1.1697575161855121E-130</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>C(thz_class)[T.6]</t>
-        </is>
+      <c r="A9" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B9" t="n">
-        <v>0.1730082112949592</v>
+        <v>0.17300821129495919</v>
       </c>
       <c r="C9" t="n">
-        <v>0.01760296517197624</v>
+        <v>1.760296517197624E-2</v>
       </c>
       <c r="D9" t="n">
         <v>1.188875867254368</v>
       </c>
       <c r="E9" t="n">
-        <v>5.065061882416507e-86</v>
+        <v>5.0650618824165067E-86</v>
       </c>
       <c r="F9" t="n">
-        <v>0.6994157896396183</v>
+        <v>0.69941578963961826</v>
       </c>
       <c r="G9" t="n">
-        <v>0.01106359174692289</v>
+        <v>1.1063591746922889E-2</v>
       </c>
       <c r="H9" t="n">
-        <v>2.012576595857271</v>
+        <v>2.0125765958572708</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>0.2432079763544457</v>
+        <v>0.24320797635444569</v>
       </c>
       <c r="K9" t="n">
-        <v>0.01217057597894632</v>
+        <v>1.2170575978946319E-2</v>
       </c>
       <c r="L9" t="n">
-        <v>1.275333835820497</v>
+        <v>1.2753338358204971</v>
       </c>
       <c r="M9" t="n">
         <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>0.3546508420498622</v>
+        <v>0.35465084204986219</v>
       </c>
       <c r="O9" t="n">
-        <v>0.01644634589550434</v>
+        <v>1.6446345895504338E-2</v>
       </c>
       <c r="P9" t="n">
         <v>1.425682778891338</v>
@@ -932,263 +996,253 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>C(thz_class)[T.7]</t>
-        </is>
+      <c r="A10" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B10" t="n">
-        <v>0.06573163185190448</v>
+        <v>6.5731631851904476E-2</v>
       </c>
       <c r="C10" t="n">
-        <v>0.01733727497422259</v>
+        <v>1.7337274974222591E-2</v>
       </c>
       <c r="D10" t="n">
-        <v>1.067940077604346</v>
+        <v>1.0679400776043459</v>
       </c>
       <c r="E10" t="n">
-        <v>3.3845052972799e-14</v>
+        <v>3.3845052972799E-14</v>
       </c>
       <c r="F10" t="n">
-        <v>0.748326692475199</v>
+        <v>0.74832669247519901</v>
       </c>
       <c r="G10" t="n">
-        <v>0.01104366448693379</v>
+        <v>1.104366448693379E-2</v>
       </c>
       <c r="H10" t="n">
-        <v>2.113460586658116</v>
+        <v>2.1134605866581162</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0790581603722551</v>
+        <v>7.9058160372255104E-2</v>
       </c>
       <c r="K10" t="n">
-        <v>0.01377589548552769</v>
+        <v>1.3775895485527691E-2</v>
       </c>
       <c r="L10" t="n">
-        <v>1.082267265306926</v>
+        <v>1.0822672653069261</v>
       </c>
       <c r="M10" t="n">
-        <v>1.706588204236379e-30</v>
+        <v>1.7065882042363791E-30</v>
       </c>
       <c r="N10" t="n">
-        <v>0.3622222861895384</v>
+        <v>0.36222228618953839</v>
       </c>
       <c r="O10" t="n">
-        <v>0.02474715225317137</v>
+        <v>2.4747152253171371E-2</v>
       </c>
       <c r="P10" t="n">
         <v>1.436518224635329</v>
       </c>
       <c r="Q10" t="n">
-        <v>2.232281451476795e-188</v>
+        <v>2.2322814514767949E-188</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>C(mst_class)[T.3]</t>
-        </is>
+      <c r="A11" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B11" t="n">
-        <v>0.02561415238434558</v>
+        <v>2.5614152384345581E-2</v>
       </c>
       <c r="C11" t="n">
-        <v>0.00770547756585684</v>
+        <v>7.7054775658568402E-3</v>
       </c>
       <c r="D11" t="n">
-        <v>1.02594501365579</v>
+        <v>1.0259450136557899</v>
       </c>
       <c r="E11" t="n">
-        <v>2.965031898692152e-11</v>
+        <v>2.9650318986921517E-11</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.0937015401520401</v>
+        <v>-9.3701540152040103E-2</v>
       </c>
       <c r="G11" t="n">
-        <v>0.01301071279675365</v>
+        <v>1.301071279675365E-2</v>
       </c>
       <c r="H11" t="n">
-        <v>0.9105544856428314</v>
+        <v>0.91055448564283137</v>
       </c>
       <c r="I11" t="n">
-        <v>4.900907344318166e-47</v>
+        <v>4.9009073443181664E-47</v>
       </c>
       <c r="J11" t="n">
-        <v>0.2256555015532528</v>
+        <v>0.22565550155325281</v>
       </c>
       <c r="K11" t="n">
-        <v>0.02349568268124088</v>
+        <v>2.349568268124088E-2</v>
       </c>
       <c r="L11" t="n">
-        <v>1.253143884786743</v>
+        <v>1.2531438847867431</v>
       </c>
       <c r="M11" t="n">
-        <v>3.15716364016927e-82</v>
+        <v>3.1571636401692701E-82</v>
       </c>
       <c r="N11" t="n">
-        <v>-0.08702285863256454</v>
+        <v>-8.7022858632564537E-2</v>
       </c>
       <c r="O11" t="n">
-        <v>0.01696685798576265</v>
+        <v>1.696685798576265E-2</v>
       </c>
       <c r="P11" t="n">
-        <v>0.9166561418877308</v>
+        <v>0.91665614188773081</v>
       </c>
       <c r="Q11" t="n">
-        <v>1.089603544049179e-24</v>
+        <v>1.0896035440491791E-24</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>C(mst_class)[T.4]</t>
-        </is>
+      <c r="A12" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B12" t="n">
-        <v>0.284499151982661</v>
+        <v>0.28449915198266101</v>
       </c>
       <c r="C12" t="n">
-        <v>0.008639113412911762</v>
+        <v>8.6391134129117624E-3</v>
       </c>
       <c r="D12" t="n">
-        <v>1.329096186202878</v>
+        <v>1.3290961862028781</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.06423340576183081</v>
+        <v>6.4233405761830814E-2</v>
       </c>
       <c r="G12" t="n">
-        <v>0.01345877315736073</v>
+        <v>1.3458773157360731E-2</v>
       </c>
       <c r="H12" t="n">
-        <v>1.066341259911704</v>
+        <v>1.0663412599117039</v>
       </c>
       <c r="I12" t="n">
-        <v>1.358325744594069e-21</v>
+        <v>1.3583257445940689E-21</v>
       </c>
       <c r="J12" t="n">
-        <v>0.2991122983497493</v>
+        <v>0.29911229834974928</v>
       </c>
       <c r="K12" t="n">
-        <v>0.0240622307467625</v>
+        <v>2.4062230746762499E-2</v>
       </c>
       <c r="L12" t="n">
-        <v>1.348661067381539</v>
+        <v>1.3486610673815389</v>
       </c>
       <c r="M12" t="n">
-        <v>1.939171649622361e-136</v>
+        <v>1.9391716496223612E-136</v>
       </c>
       <c r="N12" t="n">
-        <v>-0.05337964920882654</v>
+        <v>-5.3379649208826541E-2</v>
       </c>
       <c r="O12" t="n">
-        <v>0.0176740460346055</v>
+        <v>1.7674046034605501E-2</v>
       </c>
       <c r="P12" t="n">
-        <v>0.9480200290989196</v>
+        <v>0.94802002909891958</v>
       </c>
       <c r="Q12" t="n">
-        <v>1.536792347685073e-09</v>
+        <v>1.536792347685073E-9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>C(mst_class)[T.5]</t>
-        </is>
+      <c r="A13" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B13" t="n">
-        <v>0.4611029103811264</v>
+        <v>0.46110291038112639</v>
       </c>
       <c r="C13" t="n">
-        <v>0.009563435055568139</v>
+        <v>9.563435055568139E-3</v>
       </c>
       <c r="D13" t="n">
-        <v>1.585822040434054</v>
+        <v>1.5858220404340539</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.271929992836308</v>
+        <v>0.27192999283630798</v>
       </c>
       <c r="G13" t="n">
-        <v>0.0136903887307876</v>
+        <v>1.36903887307876E-2</v>
       </c>
       <c r="H13" t="n">
-        <v>1.312495114034469</v>
+        <v>1.3124951140344689</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>0.4528512035603207</v>
+        <v>0.45285120356032071</v>
       </c>
       <c r="K13" t="n">
-        <v>0.02379718821351485</v>
+        <v>2.3797188213514849E-2</v>
       </c>
       <c r="L13" t="n">
-        <v>1.572790143528506</v>
+        <v>1.5727901435285061</v>
       </c>
       <c r="M13" t="n">
         <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>-0.04365442256223725</v>
+        <v>-4.3654422562237248E-2</v>
       </c>
       <c r="O13" t="n">
-        <v>0.01811877904956566</v>
+        <v>1.8118779049565659E-2</v>
       </c>
       <c r="P13" t="n">
-        <v>0.9572847163178325</v>
+        <v>0.95728471631783252</v>
       </c>
       <c r="Q13" t="n">
-        <v>1.445012476831519e-06</v>
+        <v>1.445012476831519E-6</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>C(mst_class)[T.6]</t>
-        </is>
+      <c r="A14" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B14" t="n">
-        <v>0.5503954066702998</v>
+        <v>0.55039540667029985</v>
       </c>
       <c r="C14" t="n">
-        <v>0.01008745187397105</v>
+        <v>1.0087451873971051E-2</v>
       </c>
       <c r="D14" t="n">
-        <v>1.733938493183803</v>
+        <v>1.7339384931838031</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2566522874963661</v>
+        <v>0.25665228749636609</v>
       </c>
       <c r="G14" t="n">
-        <v>0.01342472257340252</v>
+        <v>1.342472257340252E-2</v>
       </c>
       <c r="H14" t="n">
-        <v>1.292595596959112</v>
+        <v>1.2925955969591121</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>0.4481294383233159</v>
+        <v>0.44812943832331592</v>
       </c>
       <c r="K14" t="n">
-        <v>0.02375532394999963</v>
+        <v>2.3755323949999629E-2</v>
       </c>
       <c r="L14" t="n">
-        <v>1.565381302871863</v>
+        <v>1.5653813028718631</v>
       </c>
       <c r="M14" t="n">
         <v>0</v>
@@ -1197,249 +1251,239 @@
         <v>0.1021667134295864</v>
       </c>
       <c r="O14" t="n">
-        <v>0.01713607865695863</v>
+        <v>1.7136078656958629E-2</v>
       </c>
       <c r="P14" t="n">
-        <v>1.107568102814186</v>
+        <v>1.1075681028141859</v>
       </c>
       <c r="Q14" t="n">
-        <v>8.856773176199827e-33</v>
+        <v>8.8567731761998265E-33</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>C(soil_class)[T.2]</t>
-        </is>
+      <c r="A15" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B15" t="n">
         <v>0.6355214754207088</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0235055531112102</v>
+        <v>2.3505553111210199E-2</v>
       </c>
       <c r="D15" t="n">
-        <v>1.888006433743653</v>
+        <v>1.8880064337436531</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.9207986608071315</v>
+        <v>0.92079866080713146</v>
       </c>
       <c r="G15" t="n">
-        <v>0.02693684843565091</v>
+        <v>2.6936848435650911E-2</v>
       </c>
       <c r="H15" t="n">
-        <v>2.511295262324382</v>
+        <v>2.5112952623243818</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>0.4897620679931707</v>
+        <v>0.48976206799317068</v>
       </c>
       <c r="K15" t="n">
-        <v>0.03941499206919688</v>
+        <v>3.941499206919688E-2</v>
       </c>
       <c r="L15" t="n">
-        <v>1.63192788588177</v>
+        <v>1.6319278858817701</v>
       </c>
       <c r="M15" t="n">
-        <v>2.48723203113967e-136</v>
+        <v>2.48723203113967E-136</v>
       </c>
       <c r="N15" t="n">
-        <v>0.4945858412584265</v>
+        <v>0.49458584125842647</v>
       </c>
       <c r="O15" t="n">
-        <v>0.02910726716718742</v>
+        <v>2.9107267167187419E-2</v>
       </c>
       <c r="P15" t="n">
-        <v>1.639818953046632</v>
+        <v>1.6398189530466321</v>
       </c>
       <c r="Q15" t="n">
-        <v>3.883250656949213e-253</v>
+        <v>3.8832506569492132E-253</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>C(soil_class)[T.3]</t>
-        </is>
+      <c r="A16" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B16" t="n">
-        <v>0.6522860679445137</v>
+        <v>0.65228606794451371</v>
       </c>
       <c r="C16" t="n">
-        <v>0.01907177959802331</v>
+        <v>1.9071779598023308E-2</v>
       </c>
       <c r="D16" t="n">
-        <v>1.919924894726258</v>
+        <v>1.9199248947262579</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.9016139048859644</v>
+        <v>0.90161390488596438</v>
       </c>
       <c r="G16" t="n">
-        <v>0.0203730609635784</v>
+        <v>2.0373060963578399E-2</v>
       </c>
       <c r="H16" t="n">
-        <v>2.463575881610082</v>
+        <v>2.4635758816100819</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>0.56132943490094</v>
+        <v>0.56132943490094001</v>
       </c>
       <c r="K16" t="n">
-        <v>0.03630368711418908</v>
+        <v>3.6303687114189083E-2</v>
       </c>
       <c r="L16" t="n">
-        <v>1.753001453170712</v>
+        <v>1.7530014531707121</v>
       </c>
       <c r="M16" t="n">
-        <v>5.666109233642553e-210</v>
+        <v>5.6661092336425533E-210</v>
       </c>
       <c r="N16" t="n">
-        <v>0.4749615107163253</v>
+        <v>0.47496151071632531</v>
       </c>
       <c r="O16" t="n">
-        <v>0.02201780537977128</v>
+        <v>2.2017805379771278E-2</v>
       </c>
       <c r="P16" t="n">
-        <v>1.607952307362244</v>
+        <v>1.6079523073622439</v>
       </c>
       <c r="Q16" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>C(soil_class)[T.4]</t>
-        </is>
+      <c r="A17" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B17" t="n">
-        <v>0.5018969915945826</v>
+        <v>0.50189699159458256</v>
       </c>
       <c r="C17" t="n">
-        <v>0.01896947200638264</v>
+        <v>1.8969472006382639E-2</v>
       </c>
       <c r="D17" t="n">
-        <v>1.651851849494483</v>
+        <v>1.6518518494944829</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>0.6443256763603922</v>
+        <v>0.64432567636039217</v>
       </c>
       <c r="G17" t="n">
-        <v>0.01992753340592882</v>
+        <v>1.9927533405928819E-2</v>
       </c>
       <c r="H17" t="n">
-        <v>1.904702210401852</v>
+        <v>1.9047022104018521</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>0.4025243368690578</v>
+        <v>0.40252433686905781</v>
       </c>
       <c r="K17" t="n">
-        <v>0.03587478035144256</v>
+        <v>3.5874780351442558E-2</v>
       </c>
       <c r="L17" t="n">
-        <v>1.495595322889575</v>
+        <v>1.4955953228895751</v>
       </c>
       <c r="M17" t="n">
-        <v>1.583873594546386e-111</v>
+        <v>1.5838735945463861E-111</v>
       </c>
       <c r="N17" t="n">
-        <v>0.3377725560984647</v>
+        <v>0.33777255609846468</v>
       </c>
       <c r="O17" t="n">
-        <v>0.02054552437298099</v>
+        <v>2.0545524372980989E-2</v>
       </c>
       <c r="P17" t="n">
-        <v>1.401821631362851</v>
+        <v>1.4018216313628511</v>
       </c>
       <c r="Q17" t="n">
-        <v>4.189744576021895e-237</v>
+        <v>4.1897445760218947E-237</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>C(soil_class)[T.5]</t>
-        </is>
+      <c r="A18" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B18" t="n">
         <v>0.2927297893328295</v>
       </c>
       <c r="C18" t="n">
-        <v>0.02185234332425468</v>
+        <v>2.1852343324254678E-2</v>
       </c>
       <c r="D18" t="n">
         <v>1.340080637421982</v>
       </c>
       <c r="E18" t="n">
-        <v>4.04647950138541e-158</v>
+        <v>4.0464795013854104E-158</v>
       </c>
       <c r="F18" t="n">
-        <v>0.3825689311226341</v>
+        <v>0.38256893112263413</v>
       </c>
       <c r="G18" t="n">
-        <v>0.02222070144067543</v>
+        <v>2.2220701440675429E-2</v>
       </c>
       <c r="H18" t="n">
         <v>1.466045927066274</v>
       </c>
       <c r="I18" t="n">
-        <v>7.936109466381916e-260</v>
+        <v>7.9361094663819158E-260</v>
       </c>
       <c r="J18" t="n">
         <v>0.1656867639595033</v>
       </c>
       <c r="K18" t="n">
-        <v>0.03767989978223271</v>
+        <v>3.7679899782232712E-2</v>
       </c>
       <c r="L18" t="n">
         <v>1.180203361590366</v>
       </c>
       <c r="M18" t="n">
-        <v>1.437662226471549e-18</v>
+        <v>1.437662226471549E-18</v>
       </c>
       <c r="N18" t="n">
-        <v>0.05723762032020107</v>
+        <v>5.723762032020107E-2</v>
       </c>
       <c r="O18" t="n">
-        <v>0.02222352602079982</v>
+        <v>2.2223526020799821E-2</v>
       </c>
       <c r="P18" t="n">
         <v>1.058907398418178</v>
       </c>
       <c r="Q18" t="n">
-        <v>2.58985689532663e-07</v>
+        <v>2.5898568953266302E-7</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>C(soil_class)[T.6]</t>
-        </is>
+      <c r="A19" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B19" t="n">
         <v>0.7279966944041083</v>
       </c>
       <c r="C19" t="n">
-        <v>0.02013467709853975</v>
+        <v>2.0134677098539749E-2</v>
       </c>
       <c r="D19" t="n">
-        <v>2.070927748193028</v>
+        <v>2.0709277481930282</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -1448,50 +1492,48 @@
         <v>0.9270893244424766</v>
       </c>
       <c r="G19" t="n">
-        <v>0.02186576090100962</v>
+        <v>2.1865760901009619E-2</v>
       </c>
       <c r="H19" t="n">
-        <v>2.52714276951695</v>
+        <v>2.5271427695169502</v>
       </c>
       <c r="I19" t="n">
         <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>0.5154035774721351</v>
+        <v>0.51540357747213505</v>
       </c>
       <c r="K19" t="n">
-        <v>0.03700678512442015</v>
+        <v>3.7006785124420148E-2</v>
       </c>
       <c r="L19" t="n">
         <v>1.674314080908438</v>
       </c>
       <c r="M19" t="n">
-        <v>9.489112261697848e-171</v>
+        <v>9.4891122616978476E-171</v>
       </c>
       <c r="N19" t="n">
-        <v>0.4270155660577014</v>
+        <v>0.42701556605770141</v>
       </c>
       <c r="O19" t="n">
-        <v>0.02166586795462824</v>
+        <v>2.1665867954628239E-2</v>
       </c>
       <c r="P19" t="n">
-        <v>1.532676519269471</v>
+        <v>1.5326765192694709</v>
       </c>
       <c r="Q19" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>n_total</t>
-        </is>
+      <c r="A20" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B20" t="n">
-        <v>0.003203178145427554</v>
+        <v>3.2031781454275542E-3</v>
       </c>
       <c r="C20" t="n">
-        <v>7.496258230593035e-05</v>
+        <v>7.4962582305930354E-5</v>
       </c>
       <c r="D20" t="n">
         <v>1.003208313802554</v>
@@ -1500,65 +1542,63 @@
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.0009411451073333683</v>
+        <v>-9.4114510733336832E-4</v>
       </c>
       <c r="G20" t="n">
-        <v>7.44880413323333e-05</v>
+        <v>7.4488041332333304E-5</v>
       </c>
       <c r="H20" t="n">
-        <v>0.9990592976308187</v>
+        <v>0.99905929763081869</v>
       </c>
       <c r="I20" t="n">
-        <v>6.880934130649236e-141</v>
+        <v>6.8809341306492362E-141</v>
       </c>
       <c r="J20" t="n">
-        <v>-0.001726933737854424</v>
+        <v>-1.726933737854424E-3</v>
       </c>
       <c r="K20" t="n">
-        <v>7.787894251647931e-05</v>
+        <v>7.7878942516479308E-5</v>
       </c>
       <c r="L20" t="n">
-        <v>0.998274556554211</v>
+        <v>0.99827455655421105</v>
       </c>
       <c r="M20" t="n">
         <v>0</v>
       </c>
       <c r="N20" t="n">
-        <v>0.0009722374505679556</v>
+        <v>9.7223745056795559E-4</v>
       </c>
       <c r="O20" t="n">
-        <v>9.720506524447982e-05</v>
+        <v>9.7205065244479824E-5</v>
       </c>
       <c r="P20" t="n">
-        <v>1.000972710226603</v>
+        <v>1.0009727102266031</v>
       </c>
       <c r="Q20" t="n">
-        <v>5.0987675228035e-89</v>
+        <v>5.0987675228034997E-89</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>p_fertilizer</t>
-        </is>
+      <c r="A21" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.01401602792773995</v>
+        <v>-1.4016027927739949E-2</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0004929134330041681</v>
+        <v>4.929134330041681E-4</v>
       </c>
       <c r="D21" t="n">
-        <v>0.9860817392893387</v>
+        <v>0.98608173928933873</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0113229561056198</v>
+        <v>1.13229561056198E-2</v>
       </c>
       <c r="G21" t="n">
-        <v>0.0004502626415283321</v>
+        <v>4.5026264152833208E-4</v>
       </c>
       <c r="H21" t="n">
         <v>1.011387303411005</v>
@@ -1567,10 +1607,10 @@
         <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>0.01318683074725847</v>
+        <v>1.318683074725847E-2</v>
       </c>
       <c r="K21" t="n">
-        <v>0.0004466497138747139</v>
+        <v>4.4664971387471393E-4</v>
       </c>
       <c r="L21" t="n">
         <v>1.013274160444948</v>
@@ -1579,29 +1619,27 @@
         <v>0</v>
       </c>
       <c r="N21" t="n">
-        <v>0.004746883377796711</v>
+        <v>4.7468833777967109E-3</v>
       </c>
       <c r="O21" t="n">
-        <v>0.0006894144671805433</v>
+        <v>6.8941446718054334E-4</v>
       </c>
       <c r="P21" t="n">
-        <v>1.004758167676716</v>
+        <v>1.0047581676767161</v>
       </c>
       <c r="Q21" t="n">
-        <v>3.821285630095189e-43</v>
+        <v>3.8212856300951887E-43</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>irrigation_tot</t>
-        </is>
+      <c r="A22" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B22" t="n">
-        <v>0.4199043420301316</v>
+        <v>0.41990434203013161</v>
       </c>
       <c r="C22" t="n">
-        <v>0.01326047267865058</v>
+        <v>1.3260472678650581E-2</v>
       </c>
       <c r="D22" t="n">
         <v>1.521815974829098</v>
@@ -1610,56 +1648,54 @@
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>0.5242107950030375</v>
+        <v>0.52421079500303747</v>
       </c>
       <c r="G22" t="n">
-        <v>0.01553214349130438</v>
+        <v>1.5532143491304381E-2</v>
       </c>
       <c r="H22" t="n">
-        <v>1.689125256116848</v>
+        <v>1.6891252561168479</v>
       </c>
       <c r="I22" t="n">
         <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>0.2141759209920092</v>
+        <v>0.21417592099200919</v>
       </c>
       <c r="K22" t="n">
-        <v>0.01876151570242937</v>
+        <v>1.8761515702429371E-2</v>
       </c>
       <c r="L22" t="n">
-        <v>1.2388405736873</v>
+        <v>1.2388405736873001</v>
       </c>
       <c r="M22" t="n">
-        <v>2.236305433369659e-115</v>
+        <v>2.236305433369659E-115</v>
       </c>
       <c r="N22" t="n">
-        <v>0.4729836278530679</v>
+        <v>0.47298362785306791</v>
       </c>
       <c r="O22" t="n">
-        <v>0.01371872711883708</v>
+        <v>1.3718727118837081E-2</v>
       </c>
       <c r="P22" t="n">
-        <v>1.6047751091473</v>
+        <v>1.6047751091472999</v>
       </c>
       <c r="Q22" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>mechanized</t>
-        </is>
+      <c r="A23" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B23" t="n">
-        <v>0.2871813033869203</v>
+        <v>0.28718130338692027</v>
       </c>
       <c r="C23" t="n">
-        <v>0.008886699605510475</v>
+        <v>8.8866996055104747E-3</v>
       </c>
       <c r="D23" t="n">
-        <v>1.332665808398721</v>
+        <v>1.3326658083987211</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
@@ -1668,50 +1704,48 @@
         <v>0.3843961737409114</v>
       </c>
       <c r="G23" t="n">
-        <v>0.007612168696926212</v>
+        <v>7.6121686969262119E-3</v>
       </c>
       <c r="H23" t="n">
-        <v>1.46872719758442</v>
+        <v>1.4687271975844201</v>
       </c>
       <c r="I23" t="n">
         <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>0.3767148182328474</v>
+        <v>0.37671481823284741</v>
       </c>
       <c r="K23" t="n">
-        <v>0.01149995827164818</v>
+        <v>1.1499958271648181E-2</v>
       </c>
       <c r="L23" t="n">
-        <v>1.457488600922992</v>
+        <v>1.4574886009229919</v>
       </c>
       <c r="M23" t="n">
         <v>0</v>
       </c>
       <c r="N23" t="n">
-        <v>0.1458473452541602</v>
+        <v>0.14584734525416021</v>
       </c>
       <c r="O23" t="n">
-        <v>0.008876635350468213</v>
+        <v>8.8766353504682125E-3</v>
       </c>
       <c r="P23" t="n">
         <v>1.157019550043481</v>
       </c>
       <c r="Q23" t="n">
-        <v>7.945254647942204e-237</v>
+        <v>7.9452546479422037E-237</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>pesticides</t>
-        </is>
+      <c r="A24" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="B24" t="n">
-        <v>0.2721591544360243</v>
+        <v>0.27215915443602429</v>
       </c>
       <c r="C24" t="n">
-        <v>0.008477295677367607</v>
+        <v>8.4772956773676075E-3</v>
       </c>
       <c r="D24" t="n">
         <v>1.312795921979919</v>
@@ -1720,40 +1754,40 @@
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>0.002358239203540492</v>
+        <v>2.358239203540492E-3</v>
       </c>
       <c r="G24" t="n">
-        <v>0.001615072584749762</v>
+        <v>1.615072584749762E-3</v>
       </c>
       <c r="H24" t="n">
-        <v>1.00236102203671</v>
+        <v>1.0023610220367101</v>
       </c>
       <c r="I24" t="n">
-        <v>0.003497071247451559</v>
+        <v>3.4970712474515588E-3</v>
       </c>
       <c r="J24" t="n">
-        <v>-0.02833963074063931</v>
+        <v>-2.8339630740639311E-2</v>
       </c>
       <c r="K24" t="n">
-        <v>0.00303271026757056</v>
+        <v>3.03271026757056E-3</v>
       </c>
       <c r="L24" t="n">
-        <v>0.9720581698957249</v>
+        <v>0.97205816989572491</v>
       </c>
       <c r="M24" t="n">
-        <v>6.049058075392621e-78</v>
+        <v>6.0490580753926215E-78</v>
       </c>
       <c r="N24" t="n">
-        <v>-0.0131034728373501</v>
+        <v>-1.31034728373501E-2</v>
       </c>
       <c r="O24" t="n">
-        <v>0.002168375550953063</v>
+        <v>2.1683755509530628E-3</v>
       </c>
       <c r="P24" t="n">
-        <v>0.9869820039081229</v>
+        <v>0.98698200390812285</v>
       </c>
       <c r="Q24" t="n">
-        <v>1.252660595515936e-33</v>
+        <v>1.2526605955159359E-33</v>
       </c>
     </row>
   </sheetData>
@@ -1764,204 +1798,161 @@
     <mergeCell ref="N1:Q1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>McFaddens_roh</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>RootMeanGammaDeviance</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>AIC</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>BIC</t>
-        </is>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Wheat</t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>Calibration</t>
-        </is>
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3794892238488911</v>
+        <v>0.37948922384889111</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5186236352679973</v>
+        <v>0.51862363526799726</v>
       </c>
       <c r="E2" t="n">
-        <v>2877736.41714726</v>
+        <v>2877736.4171472602</v>
       </c>
       <c r="F2" t="n">
-        <v>2877947.113230278</v>
+        <v>2877947.1132302778</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n"/>
-      <c r="B3" s="1" t="inlineStr">
-        <is>
-          <t>Validation</t>
-        </is>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="C3" t="n">
-        <v>0.3732692490558556</v>
+        <v>0.37326924905585562</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5220449769072656</v>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+        <v>0.52204497690726559</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Corn</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="inlineStr">
-        <is>
-          <t>Calibration</t>
-        </is>
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4805234511143502</v>
+        <v>0.48052345111435019</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5826191384432685</v>
+        <v>0.58261913844326851</v>
       </c>
       <c r="E4" t="n">
-        <v>2820729.315384207</v>
+        <v>2820729.3153842068</v>
       </c>
       <c r="F4" t="n">
-        <v>2820938.464223439</v>
+        <v>2820938.4642234389</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n"/>
-      <c r="B5" s="1" t="inlineStr">
-        <is>
-          <t>Validation</t>
-        </is>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="C5" t="n">
-        <v>0.470395358298599</v>
+        <v>0.47039535829859902</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5863733019508696</v>
-      </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
+        <v>0.58637330195086956</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Soybean</t>
-        </is>
-      </c>
-      <c r="B6" s="1" t="inlineStr">
-        <is>
-          <t>Calibration</t>
-        </is>
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="C6" t="n">
-        <v>0.3470340997675996</v>
+        <v>0.34703409976759958</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3822640739038385</v>
+        <v>0.38226407390383849</v>
       </c>
       <c r="E6" t="n">
         <v>1007503.056559569</v>
       </c>
       <c r="F6" t="n">
-        <v>1007692.871725475</v>
+        <v>1007692.8717254749</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n"/>
-      <c r="B7" s="1" t="inlineStr">
-        <is>
-          <t>Validation</t>
-        </is>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3358403685908677</v>
+        <v>0.33584036859086769</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3880030642065611</v>
-      </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+        <v>0.38800306420656111</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Rice</t>
-        </is>
-      </c>
-      <c r="B8" s="1" t="inlineStr">
-        <is>
-          <t>Calibration</t>
-        </is>
+      <c r="A8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="C8" t="n">
-        <v>0.4108902893979675</v>
+        <v>0.41089028939796751</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4944648328986029</v>
+        <v>0.49446483289860288</v>
       </c>
       <c r="E8" t="n">
-        <v>1328827.06215673</v>
+        <v>1328827.0621567301</v>
       </c>
       <c r="F8" t="n">
-        <v>1329020.849868904</v>
+        <v>1329020.8498689041</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n"/>
-      <c r="B9" s="1" t="inlineStr">
-        <is>
-          <t>Validation</t>
-        </is>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="C9" t="n">
-        <v>0.4042148116274608</v>
+        <v>0.40421481162746081</v>
       </c>
       <c r="D9" t="n">
-        <v>0.4965871446612434</v>
-      </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
+        <v>0.49658714466124337</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1971,5 +1962,500 @@
     <mergeCell ref="A8:A9"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>6.75710342115087</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2.59944290592251</v>
+      </c>
+      <c r="E2" t="n">
+        <v>6.75710342115087</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>8.87130398638317</v>
+      </c>
+      <c r="H2" t="n">
+        <v>2.9784734322104</v>
+      </c>
+      <c r="I2" t="n">
+        <v>8.87130398638317</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
+        <v>6.22874545653217</v>
+      </c>
+      <c r="L2" t="n">
+        <v>2.49574547110321</v>
+      </c>
+      <c r="M2" t="n">
+        <v>6.22874545653217</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="n">
+        <v>6.84139818388234</v>
+      </c>
+      <c r="P2" t="n">
+        <v>2.61560665695023</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>6.84139818388234</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>5.4861832944713</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2.34226029605407</v>
+      </c>
+      <c r="E3" t="n">
+        <v>5.4861832944713</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>9.13573612682127</v>
+      </c>
+      <c r="H3" t="n">
+        <v>3.02253802735735</v>
+      </c>
+      <c r="I3" t="n">
+        <v>9.13573612682127</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="n">
+        <v>4.43132484365412</v>
+      </c>
+      <c r="L3" t="n">
+        <v>2.10507122056574</v>
+      </c>
+      <c r="M3" t="n">
+        <v>4.43132484365412</v>
+      </c>
+      <c r="N3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" t="n">
+        <v>5.81116298971907</v>
+      </c>
+      <c r="P3" t="n">
+        <v>2.41063539128568</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>5.81116298971907</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2.31137943316157</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.52032214782314</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2.31137943316157</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2.01087765522363</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.41805417922716</v>
+      </c>
+      <c r="I4" t="n">
+        <v>2.01087765522363</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>2.24032898787961</v>
+      </c>
+      <c r="L4" t="n">
+        <v>1.49677285781097</v>
+      </c>
+      <c r="M4" t="n">
+        <v>2.24032898787961</v>
+      </c>
+      <c r="N4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" t="n">
+        <v>2.6826236405931</v>
+      </c>
+      <c r="P4" t="n">
+        <v>1.63787168013648</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>2.6826236405931</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.69915696935528</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.30351715345648</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.69915696935528</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.36657264690041</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.169004981555</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1.36657264690041</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" t="n">
+        <v>2.67807664112406</v>
+      </c>
+      <c r="L5" t="n">
+        <v>1.63648300972667</v>
+      </c>
+      <c r="M5" t="n">
+        <v>2.67807664112406</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" t="n">
+        <v>2.24472872457496</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1.4982418778605</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>2.24472872457496</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2.70784096199453</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.64555187155997</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2.70784096199453</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2.82519827874102</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.68083261473028</v>
+      </c>
+      <c r="I6" t="n">
+        <v>2.82519827874102</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" t="n">
+        <v>2.36294034152515</v>
+      </c>
+      <c r="L6" t="n">
+        <v>1.5371858513287</v>
+      </c>
+      <c r="M6" t="n">
+        <v>2.36294034152515</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" t="n">
+        <v>1.93920071724882</v>
+      </c>
+      <c r="P6" t="n">
+        <v>1.39255187237274</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>1.93920071724882</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="n">
+        <v>3.87207736332548</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.11942586027741</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.25311425665782</v>
+      </c>
+      <c r="F7" t="n">
+        <v>6</v>
+      </c>
+      <c r="G7" t="n">
+        <v>4.10843872072257</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1.12496687440875</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1.265550468517</v>
+      </c>
+      <c r="J7" t="n">
+        <v>6</v>
+      </c>
+      <c r="K7" t="n">
+        <v>6.80597307704862</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1.1732958077024</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1.37662305237203</v>
+      </c>
+      <c r="N7" t="n">
+        <v>6</v>
+      </c>
+      <c r="O7" t="n">
+        <v>3.90507538692139</v>
+      </c>
+      <c r="P7" t="n">
+        <v>1.12021775519978</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>1.25488781906484</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.62492792117659</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.06256195672155</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.12903791187193</v>
+      </c>
+      <c r="F8" t="n">
+        <v>4</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2.11936506115047</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1.09843843651614</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1.20656699881603</v>
+      </c>
+      <c r="J8" t="n">
+        <v>4</v>
+      </c>
+      <c r="K8" t="n">
+        <v>2.16792918631411</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1.10155360605282</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1.21342034700796</v>
+      </c>
+      <c r="N8" t="n">
+        <v>4</v>
+      </c>
+      <c r="O8" t="n">
+        <v>1.83407164881423</v>
+      </c>
+      <c r="P8" t="n">
+        <v>1.07876547110013</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>1.16373494163788</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="n">
+        <v>5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>3.23004204051476</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.12439994965912</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1.26427524679343</v>
+      </c>
+      <c r="F9" t="n">
+        <v>5</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2.61994910235162</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1.10110639626739</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1.21243529590096</v>
+      </c>
+      <c r="J9" t="n">
+        <v>5</v>
+      </c>
+      <c r="K9" t="n">
+        <v>4.59150026457548</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1.164650081379</v>
+      </c>
+      <c r="M9" t="n">
+        <v>1.3564098120561</v>
+      </c>
+      <c r="N9" t="n">
+        <v>5</v>
+      </c>
+      <c r="O9" t="n">
+        <v>3.42896503888719</v>
+      </c>
+      <c r="P9" t="n">
+        <v>1.13113985751725</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>1.27947737726415</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId4"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removes p_fertilizer as an independent variable in the GLM and updates all outputs based on the modified model
</commit_message>
<xml_diff>
--- a/reports/Model_results.xlsx
+++ b/reports/Model_results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">row.names</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t xml:space="preserve">n_total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p_fertilizer</t>
   </si>
   <si>
     <t xml:space="preserve">irrigation_tot</t>
@@ -239,8 +236,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q9" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:Q9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q8" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:Q8"/>
   <tableColumns count="17">
     <tableColumn id="1" name="row.names"/>
     <tableColumn id="2" name="Corn.Df"/>
@@ -571,30 +568,34 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Rice</t>
         </is>
       </c>
-      <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Soybean</t>
         </is>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
       <c r="M1" s="1"/>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Wheat</t>
-        </is>
-      </c>
+      <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="1"/>
@@ -605,75 +606,95 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>+-95%Confidence_Interval</t>
+          <t>Multiplicative_Coefficients</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>Odds_ratios</t>
+          <t>lower_95%_Confidence_Interval</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
+          <t>upper_95%_Confidence_Interval</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
           <t>p-value</t>
         </is>
       </c>
-      <c r="F2" s="1" t="inlineStr">
+      <c r="G2" s="1" t="inlineStr">
         <is>
           <t>Coefficients</t>
         </is>
       </c>
-      <c r="G2" s="1" t="inlineStr">
-        <is>
-          <t>+-95%Confidence_Interval</t>
-        </is>
-      </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>Odds_ratios</t>
+          <t>Multiplicative_Coefficients</t>
         </is>
       </c>
       <c r="I2" s="1" t="inlineStr">
         <is>
+          <t>lower_95%_Confidence_Interval</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
+        <is>
+          <t>upper_95%_Confidence_Interval</t>
+        </is>
+      </c>
+      <c r="K2" s="1" t="inlineStr">
+        <is>
           <t>p-value</t>
         </is>
       </c>
-      <c r="J2" s="1" t="inlineStr">
+      <c r="L2" s="1" t="inlineStr">
         <is>
           <t>Coefficients</t>
         </is>
       </c>
-      <c r="K2" s="1" t="inlineStr">
-        <is>
-          <t>+-95%Confidence_Interval</t>
-        </is>
-      </c>
-      <c r="L2" s="1" t="inlineStr">
-        <is>
-          <t>Odds_ratios</t>
-        </is>
-      </c>
       <c r="M2" s="1" t="inlineStr">
         <is>
+          <t>Multiplicative_Coefficients</t>
+        </is>
+      </c>
+      <c r="N2" s="1" t="inlineStr">
+        <is>
+          <t>lower_95%_Confidence_Interval</t>
+        </is>
+      </c>
+      <c r="O2" s="1" t="inlineStr">
+        <is>
+          <t>upper_95%_Confidence_Interval</t>
+        </is>
+      </c>
+      <c r="P2" s="1" t="inlineStr">
+        <is>
           <t>p-value</t>
         </is>
       </c>
-      <c r="N2" s="1" t="inlineStr">
+      <c r="Q2" s="1" t="inlineStr">
         <is>
           <t>Coefficients</t>
         </is>
       </c>
-      <c r="O2" s="1" t="inlineStr">
-        <is>
-          <t>+-95%Confidence_Interval</t>
-        </is>
-      </c>
-      <c r="P2" s="1" t="inlineStr">
-        <is>
-          <t>Odds_ratios</t>
-        </is>
-      </c>
-      <c r="Q2" s="1" t="inlineStr">
+      <c r="R2" s="1" t="inlineStr">
+        <is>
+          <t>Multiplicative_Coefficients</t>
+        </is>
+      </c>
+      <c r="S2" s="1" t="inlineStr">
+        <is>
+          <t>lower_95%_Confidence_Interval</t>
+        </is>
+      </c>
+      <c r="T2" s="1" t="inlineStr">
+        <is>
+          <t>upper_95%_Confidence_Interval</t>
+        </is>
+      </c>
+      <c r="U2" s="1" t="inlineStr">
         <is>
           <t>p-value</t>
         </is>
@@ -686,51 +707,63 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6.406625842951103</v>
+        <v>6.653694065171996</v>
       </c>
       <c r="C4" t="n">
-        <v>0.04289302453120225</v>
+        <v>775.6443204490575</v>
       </c>
       <c r="D4" t="n">
-        <v>605.8460088390894</v>
+        <v>757.6128606890784</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>794.1049354649018</v>
       </c>
       <c r="F4" t="n">
-        <v>6.626383191030197</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.02351118964116861</v>
+        <v>7.40385200862946</v>
       </c>
       <c r="H4" t="n">
-        <v>754.7474507933468</v>
+        <v>1642.298409081678</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1601.325489799361</v>
       </c>
       <c r="J4" t="n">
-        <v>7.401874530574021</v>
+        <v>1684.319697433999</v>
       </c>
       <c r="K4" t="n">
-        <v>0.02536374443002387</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>1639.054008939526</v>
+        <v>6.526986035436765</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>683.3355555181012</v>
       </c>
       <c r="N4" t="n">
-        <v>6.498038789327854</v>
+        <v>654.0484985749043</v>
       </c>
       <c r="O4" t="n">
-        <v>0.02470884281285191</v>
+        <v>713.9340315781722</v>
       </c>
       <c r="P4" t="n">
-        <v>663.8384285221698</v>
+        <v>0</v>
       </c>
       <c r="Q4" t="n">
+        <v>6.408315505740218</v>
+      </c>
+      <c r="R4" t="n">
+        <v>606.8705496166206</v>
+      </c>
+      <c r="S4" t="n">
+        <v>591.9044610261263</v>
+      </c>
+      <c r="T4" t="n">
+        <v>622.215050303064</v>
+      </c>
+      <c r="U4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -741,52 +774,64 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1633912825627313</v>
+        <v>0.1249029972103712</v>
       </c>
       <c r="C5" t="n">
-        <v>0.02234539833175572</v>
+        <v>1.133038539836847</v>
       </c>
       <c r="D5" t="n">
-        <v>1.177497333735952</v>
+        <v>1.11842504869728</v>
       </c>
       <c r="E5" t="n">
-        <v>1.392673409602758e-46</v>
+        <v>1.147842972804419</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1438897880480912</v>
+        <v>2.525597981128465e-79</v>
       </c>
       <c r="G5" t="n">
-        <v>0.01294229724641172</v>
+        <v>0.3027858888069881</v>
       </c>
       <c r="H5" t="n">
-        <v>1.154756833506827</v>
+        <v>1.353624607233014</v>
       </c>
       <c r="I5" t="n">
-        <v>2.856733592169026e-105</v>
+        <v>1.317348077630769</v>
       </c>
       <c r="J5" t="n">
-        <v>0.3100000194259448</v>
+        <v>1.390900103336467</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0270498382061668</v>
+        <v>8.495910382923312e-106</v>
       </c>
       <c r="L5" t="n">
-        <v>1.363425140617999</v>
+        <v>0.1056225768246586</v>
       </c>
       <c r="M5" t="n">
-        <v>9.806455545049278e-112</v>
+        <v>1.111402328342066</v>
       </c>
       <c r="N5" t="n">
-        <v>0.003131165845131262</v>
+        <v>1.086557815035486</v>
       </c>
       <c r="O5" t="n">
-        <v>0.02299853835754441</v>
+        <v>1.136814919879643</v>
       </c>
       <c r="P5" t="n">
-        <v>1.003136073065343</v>
+        <v>5.343869709449388e-20</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.789590938423563</v>
+        <v>0.01446299795390154</v>
+      </c>
+      <c r="R5" t="n">
+        <v>1.014568093161488</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.9912035779283578</v>
+      </c>
+      <c r="T5" t="n">
+        <v>1.03848335355357</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.2237205265092796</v>
       </c>
     </row>
     <row r="6">
@@ -796,52 +841,64 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.0406988412384227</v>
+        <v>0.06152126658156877</v>
       </c>
       <c r="C6" t="n">
-        <v>0.01237576099879626</v>
+        <v>1.063453112300676</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9601182344308888</v>
+        <v>1.05031979606189</v>
       </c>
       <c r="E6" t="n">
-        <v>1.152017860315702e-10</v>
+        <v>1.076750648995055</v>
       </c>
       <c r="F6" t="n">
-        <v>0.08975961304354596</v>
+        <v>2.917583082418097e-22</v>
       </c>
       <c r="G6" t="n">
-        <v>0.01239566221974295</v>
+        <v>-0.1290588166775204</v>
       </c>
       <c r="H6" t="n">
-        <v>1.093911290090704</v>
+        <v>0.878922268737635</v>
       </c>
       <c r="I6" t="n">
-        <v>1.019378204942127e-45</v>
+        <v>0.8692633268130071</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.129434953420793</v>
+        <v>0.8886885373562872</v>
       </c>
       <c r="K6" t="n">
-        <v>0.01109875125444015</v>
+        <v>5.749179130177811e-116</v>
       </c>
       <c r="L6" t="n">
-        <v>0.8785917359445433</v>
+        <v>-0.1369727623241402</v>
       </c>
       <c r="M6" t="n">
-        <v>1.235523025736801e-115</v>
+        <v>0.8719939768979446</v>
       </c>
       <c r="N6" t="n">
-        <v>0.2137759410906344</v>
+        <v>0.8613328043847791</v>
       </c>
       <c r="O6" t="n">
-        <v>0.01700512128083426</v>
+        <v>0.8827871083923271</v>
       </c>
       <c r="P6" t="n">
-        <v>1.238345161440894</v>
+        <v>1.391374302278439e-105</v>
       </c>
       <c r="Q6" t="n">
-        <v>4.800544786868342e-134</v>
+        <v>0.2771126936355223</v>
+      </c>
+      <c r="R6" t="n">
+        <v>1.319315041066095</v>
+      </c>
+      <c r="S6" t="n">
+        <v>1.296857383137012</v>
+      </c>
+      <c r="T6" t="n">
+        <v>1.342161597887392</v>
+      </c>
+      <c r="U6" t="n">
+        <v>1.225430070380547e-219</v>
       </c>
     </row>
     <row r="7">
@@ -851,52 +908,64 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.07437815605728687</v>
+        <v>0.4678338514039946</v>
       </c>
       <c r="C7" t="n">
-        <v>0.01214512492780788</v>
+        <v>1.596532119079351</v>
       </c>
       <c r="D7" t="n">
-        <v>1.077214083514717</v>
+        <v>1.578114178404571</v>
       </c>
       <c r="E7" t="n">
-        <v>3.424520148944059e-33</v>
+        <v>1.615165012856601</v>
       </c>
       <c r="F7" t="n">
-        <v>0.5488077736144407</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.01177426448610375</v>
+        <v>0.2943078596261209</v>
       </c>
       <c r="H7" t="n">
-        <v>1.731187819223424</v>
+        <v>1.34219704834991</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1.323361626882931</v>
       </c>
       <c r="J7" t="n">
-        <v>0.2995081967522047</v>
+        <v>1.361300554590266</v>
       </c>
       <c r="K7" t="n">
-        <v>0.01415667883080751</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>1.349195105849082</v>
+        <v>-0.1210970120014277</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>0.885948007834366</v>
       </c>
       <c r="N7" t="n">
-        <v>-0.1023613020831547</v>
+        <v>0.8767141321965969</v>
       </c>
       <c r="O7" t="n">
-        <v>0.01702709182020332</v>
+        <v>0.8952791380459609</v>
       </c>
       <c r="P7" t="n">
-        <v>0.9027033441439863</v>
+        <v>1.292712331667857e-113</v>
       </c>
       <c r="Q7" t="n">
-        <v>4.795435350110615e-32</v>
+        <v>-0.05696231443909502</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.9446296675946203</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.9284933106378211</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.9610464595452466</v>
+      </c>
+      <c r="U7" t="n">
+        <v>9.189718745563419e-11</v>
       </c>
     </row>
     <row r="8">
@@ -906,52 +975,64 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1414323576934178</v>
+        <v>0.5891912224409646</v>
       </c>
       <c r="C8" t="n">
-        <v>0.02118724767469773</v>
+        <v>1.802529979905171</v>
       </c>
       <c r="D8" t="n">
-        <v>1.151922582924936</v>
+        <v>1.774681569036421</v>
       </c>
       <c r="E8" t="n">
-        <v>4.094188704041516e-39</v>
+        <v>1.830815389727112</v>
       </c>
       <c r="F8" t="n">
-        <v>0.6783116131459639</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0157553313512987</v>
+        <v>0.2616913818212571</v>
       </c>
       <c r="H8" t="n">
-        <v>1.97054787485061</v>
+        <v>1.299125546795083</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1.271258177371035</v>
       </c>
       <c r="J8" t="n">
-        <v>0.270406944401079</v>
+        <v>1.327603799431086</v>
       </c>
       <c r="K8" t="n">
-        <v>0.02179118713760009</v>
+        <v>1.090492217249523e-123</v>
       </c>
       <c r="L8" t="n">
-        <v>1.310497641914311</v>
+        <v>-0.09407923533634065</v>
       </c>
       <c r="M8" t="n">
-        <v>1.169757516185512e-130</v>
+        <v>0.9102106385373464</v>
       </c>
       <c r="N8" t="n">
-        <v>-0.1185193741271747</v>
+        <v>0.8920229325831337</v>
       </c>
       <c r="O8" t="n">
-        <v>0.01747924622558644</v>
+        <v>0.9287691787333638</v>
       </c>
       <c r="P8" t="n">
-        <v>0.8882346067198693</v>
+        <v>6.513105643841843e-20</v>
       </c>
       <c r="Q8" t="n">
-        <v>2.656886049778536e-40</v>
+        <v>-0.05029707666995033</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.9509468784019296</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.9343983024826471</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0.9677885363658056</v>
+      </c>
+      <c r="U8" t="n">
+        <v>1.961192430560364e-08</v>
       </c>
     </row>
     <row r="9">
@@ -961,52 +1042,64 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2432079763544457</v>
+        <v>0.6220827950934207</v>
       </c>
       <c r="C9" t="n">
-        <v>0.01192694529492155</v>
+        <v>1.862803842899517</v>
       </c>
       <c r="D9" t="n">
-        <v>1.275333835820497</v>
+        <v>1.84315998160072</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>1.882657062740479</v>
       </c>
       <c r="F9" t="n">
-        <v>0.6994157896396183</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.01084212068181167</v>
+        <v>0.3558725408372717</v>
       </c>
       <c r="H9" t="n">
-        <v>2.012576595857271</v>
+        <v>1.427425598196886</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1.404654319573738</v>
       </c>
       <c r="J9" t="n">
-        <v>0.3546508420498622</v>
+        <v>1.450566028947293</v>
       </c>
       <c r="K9" t="n">
-        <v>0.01611712281623834</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>1.425682778891338</v>
+        <v>0.04366230913117231</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>1.044629533464751</v>
       </c>
       <c r="N9" t="n">
-        <v>0.1730082112949592</v>
+        <v>1.033954282469107</v>
       </c>
       <c r="O9" t="n">
-        <v>0.01725058887909317</v>
+        <v>1.055415003051055</v>
       </c>
       <c r="P9" t="n">
-        <v>1.188875867254368</v>
+        <v>7.998987836615423e-17</v>
       </c>
       <c r="Q9" t="n">
-        <v>5.065061882416507e-86</v>
+        <v>0.2307326559880605</v>
+      </c>
+      <c r="R9" t="n">
+        <v>1.259522468644513</v>
+      </c>
+      <c r="S9" t="n">
+        <v>1.237803528534077</v>
+      </c>
+      <c r="T9" t="n">
+        <v>1.281622496987973</v>
+      </c>
+      <c r="U9" t="n">
+        <v>5.113138271252217e-149</v>
       </c>
     </row>
     <row r="10">
@@ -1016,52 +1109,64 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.0790581603722551</v>
+        <v>0.6339208977587847</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0135001295032111</v>
+        <v>1.884986949924032</v>
       </c>
       <c r="D10" t="n">
-        <v>1.082267265306926</v>
+        <v>1.865691073927753</v>
       </c>
       <c r="E10" t="n">
-        <v>1.706588204236379e-30</v>
+        <v>1.904482393166822</v>
       </c>
       <c r="F10" t="n">
-        <v>0.748326692475199</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.01082259232586713</v>
+        <v>0.3816904105703115</v>
       </c>
       <c r="H10" t="n">
-        <v>2.113460586658116</v>
+        <v>1.464758541168982</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>1.430094360949287</v>
       </c>
       <c r="J10" t="n">
-        <v>0.3622222861895384</v>
+        <v>1.500262949434542</v>
       </c>
       <c r="K10" t="n">
-        <v>0.02425176356807257</v>
+        <v>3.4688202214557e-214</v>
       </c>
       <c r="L10" t="n">
-        <v>1.436518224635329</v>
+        <v>-0.1268749410218937</v>
       </c>
       <c r="M10" t="n">
-        <v>2.232281451476795e-188</v>
+        <v>0.8808438231377492</v>
       </c>
       <c r="N10" t="n">
-        <v>0.06573163185190448</v>
+        <v>0.870222682270393</v>
       </c>
       <c r="O10" t="n">
-        <v>0.01699021726977193</v>
+        <v>0.8915945959207318</v>
       </c>
       <c r="P10" t="n">
-        <v>1.067940077604346</v>
+        <v>2.224608982617227e-93</v>
       </c>
       <c r="Q10" t="n">
-        <v>3.3845052972799e-14</v>
+        <v>0.1746521819513246</v>
+      </c>
+      <c r="R10" t="n">
+        <v>1.190831951726383</v>
+      </c>
+      <c r="S10" t="n">
+        <v>1.170940448605159</v>
+      </c>
+      <c r="T10" t="n">
+        <v>1.211061364343254</v>
+      </c>
+      <c r="U10" t="n">
+        <v>8.327684885107373e-92</v>
       </c>
     </row>
     <row r="11">
@@ -1071,52 +1176,64 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.2256555015532528</v>
+        <v>-0.08609264833499294</v>
       </c>
       <c r="C11" t="n">
-        <v>0.02302534592370681</v>
+        <v>0.9175092215804909</v>
       </c>
       <c r="D11" t="n">
-        <v>1.253143884786743</v>
+        <v>0.9058539366279749</v>
       </c>
       <c r="E11" t="n">
-        <v>3.15716364016927e-82</v>
+        <v>0.9293144707400732</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.0937015401520401</v>
+        <v>8.935695909321513e-40</v>
       </c>
       <c r="G11" t="n">
-        <v>0.01275026424741578</v>
+        <v>-0.07213108208518282</v>
       </c>
       <c r="H11" t="n">
-        <v>0.9105544856428314</v>
+        <v>0.9304089278751361</v>
       </c>
       <c r="I11" t="n">
-        <v>4.900907344318166e-47</v>
+        <v>0.915211282227768</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.08702285863256454</v>
+        <v>0.945858939765915</v>
       </c>
       <c r="K11" t="n">
-        <v>0.01662721529145031</v>
+        <v>9.151913301287251e-18</v>
       </c>
       <c r="L11" t="n">
-        <v>0.9166561418877308</v>
+        <v>0.201177753474984</v>
       </c>
       <c r="M11" t="n">
-        <v>1.089603544049179e-24</v>
+        <v>1.222842116941473</v>
       </c>
       <c r="N11" t="n">
-        <v>0.02561415238434558</v>
+        <v>1.194375950156493</v>
       </c>
       <c r="O11" t="n">
-        <v>0.007551229256380384</v>
+        <v>1.251986732293107</v>
       </c>
       <c r="P11" t="n">
-        <v>1.02594501365579</v>
+        <v>6.658339096800721e-63</v>
       </c>
       <c r="Q11" t="n">
-        <v>2.965031898692152e-11</v>
+        <v>0.006774804599330751</v>
+      </c>
+      <c r="R11" t="n">
+        <v>1.006797805500877</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.9991378648589274</v>
+      </c>
+      <c r="T11" t="n">
+        <v>1.014516471462626</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0.08210184892209839</v>
       </c>
     </row>
     <row r="12">
@@ -1126,51 +1243,63 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.2991122983497493</v>
+        <v>0.07465257083557482</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0235805528256734</v>
+        <v>1.077509727541303</v>
       </c>
       <c r="D12" t="n">
-        <v>1.348661067381539</v>
+        <v>1.063353767195672</v>
       </c>
       <c r="E12" t="n">
-        <v>1.939171649622361e-136</v>
+        <v>1.091854139951985</v>
       </c>
       <c r="F12" t="n">
-        <v>0.06423340576183081</v>
+        <v>1.878626565235248e-28</v>
       </c>
       <c r="G12" t="n">
-        <v>0.01318935533226073</v>
+        <v>-0.04224488454998609</v>
       </c>
       <c r="H12" t="n">
-        <v>1.066341259911704</v>
+        <v>0.9586349969263909</v>
       </c>
       <c r="I12" t="n">
-        <v>1.358325744594069e-21</v>
+        <v>0.9423003823438444</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.05337964920882654</v>
+        <v>0.9752527692350296</v>
       </c>
       <c r="K12" t="n">
-        <v>0.01732024684446487</v>
+        <v>1.452205406421525e-06</v>
       </c>
       <c r="L12" t="n">
-        <v>0.9480200290989196</v>
+        <v>0.2958245090916408</v>
       </c>
       <c r="M12" t="n">
-        <v>1.536792347685073e-09</v>
+        <v>1.344234235244621</v>
       </c>
       <c r="N12" t="n">
-        <v>0.284499151982661</v>
+        <v>1.312206168383227</v>
       </c>
       <c r="O12" t="n">
-        <v>0.008466175573832002</v>
+        <v>1.377044036784294</v>
       </c>
       <c r="P12" t="n">
-        <v>1.329096186202878</v>
+        <v>9.72545415980767e-128</v>
       </c>
       <c r="Q12" t="n">
+        <v>0.2640070487770936</v>
+      </c>
+      <c r="R12" t="n">
+        <v>1.302137374744645</v>
+      </c>
+      <c r="S12" t="n">
+        <v>1.291036264922997</v>
+      </c>
+      <c r="T12" t="n">
+        <v>1.313333938615588</v>
+      </c>
+      <c r="U12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1181,51 +1310,63 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.4528512035603207</v>
+        <v>0.2975260969293818</v>
       </c>
       <c r="C13" t="n">
-        <v>0.02332081591590507</v>
+        <v>1.346523515023337</v>
       </c>
       <c r="D13" t="n">
-        <v>1.572790143528506</v>
+        <v>1.328546724428843</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>1.364743552614069</v>
       </c>
       <c r="F13" t="n">
-        <v>0.271929992836308</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>0.01341633442334839</v>
+        <v>-0.0252317182106811</v>
       </c>
       <c r="H13" t="n">
-        <v>1.312495114034469</v>
+        <v>0.9750839411424537</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>0.9581795467773879</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.04365442256223725</v>
+        <v>0.992286566199054</v>
       </c>
       <c r="K13" t="n">
-        <v>0.01775607719049378</v>
+        <v>0.004687232321772079</v>
       </c>
       <c r="L13" t="n">
-        <v>0.9572847163178325</v>
+        <v>0.4595282099994731</v>
       </c>
       <c r="M13" t="n">
-        <v>1.445012476831519e-06</v>
+        <v>1.583326810996736</v>
       </c>
       <c r="N13" t="n">
-        <v>0.4611029103811264</v>
+        <v>1.546007909611866</v>
       </c>
       <c r="O13" t="n">
-        <v>0.009371994138700657</v>
+        <v>1.621546548911559</v>
       </c>
       <c r="P13" t="n">
-        <v>1.585822040434054</v>
+        <v>0</v>
       </c>
       <c r="Q13" t="n">
+        <v>0.4543485283843902</v>
+      </c>
+      <c r="R13" t="n">
+        <v>1.575146885217066</v>
+      </c>
+      <c r="S13" t="n">
+        <v>1.560247823337499</v>
+      </c>
+      <c r="T13" t="n">
+        <v>1.590188220677516</v>
+      </c>
+      <c r="U13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1236,51 +1377,63 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.4481294383233159</v>
+        <v>0.2603983836940528</v>
       </c>
       <c r="C14" t="n">
-        <v>0.02327978969154054</v>
+        <v>1.297446865395901</v>
       </c>
       <c r="D14" t="n">
-        <v>1.565381302871863</v>
+        <v>1.28044260550035</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>1.31467694162508</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2566522874963661</v>
+        <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0.0131559863731554</v>
+        <v>0.1195123546732364</v>
       </c>
       <c r="H14" t="n">
-        <v>1.292595596959112</v>
+        <v>1.126947167045202</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1.108433190378345</v>
       </c>
       <c r="J14" t="n">
-        <v>0.1021667134295864</v>
+        <v>1.145770379609176</v>
       </c>
       <c r="K14" t="n">
-        <v>0.0167930485019422</v>
+        <v>2.1297826359626e-45</v>
       </c>
       <c r="L14" t="n">
-        <v>1.107568102814186</v>
+        <v>0.4121663588025503</v>
       </c>
       <c r="M14" t="n">
-        <v>8.856773176199827e-33</v>
+        <v>1.510085631471304</v>
       </c>
       <c r="N14" t="n">
-        <v>0.5503954066702998</v>
+        <v>1.474629264542815</v>
       </c>
       <c r="O14" t="n">
-        <v>0.009885521184382129</v>
+        <v>1.546394520444482</v>
       </c>
       <c r="P14" t="n">
-        <v>1.733938493183803</v>
+        <v>2.228333985493853e-253</v>
       </c>
       <c r="Q14" t="n">
+        <v>0.5173739872844975</v>
+      </c>
+      <c r="R14" t="n">
+        <v>1.677616418212903</v>
+      </c>
+      <c r="S14" t="n">
+        <v>1.660988449558783</v>
+      </c>
+      <c r="T14" t="n">
+        <v>1.694410847592043</v>
+      </c>
+      <c r="U14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1291,51 +1444,63 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.4897620679931707</v>
+        <v>0.8717504375519823</v>
       </c>
       <c r="C15" t="n">
-        <v>0.03862598245327886</v>
+        <v>2.391092650835281</v>
       </c>
       <c r="D15" t="n">
-        <v>1.63192788588177</v>
+        <v>2.3285361954902</v>
       </c>
       <c r="E15" t="n">
-        <v>2.48723203113967e-136</v>
+        <v>2.45532969423088</v>
       </c>
       <c r="F15" t="n">
-        <v>0.9207986608071315</v>
+        <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>0.02639762639544496</v>
+        <v>0.4741880183604993</v>
       </c>
       <c r="H15" t="n">
-        <v>2.511295262324382</v>
+        <v>1.606709049431205</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>1.561454371390686</v>
       </c>
       <c r="J15" t="n">
-        <v>0.4945858412584265</v>
+        <v>1.653275316156014</v>
       </c>
       <c r="K15" t="n">
-        <v>0.02852459766803628</v>
+        <v>4.02463352444384e-232</v>
       </c>
       <c r="L15" t="n">
-        <v>1.639818953046632</v>
+        <v>0.4448918650237251</v>
       </c>
       <c r="M15" t="n">
-        <v>3.883250656949213e-253</v>
+        <v>1.560321461385575</v>
       </c>
       <c r="N15" t="n">
-        <v>0.6355214754207088</v>
+        <v>1.499721185466612</v>
       </c>
       <c r="O15" t="n">
-        <v>0.02303501876733272</v>
+        <v>1.623370454757517</v>
       </c>
       <c r="P15" t="n">
-        <v>1.888006433743653</v>
+        <v>2.187747226661654e-107</v>
       </c>
       <c r="Q15" t="n">
+        <v>0.6370943669946615</v>
+      </c>
+      <c r="R15" t="n">
+        <v>1.890978399832349</v>
+      </c>
+      <c r="S15" t="n">
+        <v>1.847210629613217</v>
+      </c>
+      <c r="T15" t="n">
+        <v>1.935783202688282</v>
+      </c>
+      <c r="U15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1346,51 +1511,63 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.56132943490094</v>
+        <v>0.8640548186054547</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0355769596249107</v>
+        <v>2.372762334955616</v>
       </c>
       <c r="D16" t="n">
-        <v>1.753001453170712</v>
+        <v>2.325924233270509</v>
       </c>
       <c r="E16" t="n">
-        <v>5.666109233642553e-210</v>
+        <v>2.42054363493501</v>
       </c>
       <c r="F16" t="n">
-        <v>0.9016139048859644</v>
+        <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>0.01996523287172625</v>
+        <v>0.4574747951758786</v>
       </c>
       <c r="H16" t="n">
-        <v>2.463575881610082</v>
+        <v>1.580078920027403</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>1.54638432518579</v>
       </c>
       <c r="J16" t="n">
-        <v>0.4749615107163253</v>
+        <v>1.61450769569525</v>
       </c>
       <c r="K16" t="n">
-        <v>0.02157705278148198</v>
+        <v>0</v>
       </c>
       <c r="L16" t="n">
-        <v>1.607952307362244</v>
+        <v>0.5067039036016099</v>
       </c>
       <c r="M16" t="n">
-        <v>0</v>
+        <v>1.659811270776386</v>
       </c>
       <c r="N16" t="n">
-        <v>0.6522860679445137</v>
+        <v>1.600389125342344</v>
       </c>
       <c r="O16" t="n">
-        <v>0.01869000056660575</v>
+        <v>1.72143974922786</v>
       </c>
       <c r="P16" t="n">
-        <v>1.919924894726258</v>
+        <v>2.134680170008171e-163</v>
       </c>
       <c r="Q16" t="n">
+        <v>0.6502369331052154</v>
+      </c>
+      <c r="R16" t="n">
+        <v>1.915994737821569</v>
+      </c>
+      <c r="S16" t="n">
+        <v>1.879898880354268</v>
+      </c>
+      <c r="T16" t="n">
+        <v>1.952783670294082</v>
+      </c>
+      <c r="U16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1401,51 +1578,63 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.4025243368690578</v>
+        <v>0.6349610133172627</v>
       </c>
       <c r="C17" t="n">
-        <v>0.03515663872105629</v>
+        <v>1.886948574159272</v>
       </c>
       <c r="D17" t="n">
-        <v>1.495595322889575</v>
+        <v>1.850458027814796</v>
       </c>
       <c r="E17" t="n">
-        <v>1.583873594546386e-111</v>
+        <v>1.924158704494578</v>
       </c>
       <c r="F17" t="n">
-        <v>0.6443256763603922</v>
+        <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>0.01952862388816967</v>
+        <v>0.3255971124211283</v>
       </c>
       <c r="H17" t="n">
-        <v>1.904702210401852</v>
+        <v>1.384857314653193</v>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>1.357250703595441</v>
       </c>
       <c r="J17" t="n">
-        <v>0.3377725560984647</v>
+        <v>1.413025446859599</v>
       </c>
       <c r="K17" t="n">
-        <v>0.02013424390726631</v>
+        <v>1.975963775608436e-220</v>
       </c>
       <c r="L17" t="n">
-        <v>1.401821631362851</v>
+        <v>0.4158423848672826</v>
       </c>
       <c r="M17" t="n">
-        <v>4.189744576021895e-237</v>
+        <v>1.515646961146393</v>
       </c>
       <c r="N17" t="n">
-        <v>0.5018969915945826</v>
+        <v>1.461952456758626</v>
       </c>
       <c r="O17" t="n">
-        <v>0.01858974096912536</v>
+        <v>1.571313554153131</v>
       </c>
       <c r="P17" t="n">
-        <v>1.651851849494483</v>
+        <v>4.718714182669317e-113</v>
       </c>
       <c r="Q17" t="n">
+        <v>0.5013183229232893</v>
+      </c>
+      <c r="R17" t="n">
+        <v>1.650896251093657</v>
+      </c>
+      <c r="S17" t="n">
+        <v>1.619950925990413</v>
+      </c>
+      <c r="T17" t="n">
+        <v>1.682432713329749</v>
+      </c>
+      <c r="U17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1456,52 +1645,64 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.1656867639595033</v>
+        <v>0.3692192260218174</v>
       </c>
       <c r="C18" t="n">
-        <v>0.03692562325712737</v>
+        <v>1.446604702309363</v>
       </c>
       <c r="D18" t="n">
-        <v>1.180203361590366</v>
+        <v>1.415418039188353</v>
       </c>
       <c r="E18" t="n">
-        <v>1.437662226471549e-18</v>
+        <v>1.478478517868519</v>
       </c>
       <c r="F18" t="n">
-        <v>0.3825689311226341</v>
+        <v>9.449975656248431e-242</v>
       </c>
       <c r="G18" t="n">
-        <v>0.02177588726747054</v>
+        <v>0.04956812229553847</v>
       </c>
       <c r="H18" t="n">
-        <v>1.466045927066274</v>
+        <v>1.050817173854718</v>
       </c>
       <c r="I18" t="n">
-        <v>7.936109466381916e-260</v>
+        <v>1.028196511516865</v>
       </c>
       <c r="J18" t="n">
-        <v>0.05723762032020107</v>
+        <v>1.073935498223974</v>
       </c>
       <c r="K18" t="n">
-        <v>0.0217786553051282</v>
+        <v>8.032290906752875e-06</v>
       </c>
       <c r="L18" t="n">
-        <v>1.058907398418178</v>
+        <v>0.1546459836107757</v>
       </c>
       <c r="M18" t="n">
-        <v>2.58985689532663e-07</v>
+        <v>1.167244664211139</v>
       </c>
       <c r="N18" t="n">
-        <v>0.2927297893328295</v>
+        <v>1.123882052451036</v>
       </c>
       <c r="O18" t="n">
-        <v>0.02141490294667175</v>
+        <v>1.212280330625471</v>
       </c>
       <c r="P18" t="n">
-        <v>1.340080637421982</v>
+        <v>1.180926237158062e-15</v>
       </c>
       <c r="Q18" t="n">
-        <v>4.04647950138541e-158</v>
+        <v>0.3005192481228183</v>
+      </c>
+      <c r="R18" t="n">
+        <v>1.350559901232937</v>
+      </c>
+      <c r="S18" t="n">
+        <v>1.321418738087801</v>
+      </c>
+      <c r="T18" t="n">
+        <v>1.380343712590161</v>
+      </c>
+      <c r="U18" t="n">
+        <v>1.392270680975141e-160</v>
       </c>
     </row>
     <row r="19">
@@ -1511,51 +1712,63 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.5154035774721351</v>
+        <v>0.8923333567972855</v>
       </c>
       <c r="C19" t="n">
-        <v>0.03626598301373807</v>
+        <v>2.440818311870382</v>
       </c>
       <c r="D19" t="n">
-        <v>1.674314080908438</v>
+        <v>2.38913471231449</v>
       </c>
       <c r="E19" t="n">
-        <v>9.489112261697848e-171</v>
+        <v>2.493619970801194</v>
       </c>
       <c r="F19" t="n">
-        <v>0.9270893244424766</v>
+        <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>0.02142805193027142</v>
+        <v>0.4094446794959185</v>
       </c>
       <c r="H19" t="n">
-        <v>2.52714276951695</v>
+        <v>1.505981250594748</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1.474393776410798</v>
       </c>
       <c r="J19" t="n">
-        <v>0.4270155660577014</v>
+        <v>1.538245456152152</v>
       </c>
       <c r="K19" t="n">
-        <v>0.02123216044243592</v>
+        <v>0</v>
       </c>
       <c r="L19" t="n">
-        <v>1.532676519269471</v>
+        <v>0.4863679009000694</v>
       </c>
       <c r="M19" t="n">
-        <v>0</v>
+        <v>1.626398239533661</v>
       </c>
       <c r="N19" t="n">
-        <v>0.7279966944041083</v>
+        <v>1.567086367391131</v>
       </c>
       <c r="O19" t="n">
-        <v>0.01973162097674064</v>
+        <v>1.687954977211527</v>
       </c>
       <c r="P19" t="n">
-        <v>2.070927748193028</v>
+        <v>3.27202687222201e-145</v>
       </c>
       <c r="Q19" t="n">
+        <v>0.734990247102709</v>
+      </c>
+      <c r="R19" t="n">
+        <v>2.085461653112537</v>
+      </c>
+      <c r="S19" t="n">
+        <v>2.043997496535683</v>
+      </c>
+      <c r="T19" t="n">
+        <v>2.127766943929302</v>
+      </c>
+      <c r="U19" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1566,280 +1779,273 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-0.001726933737854424</v>
+        <v>0.0005026253345663635</v>
       </c>
       <c r="C20" t="n">
-        <v>7.631996124318231e-05</v>
+        <v>1.000502751671846</v>
       </c>
       <c r="D20" t="n">
-        <v>0.998274556554211</v>
+        <v>1.000456433425546</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>1.000549072062547</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.0009411451073333683</v>
+        <v>1.781792304658911e-100</v>
       </c>
       <c r="G20" t="n">
-        <v>7.299693914515214e-05</v>
+        <v>0.001538049822201306</v>
       </c>
       <c r="H20" t="n">
-        <v>0.9990592976308187</v>
+        <v>1.001539233227463</v>
       </c>
       <c r="I20" t="n">
-        <v>6.880934130649236e-141</v>
+        <v>1.001487665640435</v>
       </c>
       <c r="J20" t="n">
-        <v>0.0009722374505679556</v>
+        <v>1.001590803469758</v>
       </c>
       <c r="K20" t="n">
-        <v>9.525921349702327e-05</v>
+        <v>0</v>
       </c>
       <c r="L20" t="n">
-        <v>1.000972710226603</v>
+        <v>-2.505158541384011e-05</v>
       </c>
       <c r="M20" t="n">
-        <v>5.0987675228035e-89</v>
+        <v>0.9999749487283746</v>
       </c>
       <c r="N20" t="n">
-        <v>0.003203178145427554</v>
+        <v>0.9999222505835584</v>
       </c>
       <c r="O20" t="n">
-        <v>7.34619807538717e-05</v>
+        <v>1.000027649650501</v>
       </c>
       <c r="P20" t="n">
-        <v>1.003208313802554</v>
+        <v>0.3515031631568395</v>
       </c>
       <c r="Q20" t="n">
+        <v>0.001564107181939395</v>
+      </c>
+      <c r="R20" t="n">
+        <v>1.001565331035574</v>
+      </c>
+      <c r="S20" t="n">
+        <v>1.001520303580794</v>
+      </c>
+      <c r="T20" t="n">
+        <v>1.001610360514748</v>
+      </c>
+      <c r="U20" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>p_fertilizer</t>
+          <t>irrigation_tot</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.01318683074725847</v>
+        <v>0.5116283490096347</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0004377086764497801</v>
+        <v>1.66800507918963</v>
       </c>
       <c r="D21" t="n">
-        <v>1.013274160444948</v>
+        <v>1.642830633430284</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>1.693565293698593</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0113229561056198</v>
+        <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>0.0004412492804897004</v>
+        <v>0.4806473634863596</v>
       </c>
       <c r="H21" t="n">
-        <v>1.011387303411005</v>
+        <v>1.617120928457011</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>1.595645303848412</v>
       </c>
       <c r="J21" t="n">
-        <v>0.004746883377796711</v>
+        <v>1.638885591269287</v>
       </c>
       <c r="K21" t="n">
-        <v>0.0006756137630473677</v>
+        <v>0</v>
       </c>
       <c r="L21" t="n">
-        <v>1.004758167676716</v>
+        <v>0.2100274559687152</v>
       </c>
       <c r="M21" t="n">
-        <v>3.821285630095189e-43</v>
+        <v>1.233711932247958</v>
       </c>
       <c r="N21" t="n">
-        <v>-0.01401602792773995</v>
+        <v>1.21086769543165</v>
       </c>
       <c r="O21" t="n">
-        <v>0.0004830462880920823</v>
+        <v>1.256987148565733</v>
       </c>
       <c r="P21" t="n">
-        <v>0.9860817392893387</v>
+        <v>1.671877867185021e-107</v>
       </c>
       <c r="Q21" t="n">
+        <v>0.4239058132736776</v>
+      </c>
+      <c r="R21" t="n">
+        <v>1.52791767744253</v>
+      </c>
+      <c r="S21" t="n">
+        <v>1.507852653571316</v>
+      </c>
+      <c r="T21" t="n">
+        <v>1.548249706967115</v>
+      </c>
+      <c r="U21" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>irrigation_tot</t>
+          <t>mechanized</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.2141759209920092</v>
+        <v>0.4359309841668994</v>
       </c>
       <c r="C22" t="n">
-        <v>0.01838594753607212</v>
+        <v>1.54640206483958</v>
       </c>
       <c r="D22" t="n">
-        <v>1.2388405736873</v>
+        <v>1.535089956947911</v>
       </c>
       <c r="E22" t="n">
-        <v>2.236305433369659e-115</v>
+        <v>1.557797531875365</v>
       </c>
       <c r="F22" t="n">
-        <v>0.5242107950030375</v>
+        <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>0.0152212209228324</v>
+        <v>0.1608721137566806</v>
       </c>
       <c r="H22" t="n">
-        <v>1.689125256116848</v>
+        <v>1.174534752371639</v>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>1.164602947177249</v>
       </c>
       <c r="J22" t="n">
-        <v>0.4729836278530679</v>
+        <v>1.184551256608444</v>
       </c>
       <c r="K22" t="n">
-        <v>0.01344410553332681</v>
+        <v>9.251637423686757e-302</v>
       </c>
       <c r="L22" t="n">
-        <v>1.6047751091473</v>
+        <v>0.4519370166336108</v>
       </c>
       <c r="M22" t="n">
-        <v>0</v>
+        <v>1.571352976360643</v>
       </c>
       <c r="N22" t="n">
-        <v>0.4199043420301316</v>
+        <v>1.553910983625425</v>
       </c>
       <c r="O22" t="n">
-        <v>0.01299502443406625</v>
+        <v>1.588990748077915</v>
       </c>
       <c r="P22" t="n">
-        <v>1.521815974829098</v>
+        <v>0</v>
       </c>
       <c r="Q22" t="n">
+        <v>0.2964648864466628</v>
+      </c>
+      <c r="R22" t="n">
+        <v>1.34509532809147</v>
+      </c>
+      <c r="S22" t="n">
+        <v>1.333247405673994</v>
+      </c>
+      <c r="T22" t="n">
+        <v>1.357048537243436</v>
+      </c>
+      <c r="U22" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>mechanized</t>
+          <t>pesticides</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.3767148182328474</v>
+        <v>0.01545827949379634</v>
       </c>
       <c r="C23" t="n">
-        <v>0.01126975201807195</v>
+        <v>1.015578376730474</v>
       </c>
       <c r="D23" t="n">
-        <v>1.457488600922992</v>
+        <v>1.01404407418431</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>1.017115000757886</v>
       </c>
       <c r="F23" t="n">
-        <v>0.3843961737409114</v>
+        <v>2.50059771791569e-89</v>
       </c>
       <c r="G23" t="n">
-        <v>0.007459788245109289</v>
+        <v>-0.00976616818931531</v>
       </c>
       <c r="H23" t="n">
-        <v>1.46872719758442</v>
+        <v>0.9902813659632052</v>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>0.988238203307089</v>
       </c>
       <c r="J23" t="n">
-        <v>0.1458473452541602</v>
+        <v>0.9923287528171163</v>
       </c>
       <c r="K23" t="n">
-        <v>0.008698942795406395</v>
+        <v>1.899147908294156e-20</v>
       </c>
       <c r="L23" t="n">
-        <v>1.157019550043481</v>
+        <v>0.005125954721793496</v>
       </c>
       <c r="M23" t="n">
-        <v>7.945254647942204e-237</v>
+        <v>1.005139114904256</v>
       </c>
       <c r="N23" t="n">
-        <v>0.2871813033869203</v>
+        <v>1.002347358854742</v>
       </c>
       <c r="O23" t="n">
-        <v>0.00870880558411341</v>
+        <v>1.00793864660337</v>
       </c>
       <c r="P23" t="n">
-        <v>1.332665808398721</v>
+        <v>0.0003036496628352932</v>
       </c>
       <c r="Q23" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>pesticides</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>-0.02833963074063931</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0.002972001449991565</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0.9720581698957249</v>
-      </c>
-      <c r="E24" t="n">
-        <v>6.049058075392621e-78</v>
-      </c>
-      <c r="F24" t="n">
-        <v>0.002358239203540492</v>
-      </c>
-      <c r="G24" t="n">
-        <v>0.001582742049263774</v>
-      </c>
-      <c r="H24" t="n">
-        <v>1.00236102203671</v>
-      </c>
-      <c r="I24" t="n">
-        <v>0.003497071247451559</v>
-      </c>
-      <c r="J24" t="n">
-        <v>-0.0131034728373501</v>
-      </c>
-      <c r="K24" t="n">
-        <v>0.0021249689924126</v>
-      </c>
-      <c r="L24" t="n">
-        <v>0.9869820039081229</v>
-      </c>
-      <c r="M24" t="n">
-        <v>1.252660595515936e-33</v>
-      </c>
-      <c r="N24" t="n">
-        <v>0.2721591544360243</v>
-      </c>
-      <c r="O24" t="n">
-        <v>0.008307597106968823</v>
-      </c>
-      <c r="P24" t="n">
-        <v>1.312795921979919</v>
-      </c>
-      <c r="Q24" t="n">
+        <v>0.267416494438307</v>
+      </c>
+      <c r="R23" t="n">
+        <v>1.306584518206345</v>
+      </c>
+      <c r="S23" t="n">
+        <v>1.295616253795638</v>
+      </c>
+      <c r="T23" t="n">
+        <v>1.317645636364318</v>
+      </c>
+      <c r="U23" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="Q1:U1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -1894,16 +2100,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.4805234511143502</v>
+        <v>0.4691055946554749</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5826191384432685</v>
+        <v>0.5892046467577909</v>
       </c>
       <c r="E2" t="n">
-        <v>2820729.315384207</v>
+        <v>2825877.609096161</v>
       </c>
       <c r="F2" t="n">
-        <v>2820938.464223439</v>
+        <v>2826076.809213218</v>
       </c>
     </row>
     <row r="3">
@@ -1914,10 +2120,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.470395358298599</v>
+        <v>0.4735024248024569</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5863733019508696</v>
+        <v>0.5833762761602982</v>
       </c>
       <c r="E3"/>
       <c r="F3"/>
@@ -1934,16 +2140,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.4108902893979675</v>
+        <v>0.4086396766888927</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4944648328986029</v>
+        <v>0.4948846247822669</v>
       </c>
       <c r="E4" t="n">
-        <v>1328827.06215673</v>
+        <v>1330173.218601608</v>
       </c>
       <c r="F4" t="n">
-        <v>1329020.849868904</v>
+        <v>1330357.794808741</v>
       </c>
     </row>
     <row r="5">
@@ -1954,10 +2160,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.4042148116274608</v>
+        <v>0.4047994053055386</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4965871446612434</v>
+        <v>0.4976633148876741</v>
       </c>
       <c r="E5"/>
       <c r="F5"/>
@@ -1974,16 +2180,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.3470340997675996</v>
+        <v>0.3125345491357727</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3822640739038385</v>
+        <v>0.3926494020479137</v>
       </c>
       <c r="E6" t="n">
-        <v>1007503.056559569</v>
+        <v>1011746.843656312</v>
       </c>
       <c r="F6" t="n">
-        <v>1007692.871725475</v>
+        <v>1011927.632853311</v>
       </c>
     </row>
     <row r="7">
@@ -1994,10 +2200,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.3358403685908677</v>
+        <v>0.3223258184124012</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3880030642065611</v>
+        <v>0.390429794899244</v>
       </c>
       <c r="E7"/>
       <c r="F7"/>
@@ -2014,16 +2220,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.3794892238488911</v>
+        <v>0.3680774688245015</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5186236352679973</v>
+        <v>0.5240906756102784</v>
       </c>
       <c r="E8" t="n">
-        <v>2877736.41714726</v>
+        <v>2882944.595284296</v>
       </c>
       <c r="F8" t="n">
-        <v>2877947.113230278</v>
+        <v>2883145.270936384</v>
       </c>
     </row>
     <row r="9">
@@ -2034,10 +2240,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.3732692490558556</v>
+        <v>0.364135129460144</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5220449769072656</v>
+        <v>0.5242647678344248</v>
       </c>
       <c r="E9"/>
       <c r="F9"/>
@@ -2123,49 +2329,49 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>6.75710342115087</v>
+        <v>2.71193498786088</v>
       </c>
       <c r="D2" t="n">
-        <v>2.59944290592251</v>
+        <v>1.64679536915212</v>
       </c>
       <c r="E2" t="n">
-        <v>6.75710342115087</v>
+        <v>2.71193498786088</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>8.87130398638317</v>
+        <v>2.61672967511951</v>
       </c>
       <c r="H2" t="n">
-        <v>2.9784734322104</v>
+        <v>1.61763088345874</v>
       </c>
       <c r="I2" t="n">
-        <v>8.87130398638317</v>
+        <v>2.61672967511951</v>
       </c>
       <c r="J2" t="n">
         <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>6.22874545653217</v>
+        <v>2.89312973704457</v>
       </c>
       <c r="L2" t="n">
-        <v>2.49574547110321</v>
+        <v>1.70092026181258</v>
       </c>
       <c r="M2" t="n">
-        <v>6.22874545653217</v>
+        <v>2.89312973704457</v>
       </c>
       <c r="N2" t="n">
         <v>1</v>
       </c>
       <c r="O2" t="n">
-        <v>6.84139818388234</v>
+        <v>2.50661923033399</v>
       </c>
       <c r="P2" t="n">
-        <v>2.61560665695023</v>
+        <v>1.58323063080967</v>
       </c>
       <c r="Q2" t="n">
-        <v>6.84139818388234</v>
+        <v>2.50661923033399</v>
       </c>
     </row>
     <row r="3">
@@ -2176,49 +2382,49 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>5.4861832944713</v>
+        <v>2.30550444759329</v>
       </c>
       <c r="D3" t="n">
-        <v>2.34226029605407</v>
+        <v>1.51838876694781</v>
       </c>
       <c r="E3" t="n">
-        <v>5.4861832944713</v>
+        <v>2.30550444759329</v>
       </c>
       <c r="F3" t="n">
         <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>9.13573612682127</v>
+        <v>2.00153437629713</v>
       </c>
       <c r="H3" t="n">
-        <v>3.02253802735735</v>
+        <v>1.41475594230847</v>
       </c>
       <c r="I3" t="n">
-        <v>9.13573612682127</v>
+        <v>2.00153437629713</v>
       </c>
       <c r="J3" t="n">
         <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>4.43132484365412</v>
+        <v>2.24715452220963</v>
       </c>
       <c r="L3" t="n">
-        <v>2.10507122056574</v>
+        <v>1.49905120733403</v>
       </c>
       <c r="M3" t="n">
-        <v>4.43132484365412</v>
+        <v>2.24715452220963</v>
       </c>
       <c r="N3" t="n">
         <v>1</v>
       </c>
       <c r="O3" t="n">
-        <v>5.81116298971907</v>
+        <v>2.6996832382275</v>
       </c>
       <c r="P3" t="n">
-        <v>2.41063539128568</v>
+        <v>1.64307128215044</v>
       </c>
       <c r="Q3" t="n">
-        <v>5.81116298971907</v>
+        <v>2.6996832382275</v>
       </c>
     </row>
     <row r="4">
@@ -2229,49 +2435,49 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>2.31137943316157</v>
+        <v>1.63259989417477</v>
       </c>
       <c r="D4" t="n">
-        <v>1.52032214782314</v>
+        <v>1.27773232493147</v>
       </c>
       <c r="E4" t="n">
-        <v>2.31137943316157</v>
+        <v>1.63259989417477</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>2.01087765522363</v>
+        <v>1.30530027241378</v>
       </c>
       <c r="H4" t="n">
-        <v>1.41805417922716</v>
+        <v>1.14249738398553</v>
       </c>
       <c r="I4" t="n">
-        <v>2.01087765522363</v>
+        <v>1.30530027241378</v>
       </c>
       <c r="J4" t="n">
         <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>2.24032898787961</v>
+        <v>2.54876180317693</v>
       </c>
       <c r="L4" t="n">
-        <v>1.49677285781097</v>
+        <v>1.59648420072888</v>
       </c>
       <c r="M4" t="n">
-        <v>2.24032898787961</v>
+        <v>2.54876180317693</v>
       </c>
       <c r="N4" t="n">
         <v>1</v>
       </c>
       <c r="O4" t="n">
-        <v>2.6826236405931</v>
+        <v>2.24898951816017</v>
       </c>
       <c r="P4" t="n">
-        <v>1.63787168013648</v>
+        <v>1.49966313489402</v>
       </c>
       <c r="Q4" t="n">
-        <v>2.6826236405931</v>
+        <v>2.24898951816017</v>
       </c>
     </row>
     <row r="5">
@@ -2282,49 +2488,49 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>1.69915696935528</v>
+        <v>2.44843296523841</v>
       </c>
       <c r="D5" t="n">
-        <v>1.30351715345648</v>
+        <v>1.56474693328934</v>
       </c>
       <c r="E5" t="n">
-        <v>1.69915696935528</v>
+        <v>2.44843296523841</v>
       </c>
       <c r="F5" t="n">
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>1.36657264690041</v>
+        <v>2.69073780298122</v>
       </c>
       <c r="H5" t="n">
-        <v>1.169004981555</v>
+        <v>1.64034685447353</v>
       </c>
       <c r="I5" t="n">
-        <v>1.36657264690041</v>
+        <v>2.69073780298122</v>
       </c>
       <c r="J5" t="n">
         <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>2.67807664112406</v>
+        <v>1.99082991607438</v>
       </c>
       <c r="L5" t="n">
-        <v>1.63648300972667</v>
+        <v>1.41096772325748</v>
       </c>
       <c r="M5" t="n">
-        <v>2.67807664112406</v>
+        <v>1.99082991607438</v>
       </c>
       <c r="N5" t="n">
         <v>1</v>
       </c>
       <c r="O5" t="n">
-        <v>2.24472872457496</v>
+        <v>1.9384353948108</v>
       </c>
       <c r="P5" t="n">
-        <v>1.4982418778605</v>
+        <v>1.39227705389797</v>
       </c>
       <c r="Q5" t="n">
-        <v>2.24472872457496</v>
+        <v>1.9384353948108</v>
       </c>
     </row>
     <row r="6">
@@ -2332,52 +2538,52 @@
         <v>21</v>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>2.70784096199453</v>
+        <v>3.42576057199118</v>
       </c>
       <c r="D6" t="n">
-        <v>1.64555187155997</v>
+        <v>1.1080595059969</v>
       </c>
       <c r="E6" t="n">
-        <v>2.70784096199453</v>
+        <v>1.2277958688301</v>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G6" t="n">
-        <v>2.82519827874102</v>
+        <v>4.04119753548385</v>
       </c>
       <c r="H6" t="n">
-        <v>1.68083261473028</v>
+        <v>1.12342091924423</v>
       </c>
       <c r="I6" t="n">
-        <v>2.82519827874102</v>
+        <v>1.26207456179555</v>
       </c>
       <c r="J6" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K6" t="n">
-        <v>2.36294034152515</v>
+        <v>4.31297626968293</v>
       </c>
       <c r="L6" t="n">
-        <v>1.5371858513287</v>
+        <v>1.12953082941685</v>
       </c>
       <c r="M6" t="n">
-        <v>2.36294034152515</v>
+        <v>1.27583989460311</v>
       </c>
       <c r="N6" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="O6" t="n">
-        <v>1.93920071724882</v>
+        <v>3.4890316678403</v>
       </c>
       <c r="P6" t="n">
-        <v>1.39255187237274</v>
+        <v>1.1097506530751</v>
       </c>
       <c r="Q6" t="n">
-        <v>1.93920071724882</v>
+        <v>1.23154651200062</v>
       </c>
     </row>
     <row r="7">
@@ -2385,52 +2591,52 @@
         <v>22</v>
       </c>
       <c r="B7" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>3.87207736332548</v>
+        <v>1.61104397300311</v>
       </c>
       <c r="D7" t="n">
-        <v>1.11942586027741</v>
+        <v>1.06142282936737</v>
       </c>
       <c r="E7" t="n">
-        <v>1.25311425665782</v>
+        <v>1.12661842270222</v>
       </c>
       <c r="F7" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G7" t="n">
-        <v>4.10843872072257</v>
+        <v>2.05823775922541</v>
       </c>
       <c r="H7" t="n">
-        <v>1.12496687440875</v>
+        <v>1.09442736265586</v>
       </c>
       <c r="I7" t="n">
-        <v>1.265550468517</v>
+        <v>1.19777125212986</v>
       </c>
       <c r="J7" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K7" t="n">
-        <v>6.80597307704862</v>
+        <v>2.09336761144225</v>
       </c>
       <c r="L7" t="n">
-        <v>1.1732958077024</v>
+        <v>1.0967450616279</v>
       </c>
       <c r="M7" t="n">
-        <v>1.37662305237203</v>
+        <v>1.20284973020519</v>
       </c>
       <c r="N7" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O7" t="n">
-        <v>3.90507538692139</v>
+        <v>1.79670947393228</v>
       </c>
       <c r="P7" t="n">
-        <v>1.12021775519978</v>
+        <v>1.07599370918285</v>
       </c>
       <c r="Q7" t="n">
-        <v>1.25488781906484</v>
+        <v>1.15776246220107</v>
       </c>
     </row>
     <row r="8">
@@ -2438,105 +2644,52 @@
         <v>23</v>
       </c>
       <c r="B8" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>1.62492792117659</v>
+        <v>3.15985652488177</v>
       </c>
       <c r="D8" t="n">
-        <v>1.06256195672155</v>
+        <v>1.12193251956872</v>
       </c>
       <c r="E8" t="n">
-        <v>1.12903791187193</v>
+        <v>1.25873257846582</v>
       </c>
       <c r="F8" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G8" t="n">
-        <v>2.11936506115047</v>
+        <v>2.62021299999999</v>
       </c>
       <c r="H8" t="n">
-        <v>1.09843843651614</v>
+        <v>1.10111748679652</v>
       </c>
       <c r="I8" t="n">
-        <v>1.20656699881603</v>
+        <v>1.21245971972909</v>
       </c>
       <c r="J8" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K8" t="n">
-        <v>2.16792918631411</v>
+        <v>4.22480137765604</v>
       </c>
       <c r="L8" t="n">
-        <v>1.10155360605282</v>
+        <v>1.1549963974175</v>
       </c>
       <c r="M8" t="n">
-        <v>1.21342034700796</v>
+        <v>1.33401667804739</v>
       </c>
       <c r="N8" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O8" t="n">
-        <v>1.83407164881423</v>
+        <v>3.42427757256006</v>
       </c>
       <c r="P8" t="n">
-        <v>1.07876547110013</v>
+        <v>1.13098513314866</v>
       </c>
       <c r="Q8" t="n">
-        <v>1.16373494163788</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="n">
-        <v>5</v>
-      </c>
-      <c r="C9" t="n">
-        <v>3.23004204051476</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1.12439994965912</v>
-      </c>
-      <c r="E9" t="n">
-        <v>1.26427524679343</v>
-      </c>
-      <c r="F9" t="n">
-        <v>5</v>
-      </c>
-      <c r="G9" t="n">
-        <v>2.61994910235162</v>
-      </c>
-      <c r="H9" t="n">
-        <v>1.10110639626739</v>
-      </c>
-      <c r="I9" t="n">
-        <v>1.21243529590096</v>
-      </c>
-      <c r="J9" t="n">
-        <v>5</v>
-      </c>
-      <c r="K9" t="n">
-        <v>4.59150026457548</v>
-      </c>
-      <c r="L9" t="n">
-        <v>1.164650081379</v>
-      </c>
-      <c r="M9" t="n">
-        <v>1.3564098120561</v>
-      </c>
-      <c r="N9" t="n">
-        <v>5</v>
-      </c>
-      <c r="O9" t="n">
-        <v>3.42896503888719</v>
-      </c>
-      <c r="P9" t="n">
-        <v>1.13113985751725</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>1.27947737726415</v>
+        <v>1.2791273714033</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor adjustment in the report generation
</commit_message>
<xml_diff>
--- a/reports/Model_results.xlsx
+++ b/reports/Model_results.xlsx
@@ -709,61 +709,61 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6.653694065171996</v>
+        <v>6.654</v>
       </c>
       <c r="C4" t="n">
-        <v>775.6443204490575</v>
+        <v>775.644</v>
       </c>
       <c r="D4" t="n">
-        <v>757.6128606890784</v>
+        <v>757.6130000000001</v>
       </c>
       <c r="E4" t="n">
-        <v>794.1049354649018</v>
+        <v>794.105</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>7.40385200862946</v>
+        <v>7.404</v>
       </c>
       <c r="H4" t="n">
-        <v>1642.298409081678</v>
+        <v>1642.298</v>
       </c>
       <c r="I4" t="n">
-        <v>1601.325489799361</v>
+        <v>1601.325</v>
       </c>
       <c r="J4" t="n">
-        <v>1684.319697433999</v>
+        <v>1684.32</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>6.526986035436765</v>
+        <v>6.527</v>
       </c>
       <c r="M4" t="n">
-        <v>683.3355555181012</v>
+        <v>683.336</v>
       </c>
       <c r="N4" t="n">
-        <v>654.0484985749043</v>
+        <v>654.048</v>
       </c>
       <c r="O4" t="n">
-        <v>713.9340315781722</v>
+        <v>713.934</v>
       </c>
       <c r="P4" t="n">
         <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>6.408315505740218</v>
+        <v>6.408</v>
       </c>
       <c r="R4" t="n">
-        <v>606.8705496166206</v>
+        <v>606.871</v>
       </c>
       <c r="S4" t="n">
-        <v>591.9044610261263</v>
+        <v>591.904</v>
       </c>
       <c r="T4" t="n">
-        <v>622.215050303064</v>
+        <v>622.215</v>
       </c>
       <c r="U4" t="n">
         <v>0</v>
@@ -776,64 +776,64 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1249029972103712</v>
+        <v>0.125</v>
       </c>
       <c r="C5" t="n">
-        <v>1.133038539836847</v>
+        <v>1.133</v>
       </c>
       <c r="D5" t="n">
-        <v>1.11842504869728</v>
+        <v>1.118</v>
       </c>
       <c r="E5" t="n">
-        <v>1.147842972804419</v>
+        <v>1.148</v>
       </c>
       <c r="F5" t="n">
-        <v>2.525597981128465e-79</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.3027858888069881</v>
+        <v>0.303</v>
       </c>
       <c r="H5" t="n">
-        <v>1.353624607233014</v>
+        <v>1.354</v>
       </c>
       <c r="I5" t="n">
-        <v>1.317348077630769</v>
+        <v>1.317</v>
       </c>
       <c r="J5" t="n">
-        <v>1.390900103336467</v>
+        <v>1.391</v>
       </c>
       <c r="K5" t="n">
-        <v>8.495910382923312e-106</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>0.1056225768246586</v>
+        <v>0.106</v>
       </c>
       <c r="M5" t="n">
-        <v>1.111402328342066</v>
+        <v>1.111</v>
       </c>
       <c r="N5" t="n">
-        <v>1.086557815035486</v>
+        <v>1.087</v>
       </c>
       <c r="O5" t="n">
-        <v>1.136814919879643</v>
+        <v>1.137</v>
       </c>
       <c r="P5" t="n">
-        <v>5.343869709449388e-20</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.01446299795390154</v>
+        <v>0.014</v>
       </c>
       <c r="R5" t="n">
-        <v>1.014568093161488</v>
+        <v>1.015</v>
       </c>
       <c r="S5" t="n">
-        <v>0.9912035779283578</v>
+        <v>0.991</v>
       </c>
       <c r="T5" t="n">
-        <v>1.03848335355357</v>
+        <v>1.038</v>
       </c>
       <c r="U5" t="n">
-        <v>0.2237205265092796</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="6">
@@ -843,64 +843,64 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.06152126658156877</v>
+        <v>0.062</v>
       </c>
       <c r="C6" t="n">
-        <v>1.063453112300676</v>
+        <v>1.063</v>
       </c>
       <c r="D6" t="n">
-        <v>1.05031979606189</v>
+        <v>1.05</v>
       </c>
       <c r="E6" t="n">
-        <v>1.076750648995055</v>
+        <v>1.077</v>
       </c>
       <c r="F6" t="n">
-        <v>2.917583082418097e-22</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.1290588166775204</v>
+        <v>-0.129</v>
       </c>
       <c r="H6" t="n">
-        <v>0.878922268737635</v>
+        <v>0.879</v>
       </c>
       <c r="I6" t="n">
-        <v>0.8692633268130071</v>
+        <v>0.869</v>
       </c>
       <c r="J6" t="n">
-        <v>0.8886885373562872</v>
+        <v>0.889</v>
       </c>
       <c r="K6" t="n">
-        <v>5.749179130177811e-116</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.1369727623241402</v>
+        <v>-0.137</v>
       </c>
       <c r="M6" t="n">
-        <v>0.8719939768979446</v>
+        <v>0.872</v>
       </c>
       <c r="N6" t="n">
-        <v>0.8613328043847791</v>
+        <v>0.861</v>
       </c>
       <c r="O6" t="n">
-        <v>0.8827871083923271</v>
+        <v>0.883</v>
       </c>
       <c r="P6" t="n">
-        <v>1.391374302278439e-105</v>
+        <v>0</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.2771126936355223</v>
+        <v>0.277</v>
       </c>
       <c r="R6" t="n">
-        <v>1.319315041066095</v>
+        <v>1.319</v>
       </c>
       <c r="S6" t="n">
-        <v>1.296857383137012</v>
+        <v>1.297</v>
       </c>
       <c r="T6" t="n">
-        <v>1.342161597887392</v>
+        <v>1.342</v>
       </c>
       <c r="U6" t="n">
-        <v>1.225430070380547e-219</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -910,64 +910,64 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.4678338514039946</v>
+        <v>0.468</v>
       </c>
       <c r="C7" t="n">
-        <v>1.596532119079351</v>
+        <v>1.597</v>
       </c>
       <c r="D7" t="n">
-        <v>1.578114178404571</v>
+        <v>1.578</v>
       </c>
       <c r="E7" t="n">
-        <v>1.615165012856601</v>
+        <v>1.615</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2943078596261209</v>
+        <v>0.294</v>
       </c>
       <c r="H7" t="n">
-        <v>1.34219704834991</v>
+        <v>1.342</v>
       </c>
       <c r="I7" t="n">
-        <v>1.323361626882931</v>
+        <v>1.323</v>
       </c>
       <c r="J7" t="n">
-        <v>1.361300554590266</v>
+        <v>1.361</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.1210970120014277</v>
+        <v>-0.121</v>
       </c>
       <c r="M7" t="n">
-        <v>0.885948007834366</v>
+        <v>0.886</v>
       </c>
       <c r="N7" t="n">
-        <v>0.8767141321965969</v>
+        <v>0.877</v>
       </c>
       <c r="O7" t="n">
-        <v>0.8952791380459609</v>
+        <v>0.895</v>
       </c>
       <c r="P7" t="n">
-        <v>1.292712331667857e-113</v>
+        <v>0</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.05696231443909502</v>
+        <v>-0.057</v>
       </c>
       <c r="R7" t="n">
-        <v>0.9446296675946203</v>
+        <v>0.945</v>
       </c>
       <c r="S7" t="n">
-        <v>0.9284933106378211</v>
+        <v>0.928</v>
       </c>
       <c r="T7" t="n">
-        <v>0.9610464595452466</v>
+        <v>0.961</v>
       </c>
       <c r="U7" t="n">
-        <v>9.189718745563419e-11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -977,64 +977,64 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.5891912224409646</v>
+        <v>0.589</v>
       </c>
       <c r="C8" t="n">
-        <v>1.802529979905171</v>
+        <v>1.803</v>
       </c>
       <c r="D8" t="n">
-        <v>1.774681569036421</v>
+        <v>1.775</v>
       </c>
       <c r="E8" t="n">
-        <v>1.830815389727112</v>
+        <v>1.831</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.2616913818212571</v>
+        <v>0.262</v>
       </c>
       <c r="H8" t="n">
-        <v>1.299125546795083</v>
+        <v>1.299</v>
       </c>
       <c r="I8" t="n">
-        <v>1.271258177371035</v>
+        <v>1.271</v>
       </c>
       <c r="J8" t="n">
-        <v>1.327603799431086</v>
+        <v>1.328</v>
       </c>
       <c r="K8" t="n">
-        <v>1.090492217249523e-123</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.09407923533634065</v>
+        <v>-0.094</v>
       </c>
       <c r="M8" t="n">
-        <v>0.9102106385373464</v>
+        <v>0.91</v>
       </c>
       <c r="N8" t="n">
-        <v>0.8920229325831337</v>
+        <v>0.892</v>
       </c>
       <c r="O8" t="n">
-        <v>0.9287691787333638</v>
+        <v>0.929</v>
       </c>
       <c r="P8" t="n">
-        <v>6.513105643841843e-20</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>-0.05029707666995033</v>
+        <v>-0.05</v>
       </c>
       <c r="R8" t="n">
-        <v>0.9509468784019296</v>
+        <v>0.951</v>
       </c>
       <c r="S8" t="n">
-        <v>0.9343983024826471</v>
+        <v>0.9340000000000001</v>
       </c>
       <c r="T8" t="n">
-        <v>0.9677885363658056</v>
+        <v>0.968</v>
       </c>
       <c r="U8" t="n">
-        <v>1.961192430560364e-08</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1044,64 +1044,64 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.6220827950934207</v>
+        <v>0.622</v>
       </c>
       <c r="C9" t="n">
-        <v>1.862803842899517</v>
+        <v>1.863</v>
       </c>
       <c r="D9" t="n">
-        <v>1.84315998160072</v>
+        <v>1.843</v>
       </c>
       <c r="E9" t="n">
-        <v>1.882657062740479</v>
+        <v>1.883</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.3558725408372717</v>
+        <v>0.356</v>
       </c>
       <c r="H9" t="n">
-        <v>1.427425598196886</v>
+        <v>1.427</v>
       </c>
       <c r="I9" t="n">
-        <v>1.404654319573738</v>
+        <v>1.405</v>
       </c>
       <c r="J9" t="n">
-        <v>1.450566028947293</v>
+        <v>1.451</v>
       </c>
       <c r="K9" t="n">
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>0.04366230913117231</v>
+        <v>0.044</v>
       </c>
       <c r="M9" t="n">
-        <v>1.044629533464751</v>
+        <v>1.045</v>
       </c>
       <c r="N9" t="n">
-        <v>1.033954282469107</v>
+        <v>1.034</v>
       </c>
       <c r="O9" t="n">
-        <v>1.055415003051055</v>
+        <v>1.055</v>
       </c>
       <c r="P9" t="n">
-        <v>7.998987836615423e-17</v>
+        <v>0</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.2307326559880605</v>
+        <v>0.231</v>
       </c>
       <c r="R9" t="n">
-        <v>1.259522468644513</v>
+        <v>1.26</v>
       </c>
       <c r="S9" t="n">
-        <v>1.237803528534077</v>
+        <v>1.238</v>
       </c>
       <c r="T9" t="n">
-        <v>1.281622496987973</v>
+        <v>1.282</v>
       </c>
       <c r="U9" t="n">
-        <v>5.113138271252217e-149</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1111,64 +1111,64 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.6339208977587847</v>
+        <v>0.634</v>
       </c>
       <c r="C10" t="n">
-        <v>1.884986949924032</v>
+        <v>1.885</v>
       </c>
       <c r="D10" t="n">
-        <v>1.865691073927753</v>
+        <v>1.866</v>
       </c>
       <c r="E10" t="n">
-        <v>1.904482393166822</v>
+        <v>1.904</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.3816904105703115</v>
+        <v>0.382</v>
       </c>
       <c r="H10" t="n">
-        <v>1.464758541168982</v>
+        <v>1.465</v>
       </c>
       <c r="I10" t="n">
-        <v>1.430094360949287</v>
+        <v>1.43</v>
       </c>
       <c r="J10" t="n">
-        <v>1.500262949434542</v>
+        <v>1.5</v>
       </c>
       <c r="K10" t="n">
-        <v>3.4688202214557e-214</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.1268749410218937</v>
+        <v>-0.127</v>
       </c>
       <c r="M10" t="n">
-        <v>0.8808438231377492</v>
+        <v>0.881</v>
       </c>
       <c r="N10" t="n">
-        <v>0.870222682270393</v>
+        <v>0.87</v>
       </c>
       <c r="O10" t="n">
-        <v>0.8915945959207318</v>
+        <v>0.892</v>
       </c>
       <c r="P10" t="n">
-        <v>2.224608982617227e-93</v>
+        <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.1746521819513246</v>
+        <v>0.175</v>
       </c>
       <c r="R10" t="n">
-        <v>1.190831951726383</v>
+        <v>1.191</v>
       </c>
       <c r="S10" t="n">
-        <v>1.170940448605159</v>
+        <v>1.171</v>
       </c>
       <c r="T10" t="n">
-        <v>1.211061364343254</v>
+        <v>1.211</v>
       </c>
       <c r="U10" t="n">
-        <v>8.327684885107373e-92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -1178,64 +1178,64 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.08609264833499294</v>
+        <v>-0.08599999999999999</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9175092215804909</v>
+        <v>0.918</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9058539366279749</v>
+        <v>0.906</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9293144707400732</v>
+        <v>0.929</v>
       </c>
       <c r="F11" t="n">
-        <v>8.935695909321513e-40</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.07213108208518282</v>
+        <v>-0.07199999999999999</v>
       </c>
       <c r="H11" t="n">
-        <v>0.9304089278751361</v>
+        <v>0.93</v>
       </c>
       <c r="I11" t="n">
-        <v>0.915211282227768</v>
+        <v>0.915</v>
       </c>
       <c r="J11" t="n">
-        <v>0.945858939765915</v>
+        <v>0.946</v>
       </c>
       <c r="K11" t="n">
-        <v>9.151913301287251e-18</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>0.201177753474984</v>
+        <v>0.201</v>
       </c>
       <c r="M11" t="n">
-        <v>1.222842116941473</v>
+        <v>1.223</v>
       </c>
       <c r="N11" t="n">
-        <v>1.194375950156493</v>
+        <v>1.194</v>
       </c>
       <c r="O11" t="n">
-        <v>1.251986732293107</v>
+        <v>1.252</v>
       </c>
       <c r="P11" t="n">
-        <v>6.658339096800721e-63</v>
+        <v>0</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.006774804599330751</v>
+        <v>0.007</v>
       </c>
       <c r="R11" t="n">
-        <v>1.006797805500877</v>
+        <v>1.007</v>
       </c>
       <c r="S11" t="n">
-        <v>0.9991378648589274</v>
+        <v>0.999</v>
       </c>
       <c r="T11" t="n">
-        <v>1.014516471462626</v>
+        <v>1.015</v>
       </c>
       <c r="U11" t="n">
-        <v>0.08210184892209839</v>
+        <v>0.082</v>
       </c>
     </row>
     <row r="12">
@@ -1245,61 +1245,61 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.07465257083557482</v>
+        <v>0.075</v>
       </c>
       <c r="C12" t="n">
-        <v>1.077509727541303</v>
+        <v>1.078</v>
       </c>
       <c r="D12" t="n">
-        <v>1.063353767195672</v>
+        <v>1.063</v>
       </c>
       <c r="E12" t="n">
-        <v>1.091854139951985</v>
+        <v>1.092</v>
       </c>
       <c r="F12" t="n">
-        <v>1.878626565235248e-28</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.04224488454998609</v>
+        <v>-0.042</v>
       </c>
       <c r="H12" t="n">
-        <v>0.9586349969263909</v>
+        <v>0.959</v>
       </c>
       <c r="I12" t="n">
-        <v>0.9423003823438444</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="J12" t="n">
-        <v>0.9752527692350296</v>
+        <v>0.975</v>
       </c>
       <c r="K12" t="n">
-        <v>1.452205406421525e-06</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>0.2958245090916408</v>
+        <v>0.296</v>
       </c>
       <c r="M12" t="n">
-        <v>1.344234235244621</v>
+        <v>1.344</v>
       </c>
       <c r="N12" t="n">
-        <v>1.312206168383227</v>
+        <v>1.312</v>
       </c>
       <c r="O12" t="n">
-        <v>1.377044036784294</v>
+        <v>1.377</v>
       </c>
       <c r="P12" t="n">
-        <v>9.72545415980767e-128</v>
+        <v>0</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.2640070487770936</v>
+        <v>0.264</v>
       </c>
       <c r="R12" t="n">
-        <v>1.302137374744645</v>
+        <v>1.302</v>
       </c>
       <c r="S12" t="n">
-        <v>1.291036264922997</v>
+        <v>1.291</v>
       </c>
       <c r="T12" t="n">
-        <v>1.313333938615588</v>
+        <v>1.313</v>
       </c>
       <c r="U12" t="n">
         <v>0</v>
@@ -1312,61 +1312,61 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.2975260969293818</v>
+        <v>0.298</v>
       </c>
       <c r="C13" t="n">
-        <v>1.346523515023337</v>
+        <v>1.347</v>
       </c>
       <c r="D13" t="n">
-        <v>1.328546724428843</v>
+        <v>1.329</v>
       </c>
       <c r="E13" t="n">
-        <v>1.364743552614069</v>
+        <v>1.365</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.0252317182106811</v>
+        <v>-0.025</v>
       </c>
       <c r="H13" t="n">
-        <v>0.9750839411424537</v>
+        <v>0.975</v>
       </c>
       <c r="I13" t="n">
-        <v>0.9581795467773879</v>
+        <v>0.958</v>
       </c>
       <c r="J13" t="n">
-        <v>0.992286566199054</v>
+        <v>0.992</v>
       </c>
       <c r="K13" t="n">
-        <v>0.004687232321772079</v>
+        <v>0.005</v>
       </c>
       <c r="L13" t="n">
-        <v>0.4595282099994731</v>
+        <v>0.46</v>
       </c>
       <c r="M13" t="n">
-        <v>1.583326810996736</v>
+        <v>1.583</v>
       </c>
       <c r="N13" t="n">
-        <v>1.546007909611866</v>
+        <v>1.546</v>
       </c>
       <c r="O13" t="n">
-        <v>1.621546548911559</v>
+        <v>1.622</v>
       </c>
       <c r="P13" t="n">
         <v>0</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.4543485283843902</v>
+        <v>0.454</v>
       </c>
       <c r="R13" t="n">
-        <v>1.575146885217066</v>
+        <v>1.575</v>
       </c>
       <c r="S13" t="n">
-        <v>1.560247823337499</v>
+        <v>1.56</v>
       </c>
       <c r="T13" t="n">
-        <v>1.590188220677516</v>
+        <v>1.59</v>
       </c>
       <c r="U13" t="n">
         <v>0</v>
@@ -1379,61 +1379,61 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.2603983836940528</v>
+        <v>0.26</v>
       </c>
       <c r="C14" t="n">
-        <v>1.297446865395901</v>
+        <v>1.297</v>
       </c>
       <c r="D14" t="n">
-        <v>1.28044260550035</v>
+        <v>1.28</v>
       </c>
       <c r="E14" t="n">
-        <v>1.31467694162508</v>
+        <v>1.315</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0.1195123546732364</v>
+        <v>0.12</v>
       </c>
       <c r="H14" t="n">
-        <v>1.126947167045202</v>
+        <v>1.127</v>
       </c>
       <c r="I14" t="n">
-        <v>1.108433190378345</v>
+        <v>1.108</v>
       </c>
       <c r="J14" t="n">
-        <v>1.145770379609176</v>
+        <v>1.146</v>
       </c>
       <c r="K14" t="n">
-        <v>2.1297826359626e-45</v>
+        <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>0.4121663588025503</v>
+        <v>0.412</v>
       </c>
       <c r="M14" t="n">
-        <v>1.510085631471304</v>
+        <v>1.51</v>
       </c>
       <c r="N14" t="n">
-        <v>1.474629264542815</v>
+        <v>1.475</v>
       </c>
       <c r="O14" t="n">
-        <v>1.546394520444482</v>
+        <v>1.546</v>
       </c>
       <c r="P14" t="n">
-        <v>2.228333985493853e-253</v>
+        <v>0</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.5173739872844975</v>
+        <v>0.517</v>
       </c>
       <c r="R14" t="n">
-        <v>1.677616418212903</v>
+        <v>1.678</v>
       </c>
       <c r="S14" t="n">
-        <v>1.660988449558783</v>
+        <v>1.661</v>
       </c>
       <c r="T14" t="n">
-        <v>1.694410847592043</v>
+        <v>1.694</v>
       </c>
       <c r="U14" t="n">
         <v>0</v>
@@ -1446,61 +1446,61 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.8717504375519823</v>
+        <v>0.872</v>
       </c>
       <c r="C15" t="n">
-        <v>2.391092650835281</v>
+        <v>2.391</v>
       </c>
       <c r="D15" t="n">
-        <v>2.3285361954902</v>
+        <v>2.329</v>
       </c>
       <c r="E15" t="n">
-        <v>2.45532969423088</v>
+        <v>2.455</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>0.4741880183604993</v>
+        <v>0.474</v>
       </c>
       <c r="H15" t="n">
-        <v>1.606709049431205</v>
+        <v>1.607</v>
       </c>
       <c r="I15" t="n">
-        <v>1.561454371390686</v>
+        <v>1.561</v>
       </c>
       <c r="J15" t="n">
-        <v>1.653275316156014</v>
+        <v>1.653</v>
       </c>
       <c r="K15" t="n">
-        <v>4.02463352444384e-232</v>
+        <v>0</v>
       </c>
       <c r="L15" t="n">
-        <v>0.4448918650237251</v>
+        <v>0.445</v>
       </c>
       <c r="M15" t="n">
-        <v>1.560321461385575</v>
+        <v>1.56</v>
       </c>
       <c r="N15" t="n">
-        <v>1.499721185466612</v>
+        <v>1.5</v>
       </c>
       <c r="O15" t="n">
-        <v>1.623370454757517</v>
+        <v>1.623</v>
       </c>
       <c r="P15" t="n">
-        <v>2.187747226661654e-107</v>
+        <v>0</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.6370943669946615</v>
+        <v>0.637</v>
       </c>
       <c r="R15" t="n">
-        <v>1.890978399832349</v>
+        <v>1.891</v>
       </c>
       <c r="S15" t="n">
-        <v>1.847210629613217</v>
+        <v>1.847</v>
       </c>
       <c r="T15" t="n">
-        <v>1.935783202688282</v>
+        <v>1.936</v>
       </c>
       <c r="U15" t="n">
         <v>0</v>
@@ -1513,61 +1513,61 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.8640548186054547</v>
+        <v>0.864</v>
       </c>
       <c r="C16" t="n">
-        <v>2.372762334955616</v>
+        <v>2.373</v>
       </c>
       <c r="D16" t="n">
-        <v>2.325924233270509</v>
+        <v>2.326</v>
       </c>
       <c r="E16" t="n">
-        <v>2.42054363493501</v>
+        <v>2.421</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>0.4574747951758786</v>
+        <v>0.457</v>
       </c>
       <c r="H16" t="n">
-        <v>1.580078920027403</v>
+        <v>1.58</v>
       </c>
       <c r="I16" t="n">
-        <v>1.54638432518579</v>
+        <v>1.546</v>
       </c>
       <c r="J16" t="n">
-        <v>1.61450769569525</v>
+        <v>1.615</v>
       </c>
       <c r="K16" t="n">
         <v>0</v>
       </c>
       <c r="L16" t="n">
-        <v>0.5067039036016099</v>
+        <v>0.507</v>
       </c>
       <c r="M16" t="n">
-        <v>1.659811270776386</v>
+        <v>1.66</v>
       </c>
       <c r="N16" t="n">
-        <v>1.600389125342344</v>
+        <v>1.6</v>
       </c>
       <c r="O16" t="n">
-        <v>1.72143974922786</v>
+        <v>1.721</v>
       </c>
       <c r="P16" t="n">
-        <v>2.134680170008171e-163</v>
+        <v>0</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.6502369331052154</v>
+        <v>0.65</v>
       </c>
       <c r="R16" t="n">
-        <v>1.915994737821569</v>
+        <v>1.916</v>
       </c>
       <c r="S16" t="n">
-        <v>1.879898880354268</v>
+        <v>1.88</v>
       </c>
       <c r="T16" t="n">
-        <v>1.952783670294082</v>
+        <v>1.953</v>
       </c>
       <c r="U16" t="n">
         <v>0</v>
@@ -1580,61 +1580,61 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.6349610133172627</v>
+        <v>0.635</v>
       </c>
       <c r="C17" t="n">
-        <v>1.886948574159272</v>
+        <v>1.887</v>
       </c>
       <c r="D17" t="n">
-        <v>1.850458027814796</v>
+        <v>1.85</v>
       </c>
       <c r="E17" t="n">
-        <v>1.924158704494578</v>
+        <v>1.924</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>0.3255971124211283</v>
+        <v>0.326</v>
       </c>
       <c r="H17" t="n">
-        <v>1.384857314653193</v>
+        <v>1.385</v>
       </c>
       <c r="I17" t="n">
-        <v>1.357250703595441</v>
+        <v>1.357</v>
       </c>
       <c r="J17" t="n">
-        <v>1.413025446859599</v>
+        <v>1.413</v>
       </c>
       <c r="K17" t="n">
-        <v>1.975963775608436e-220</v>
+        <v>0</v>
       </c>
       <c r="L17" t="n">
-        <v>0.4158423848672826</v>
+        <v>0.416</v>
       </c>
       <c r="M17" t="n">
-        <v>1.515646961146393</v>
+        <v>1.516</v>
       </c>
       <c r="N17" t="n">
-        <v>1.461952456758626</v>
+        <v>1.462</v>
       </c>
       <c r="O17" t="n">
-        <v>1.571313554153131</v>
+        <v>1.571</v>
       </c>
       <c r="P17" t="n">
-        <v>4.718714182669317e-113</v>
+        <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.5013183229232893</v>
+        <v>0.501</v>
       </c>
       <c r="R17" t="n">
-        <v>1.650896251093657</v>
+        <v>1.651</v>
       </c>
       <c r="S17" t="n">
-        <v>1.619950925990413</v>
+        <v>1.62</v>
       </c>
       <c r="T17" t="n">
-        <v>1.682432713329749</v>
+        <v>1.682</v>
       </c>
       <c r="U17" t="n">
         <v>0</v>
@@ -1647,64 +1647,64 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.3692192260218174</v>
+        <v>0.369</v>
       </c>
       <c r="C18" t="n">
-        <v>1.446604702309363</v>
+        <v>1.447</v>
       </c>
       <c r="D18" t="n">
-        <v>1.415418039188353</v>
+        <v>1.415</v>
       </c>
       <c r="E18" t="n">
-        <v>1.478478517868519</v>
+        <v>1.478</v>
       </c>
       <c r="F18" t="n">
-        <v>9.449975656248431e-242</v>
+        <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>0.04956812229553847</v>
+        <v>0.05</v>
       </c>
       <c r="H18" t="n">
-        <v>1.050817173854718</v>
+        <v>1.051</v>
       </c>
       <c r="I18" t="n">
-        <v>1.028196511516865</v>
+        <v>1.028</v>
       </c>
       <c r="J18" t="n">
-        <v>1.073935498223974</v>
+        <v>1.074</v>
       </c>
       <c r="K18" t="n">
-        <v>8.032290906752875e-06</v>
+        <v>0</v>
       </c>
       <c r="L18" t="n">
-        <v>0.1546459836107757</v>
+        <v>0.155</v>
       </c>
       <c r="M18" t="n">
-        <v>1.167244664211139</v>
+        <v>1.167</v>
       </c>
       <c r="N18" t="n">
-        <v>1.123882052451036</v>
+        <v>1.124</v>
       </c>
       <c r="O18" t="n">
-        <v>1.212280330625471</v>
+        <v>1.212</v>
       </c>
       <c r="P18" t="n">
-        <v>1.180926237158062e-15</v>
+        <v>0</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.3005192481228183</v>
+        <v>0.301</v>
       </c>
       <c r="R18" t="n">
-        <v>1.350559901232937</v>
+        <v>1.351</v>
       </c>
       <c r="S18" t="n">
-        <v>1.321418738087801</v>
+        <v>1.321</v>
       </c>
       <c r="T18" t="n">
-        <v>1.380343712590161</v>
+        <v>1.38</v>
       </c>
       <c r="U18" t="n">
-        <v>1.392270680975141e-160</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1714,61 +1714,61 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.8923333567972855</v>
+        <v>0.892</v>
       </c>
       <c r="C19" t="n">
-        <v>2.440818311870382</v>
+        <v>2.441</v>
       </c>
       <c r="D19" t="n">
-        <v>2.38913471231449</v>
+        <v>2.389</v>
       </c>
       <c r="E19" t="n">
-        <v>2.493619970801194</v>
+        <v>2.494</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>0.4094446794959185</v>
+        <v>0.409</v>
       </c>
       <c r="H19" t="n">
-        <v>1.505981250594748</v>
+        <v>1.506</v>
       </c>
       <c r="I19" t="n">
-        <v>1.474393776410798</v>
+        <v>1.474</v>
       </c>
       <c r="J19" t="n">
-        <v>1.538245456152152</v>
+        <v>1.538</v>
       </c>
       <c r="K19" t="n">
         <v>0</v>
       </c>
       <c r="L19" t="n">
-        <v>0.4863679009000694</v>
+        <v>0.486</v>
       </c>
       <c r="M19" t="n">
-        <v>1.626398239533661</v>
+        <v>1.626</v>
       </c>
       <c r="N19" t="n">
-        <v>1.567086367391131</v>
+        <v>1.567</v>
       </c>
       <c r="O19" t="n">
-        <v>1.687954977211527</v>
+        <v>1.688</v>
       </c>
       <c r="P19" t="n">
-        <v>3.27202687222201e-145</v>
+        <v>0</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.734990247102709</v>
+        <v>0.735</v>
       </c>
       <c r="R19" t="n">
-        <v>2.085461653112537</v>
+        <v>2.085</v>
       </c>
       <c r="S19" t="n">
-        <v>2.043997496535683</v>
+        <v>2.044</v>
       </c>
       <c r="T19" t="n">
-        <v>2.127766943929302</v>
+        <v>2.128</v>
       </c>
       <c r="U19" t="n">
         <v>0</v>
@@ -1781,61 +1781,61 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.0005026253345663635</v>
+        <v>0.001</v>
       </c>
       <c r="C20" t="n">
-        <v>1.000502751671846</v>
+        <v>1.001</v>
       </c>
       <c r="D20" t="n">
-        <v>1.000456433425546</v>
+        <v>1</v>
       </c>
       <c r="E20" t="n">
-        <v>1.000549072062547</v>
+        <v>1.001</v>
       </c>
       <c r="F20" t="n">
-        <v>1.781792304658911e-100</v>
+        <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>0.001538049822201306</v>
+        <v>0.002</v>
       </c>
       <c r="H20" t="n">
-        <v>1.001539233227463</v>
+        <v>1.002</v>
       </c>
       <c r="I20" t="n">
-        <v>1.001487665640435</v>
+        <v>1.001</v>
       </c>
       <c r="J20" t="n">
-        <v>1.001590803469758</v>
+        <v>1.002</v>
       </c>
       <c r="K20" t="n">
         <v>0</v>
       </c>
       <c r="L20" t="n">
-        <v>-2.505158541384011e-05</v>
+        <v>-0</v>
       </c>
       <c r="M20" t="n">
-        <v>0.9999749487283746</v>
+        <v>1</v>
       </c>
       <c r="N20" t="n">
-        <v>0.9999222505835584</v>
+        <v>1</v>
       </c>
       <c r="O20" t="n">
-        <v>1.000027649650501</v>
+        <v>1</v>
       </c>
       <c r="P20" t="n">
-        <v>0.3515031631568395</v>
+        <v>0.352</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.001564107181939395</v>
+        <v>0.002</v>
       </c>
       <c r="R20" t="n">
-        <v>1.001565331035574</v>
+        <v>1.002</v>
       </c>
       <c r="S20" t="n">
-        <v>1.001520303580794</v>
+        <v>1.002</v>
       </c>
       <c r="T20" t="n">
-        <v>1.001610360514748</v>
+        <v>1.002</v>
       </c>
       <c r="U20" t="n">
         <v>0</v>
@@ -1848,61 +1848,61 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.5116283490096347</v>
+        <v>0.512</v>
       </c>
       <c r="C21" t="n">
-        <v>1.66800507918963</v>
+        <v>1.668</v>
       </c>
       <c r="D21" t="n">
-        <v>1.642830633430284</v>
+        <v>1.643</v>
       </c>
       <c r="E21" t="n">
-        <v>1.693565293698593</v>
+        <v>1.694</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>0.4806473634863596</v>
+        <v>0.481</v>
       </c>
       <c r="H21" t="n">
-        <v>1.617120928457011</v>
+        <v>1.617</v>
       </c>
       <c r="I21" t="n">
-        <v>1.595645303848412</v>
+        <v>1.596</v>
       </c>
       <c r="J21" t="n">
-        <v>1.638885591269287</v>
+        <v>1.639</v>
       </c>
       <c r="K21" t="n">
         <v>0</v>
       </c>
       <c r="L21" t="n">
-        <v>0.2100274559687152</v>
+        <v>0.21</v>
       </c>
       <c r="M21" t="n">
-        <v>1.233711932247958</v>
+        <v>1.234</v>
       </c>
       <c r="N21" t="n">
-        <v>1.21086769543165</v>
+        <v>1.211</v>
       </c>
       <c r="O21" t="n">
-        <v>1.256987148565733</v>
+        <v>1.257</v>
       </c>
       <c r="P21" t="n">
-        <v>1.671877867185021e-107</v>
+        <v>0</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.4239058132736776</v>
+        <v>0.424</v>
       </c>
       <c r="R21" t="n">
-        <v>1.52791767744253</v>
+        <v>1.528</v>
       </c>
       <c r="S21" t="n">
-        <v>1.507852653571316</v>
+        <v>1.508</v>
       </c>
       <c r="T21" t="n">
-        <v>1.548249706967115</v>
+        <v>1.548</v>
       </c>
       <c r="U21" t="n">
         <v>0</v>
@@ -1915,61 +1915,61 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.4359309841668994</v>
+        <v>0.436</v>
       </c>
       <c r="C22" t="n">
-        <v>1.54640206483958</v>
+        <v>1.546</v>
       </c>
       <c r="D22" t="n">
-        <v>1.535089956947911</v>
+        <v>1.535</v>
       </c>
       <c r="E22" t="n">
-        <v>1.557797531875365</v>
+        <v>1.558</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>0.1608721137566806</v>
+        <v>0.161</v>
       </c>
       <c r="H22" t="n">
-        <v>1.174534752371639</v>
+        <v>1.175</v>
       </c>
       <c r="I22" t="n">
-        <v>1.164602947177249</v>
+        <v>1.165</v>
       </c>
       <c r="J22" t="n">
-        <v>1.184551256608444</v>
+        <v>1.185</v>
       </c>
       <c r="K22" t="n">
-        <v>9.251637423686757e-302</v>
+        <v>0</v>
       </c>
       <c r="L22" t="n">
-        <v>0.4519370166336108</v>
+        <v>0.452</v>
       </c>
       <c r="M22" t="n">
-        <v>1.571352976360643</v>
+        <v>1.571</v>
       </c>
       <c r="N22" t="n">
-        <v>1.553910983625425</v>
+        <v>1.554</v>
       </c>
       <c r="O22" t="n">
-        <v>1.588990748077915</v>
+        <v>1.589</v>
       </c>
       <c r="P22" t="n">
         <v>0</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.2964648864466628</v>
+        <v>0.296</v>
       </c>
       <c r="R22" t="n">
-        <v>1.34509532809147</v>
+        <v>1.345</v>
       </c>
       <c r="S22" t="n">
-        <v>1.333247405673994</v>
+        <v>1.333</v>
       </c>
       <c r="T22" t="n">
-        <v>1.357048537243436</v>
+        <v>1.357</v>
       </c>
       <c r="U22" t="n">
         <v>0</v>
@@ -1982,61 +1982,61 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.01545827949379634</v>
+        <v>0.015</v>
       </c>
       <c r="C23" t="n">
-        <v>1.015578376730474</v>
+        <v>1.016</v>
       </c>
       <c r="D23" t="n">
-        <v>1.01404407418431</v>
+        <v>1.014</v>
       </c>
       <c r="E23" t="n">
-        <v>1.017115000757886</v>
+        <v>1.017</v>
       </c>
       <c r="F23" t="n">
-        <v>2.50059771791569e-89</v>
+        <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.00976616818931531</v>
+        <v>-0.01</v>
       </c>
       <c r="H23" t="n">
-        <v>0.9902813659632052</v>
+        <v>0.99</v>
       </c>
       <c r="I23" t="n">
-        <v>0.988238203307089</v>
+        <v>0.988</v>
       </c>
       <c r="J23" t="n">
-        <v>0.9923287528171163</v>
+        <v>0.992</v>
       </c>
       <c r="K23" t="n">
-        <v>1.899147908294156e-20</v>
+        <v>0</v>
       </c>
       <c r="L23" t="n">
-        <v>0.005125954721793496</v>
+        <v>0.005</v>
       </c>
       <c r="M23" t="n">
-        <v>1.005139114904256</v>
+        <v>1.005</v>
       </c>
       <c r="N23" t="n">
-        <v>1.002347358854742</v>
+        <v>1.002</v>
       </c>
       <c r="O23" t="n">
-        <v>1.00793864660337</v>
+        <v>1.008</v>
       </c>
       <c r="P23" t="n">
-        <v>0.0003036496628352932</v>
+        <v>0</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.267416494438307</v>
+        <v>0.267</v>
       </c>
       <c r="R23" t="n">
-        <v>1.306584518206345</v>
+        <v>1.307</v>
       </c>
       <c r="S23" t="n">
-        <v>1.295616253795638</v>
+        <v>1.296</v>
       </c>
       <c r="T23" t="n">
-        <v>1.317645636364318</v>
+        <v>1.318</v>
       </c>
       <c r="U23" t="n">
         <v>0</v>
@@ -2217,61 +2217,61 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6.653694399219825</v>
+        <v>6.654</v>
       </c>
       <c r="C4" t="n">
-        <v>775.6445795514018</v>
+        <v>775.645</v>
       </c>
       <c r="D4" t="n">
-        <v>757.613111323658</v>
+        <v>757.6130000000001</v>
       </c>
       <c r="E4" t="n">
-        <v>794.1052032961085</v>
+        <v>794.105</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>7.40385181276367</v>
+        <v>7.404</v>
       </c>
       <c r="H4" t="n">
-        <v>1642.298087411634</v>
+        <v>1642.298</v>
       </c>
       <c r="I4" t="n">
-        <v>1601.325170017269</v>
+        <v>1601.325</v>
       </c>
       <c r="J4" t="n">
-        <v>1684.319373988747</v>
+        <v>1684.319</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>6.526989397862481</v>
+        <v>6.527</v>
       </c>
       <c r="M4" t="n">
-        <v>683.3378531870082</v>
+        <v>683.338</v>
       </c>
       <c r="N4" t="n">
-        <v>654.0507448668953</v>
+        <v>654.051</v>
       </c>
       <c r="O4" t="n">
-        <v>713.9363807211282</v>
+        <v>713.936</v>
       </c>
       <c r="P4" t="n">
         <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>6.408316742608752</v>
+        <v>6.408</v>
       </c>
       <c r="R4" t="n">
-        <v>606.8713002361723</v>
+        <v>606.871</v>
       </c>
       <c r="S4" t="n">
-        <v>591.9051919837113</v>
+        <v>591.905</v>
       </c>
       <c r="T4" t="n">
-        <v>622.2158211115631</v>
+        <v>622.216</v>
       </c>
       <c r="U4" t="n">
         <v>0</v>
@@ -2284,64 +2284,64 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1249029972103602</v>
+        <v>0.125</v>
       </c>
       <c r="C5" t="n">
-        <v>1.133038539836834</v>
+        <v>1.133</v>
       </c>
       <c r="D5" t="n">
-        <v>1.118425048697268</v>
+        <v>1.118</v>
       </c>
       <c r="E5" t="n">
-        <v>1.147842972804406</v>
+        <v>1.148</v>
       </c>
       <c r="F5" t="n">
-        <v>2.525597981182667e-79</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.3027858888069986</v>
+        <v>0.303</v>
       </c>
       <c r="H5" t="n">
-        <v>1.353624607233029</v>
+        <v>1.354</v>
       </c>
       <c r="I5" t="n">
-        <v>1.31734807763079</v>
+        <v>1.317</v>
       </c>
       <c r="J5" t="n">
-        <v>1.390900103336474</v>
+        <v>1.391</v>
       </c>
       <c r="K5" t="n">
-        <v>8.49591038201229e-106</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>0.105622576824604</v>
+        <v>0.106</v>
       </c>
       <c r="M5" t="n">
-        <v>1.111402328342006</v>
+        <v>1.111</v>
       </c>
       <c r="N5" t="n">
-        <v>1.086557815035428</v>
+        <v>1.087</v>
       </c>
       <c r="O5" t="n">
-        <v>1.136814919879579</v>
+        <v>1.137</v>
       </c>
       <c r="P5" t="n">
-        <v>5.343869709664464e-20</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.01446299795393729</v>
+        <v>0.014</v>
       </c>
       <c r="R5" t="n">
-        <v>1.014568093161524</v>
+        <v>1.015</v>
       </c>
       <c r="S5" t="n">
-        <v>0.9912035779283925</v>
+        <v>0.991</v>
       </c>
       <c r="T5" t="n">
-        <v>1.038483353553608</v>
+        <v>1.038</v>
       </c>
       <c r="U5" t="n">
-        <v>0.2237205265081478</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="6">
@@ -2351,64 +2351,64 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.06152126658165592</v>
+        <v>0.062</v>
       </c>
       <c r="C6" t="n">
-        <v>1.063453112300769</v>
+        <v>1.063</v>
       </c>
       <c r="D6" t="n">
-        <v>1.050319796061982</v>
+        <v>1.05</v>
       </c>
       <c r="E6" t="n">
-        <v>1.076750648995148</v>
+        <v>1.077</v>
       </c>
       <c r="F6" t="n">
-        <v>2.917583082017456e-22</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.129058816677526</v>
+        <v>-0.129</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8789222687376301</v>
+        <v>0.879</v>
       </c>
       <c r="I6" t="n">
-        <v>0.8692633268130041</v>
+        <v>0.869</v>
       </c>
       <c r="J6" t="n">
-        <v>0.8886885373562803</v>
+        <v>0.889</v>
       </c>
       <c r="K6" t="n">
-        <v>5.749179129470247e-116</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.1369727623239789</v>
+        <v>-0.137</v>
       </c>
       <c r="M6" t="n">
-        <v>0.8719939768980852</v>
+        <v>0.872</v>
       </c>
       <c r="N6" t="n">
-        <v>0.8613328043849187</v>
+        <v>0.861</v>
       </c>
       <c r="O6" t="n">
-        <v>0.8827871083924689</v>
+        <v>0.883</v>
       </c>
       <c r="P6" t="n">
-        <v>1.39137430302594e-105</v>
+        <v>0</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.2771126936355022</v>
+        <v>0.277</v>
       </c>
       <c r="R6" t="n">
-        <v>1.319315041066069</v>
+        <v>1.319</v>
       </c>
       <c r="S6" t="n">
-        <v>1.296857383136985</v>
+        <v>1.297</v>
       </c>
       <c r="T6" t="n">
-        <v>1.342161597887365</v>
+        <v>1.342</v>
       </c>
       <c r="U6" t="n">
-        <v>1.225430070503197e-219</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -2418,64 +2418,64 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.4678338514039696</v>
+        <v>0.468</v>
       </c>
       <c r="C7" t="n">
-        <v>1.596532119079311</v>
+        <v>1.597</v>
       </c>
       <c r="D7" t="n">
-        <v>1.578114178404532</v>
+        <v>1.578</v>
       </c>
       <c r="E7" t="n">
-        <v>1.61516501285656</v>
+        <v>1.615</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2943078596261689</v>
+        <v>0.294</v>
       </c>
       <c r="H7" t="n">
-        <v>1.342197048349975</v>
+        <v>1.342</v>
       </c>
       <c r="I7" t="n">
-        <v>1.323361626882998</v>
+        <v>1.323</v>
       </c>
       <c r="J7" t="n">
-        <v>1.361300554590327</v>
+        <v>1.361</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.1210970120014736</v>
+        <v>-0.121</v>
       </c>
       <c r="M7" t="n">
-        <v>0.8859480078343254</v>
+        <v>0.886</v>
       </c>
       <c r="N7" t="n">
-        <v>0.8767141321965571</v>
+        <v>0.877</v>
       </c>
       <c r="O7" t="n">
-        <v>0.8952791380459193</v>
+        <v>0.895</v>
       </c>
       <c r="P7" t="n">
-        <v>1.292712331380647e-113</v>
+        <v>0</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.0569623144390182</v>
+        <v>-0.057</v>
       </c>
       <c r="R7" t="n">
-        <v>0.9446296675946929</v>
+        <v>0.945</v>
       </c>
       <c r="S7" t="n">
-        <v>0.9284933106378921</v>
+        <v>0.928</v>
       </c>
       <c r="T7" t="n">
-        <v>0.9610464595453209</v>
+        <v>0.961</v>
       </c>
       <c r="U7" t="n">
-        <v>9.18971874610572e-11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -2485,64 +2485,64 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.5891912224410345</v>
+        <v>0.589</v>
       </c>
       <c r="C8" t="n">
-        <v>1.802529979905298</v>
+        <v>1.803</v>
       </c>
       <c r="D8" t="n">
-        <v>1.774681569036546</v>
+        <v>1.775</v>
       </c>
       <c r="E8" t="n">
-        <v>1.830815389727239</v>
+        <v>1.831</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.2616913818212654</v>
+        <v>0.262</v>
       </c>
       <c r="H8" t="n">
-        <v>1.299125546795094</v>
+        <v>1.299</v>
       </c>
       <c r="I8" t="n">
-        <v>1.271258177371051</v>
+        <v>1.271</v>
       </c>
       <c r="J8" t="n">
-        <v>1.327603799431091</v>
+        <v>1.328</v>
       </c>
       <c r="K8" t="n">
-        <v>1.090492217111294e-123</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.09407923533636295</v>
+        <v>-0.094</v>
       </c>
       <c r="M8" t="n">
-        <v>0.9102106385373261</v>
+        <v>0.91</v>
       </c>
       <c r="N8" t="n">
-        <v>0.8920229325831146</v>
+        <v>0.892</v>
       </c>
       <c r="O8" t="n">
-        <v>0.9287691787333423</v>
+        <v>0.929</v>
       </c>
       <c r="P8" t="n">
-        <v>6.51310564368565e-20</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>-0.05029707666993567</v>
+        <v>-0.05</v>
       </c>
       <c r="R8" t="n">
-        <v>0.9509468784019436</v>
+        <v>0.951</v>
       </c>
       <c r="S8" t="n">
-        <v>0.9343983024826603</v>
+        <v>0.9340000000000001</v>
       </c>
       <c r="T8" t="n">
-        <v>0.9677885363658203</v>
+        <v>0.968</v>
       </c>
       <c r="U8" t="n">
-        <v>1.96119243058071e-08</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -2552,64 +2552,64 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.6220827950934645</v>
+        <v>0.622</v>
       </c>
       <c r="C9" t="n">
-        <v>1.862803842899598</v>
+        <v>1.863</v>
       </c>
       <c r="D9" t="n">
-        <v>1.843159981600802</v>
+        <v>1.843</v>
       </c>
       <c r="E9" t="n">
-        <v>1.882657062740561</v>
+        <v>1.883</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.3558725408373029</v>
+        <v>0.356</v>
       </c>
       <c r="H9" t="n">
-        <v>1.427425598196931</v>
+        <v>1.427</v>
       </c>
       <c r="I9" t="n">
-        <v>1.404654319573786</v>
+        <v>1.405</v>
       </c>
       <c r="J9" t="n">
-        <v>1.450566028947334</v>
+        <v>1.451</v>
       </c>
       <c r="K9" t="n">
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>0.04366230913122057</v>
+        <v>0.044</v>
       </c>
       <c r="M9" t="n">
-        <v>1.044629533464802</v>
+        <v>1.045</v>
       </c>
       <c r="N9" t="n">
-        <v>1.033954282469157</v>
+        <v>1.034</v>
       </c>
       <c r="O9" t="n">
-        <v>1.055415003051106</v>
+        <v>1.055</v>
       </c>
       <c r="P9" t="n">
-        <v>7.998987835968146e-17</v>
+        <v>0</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.2307326559881326</v>
+        <v>0.231</v>
       </c>
       <c r="R9" t="n">
-        <v>1.259522468644604</v>
+        <v>1.26</v>
       </c>
       <c r="S9" t="n">
-        <v>1.237803528534166</v>
+        <v>1.238</v>
       </c>
       <c r="T9" t="n">
-        <v>1.281622496988067</v>
+        <v>1.282</v>
       </c>
       <c r="U9" t="n">
-        <v>5.113138270294574e-149</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -2619,64 +2619,64 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.6339208977588012</v>
+        <v>0.634</v>
       </c>
       <c r="C10" t="n">
-        <v>1.884986949924063</v>
+        <v>1.885</v>
       </c>
       <c r="D10" t="n">
-        <v>1.865691073927784</v>
+        <v>1.866</v>
       </c>
       <c r="E10" t="n">
-        <v>1.904482393166853</v>
+        <v>1.904</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.3816904105703156</v>
+        <v>0.382</v>
       </c>
       <c r="H10" t="n">
-        <v>1.464758541168988</v>
+        <v>1.465</v>
       </c>
       <c r="I10" t="n">
-        <v>1.430094360949299</v>
+        <v>1.43</v>
       </c>
       <c r="J10" t="n">
-        <v>1.500262949434542</v>
+        <v>1.5</v>
       </c>
       <c r="K10" t="n">
-        <v>3.468820220771773e-214</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.1268749410218407</v>
+        <v>-0.127</v>
       </c>
       <c r="M10" t="n">
-        <v>0.8808438231377959</v>
+        <v>0.881</v>
       </c>
       <c r="N10" t="n">
-        <v>0.8702226822704396</v>
+        <v>0.87</v>
       </c>
       <c r="O10" t="n">
-        <v>0.8915945959207785</v>
+        <v>0.892</v>
       </c>
       <c r="P10" t="n">
-        <v>2.224608982962949e-93</v>
+        <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.1746521819514706</v>
+        <v>0.175</v>
       </c>
       <c r="R10" t="n">
-        <v>1.190831951726556</v>
+        <v>1.191</v>
       </c>
       <c r="S10" t="n">
-        <v>1.17094044860533</v>
+        <v>1.171</v>
       </c>
       <c r="T10" t="n">
-        <v>1.211061364343431</v>
+        <v>1.211</v>
       </c>
       <c r="U10" t="n">
-        <v>8.327684882306311e-92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -2686,64 +2686,64 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.08609264833459444</v>
+        <v>-0.08599999999999999</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9175092215808566</v>
+        <v>0.918</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9058539366283361</v>
+        <v>0.906</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9293144707404433</v>
+        <v>0.929</v>
       </c>
       <c r="F11" t="n">
-        <v>8.935695916525335e-40</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.0721310820851843</v>
+        <v>-0.07199999999999999</v>
       </c>
       <c r="H11" t="n">
-        <v>0.9304089278751347</v>
+        <v>0.93</v>
       </c>
       <c r="I11" t="n">
-        <v>0.9152112822277695</v>
+        <v>0.915</v>
       </c>
       <c r="J11" t="n">
-        <v>0.9458589397659105</v>
+        <v>0.946</v>
       </c>
       <c r="K11" t="n">
-        <v>9.151913301141971e-18</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>0.2011777534764654</v>
+        <v>0.201</v>
       </c>
       <c r="M11" t="n">
-        <v>1.222842116943284</v>
+        <v>1.223</v>
       </c>
       <c r="N11" t="n">
-        <v>1.194375950158264</v>
+        <v>1.194</v>
       </c>
       <c r="O11" t="n">
-        <v>1.25198673229496</v>
+        <v>1.252</v>
       </c>
       <c r="P11" t="n">
-        <v>6.658339082914741e-63</v>
+        <v>0</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.006774804599302983</v>
+        <v>0.007</v>
       </c>
       <c r="R11" t="n">
-        <v>1.006797805500849</v>
+        <v>1.007</v>
       </c>
       <c r="S11" t="n">
-        <v>0.9991378648588995</v>
+        <v>0.999</v>
       </c>
       <c r="T11" t="n">
-        <v>1.014516471462598</v>
+        <v>1.015</v>
       </c>
       <c r="U11" t="n">
-        <v>0.08210184892335767</v>
+        <v>0.082</v>
       </c>
     </row>
     <row r="12">
@@ -2753,61 +2753,61 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.07465257083598953</v>
+        <v>0.075</v>
       </c>
       <c r="C12" t="n">
-        <v>1.07750972754175</v>
+        <v>1.078</v>
       </c>
       <c r="D12" t="n">
-        <v>1.063353767196114</v>
+        <v>1.063</v>
       </c>
       <c r="E12" t="n">
-        <v>1.091854139952438</v>
+        <v>1.092</v>
       </c>
       <c r="F12" t="n">
-        <v>1.878626563941153e-28</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.04224488454997688</v>
+        <v>-0.042</v>
       </c>
       <c r="H12" t="n">
-        <v>0.9586349969263996</v>
+        <v>0.959</v>
       </c>
       <c r="I12" t="n">
-        <v>0.9423003823438562</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="J12" t="n">
-        <v>0.9752527692350353</v>
+        <v>0.975</v>
       </c>
       <c r="K12" t="n">
-        <v>1.452205406422461e-06</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>0.2958245090931514</v>
+        <v>0.296</v>
       </c>
       <c r="M12" t="n">
-        <v>1.344234235246651</v>
+        <v>1.344</v>
       </c>
       <c r="N12" t="n">
-        <v>1.312206168385211</v>
+        <v>1.312</v>
       </c>
       <c r="O12" t="n">
-        <v>1.377044036786373</v>
+        <v>1.377</v>
       </c>
       <c r="P12" t="n">
-        <v>9.72545413075964e-128</v>
+        <v>0</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.2640070487770619</v>
+        <v>0.264</v>
       </c>
       <c r="R12" t="n">
-        <v>1.302137374744604</v>
+        <v>1.302</v>
       </c>
       <c r="S12" t="n">
-        <v>1.291036264922955</v>
+        <v>1.291</v>
       </c>
       <c r="T12" t="n">
-        <v>1.313333938615547</v>
+        <v>1.313</v>
       </c>
       <c r="U12" t="n">
         <v>0</v>
@@ -2820,61 +2820,61 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.2975260969297974</v>
+        <v>0.298</v>
       </c>
       <c r="C13" t="n">
-        <v>1.346523515023897</v>
+        <v>1.347</v>
       </c>
       <c r="D13" t="n">
-        <v>1.328546724429396</v>
+        <v>1.329</v>
       </c>
       <c r="E13" t="n">
-        <v>1.364743552614635</v>
+        <v>1.365</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.02523171821067612</v>
+        <v>-0.025</v>
       </c>
       <c r="H13" t="n">
-        <v>0.9750839411424586</v>
+        <v>0.975</v>
       </c>
       <c r="I13" t="n">
-        <v>0.9581795467773959</v>
+        <v>0.958</v>
       </c>
       <c r="J13" t="n">
-        <v>0.9922865661990555</v>
+        <v>0.992</v>
       </c>
       <c r="K13" t="n">
-        <v>0.004687232321772305</v>
+        <v>0.005</v>
       </c>
       <c r="L13" t="n">
-        <v>0.459528210001001</v>
+        <v>0.46</v>
       </c>
       <c r="M13" t="n">
-        <v>1.583326810999155</v>
+        <v>1.583</v>
       </c>
       <c r="N13" t="n">
-        <v>1.54600790961423</v>
+        <v>1.546</v>
       </c>
       <c r="O13" t="n">
-        <v>1.621546548914034</v>
+        <v>1.622</v>
       </c>
       <c r="P13" t="n">
         <v>0</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.4543485283843884</v>
+        <v>0.454</v>
       </c>
       <c r="R13" t="n">
-        <v>1.575146885217063</v>
+        <v>1.575</v>
       </c>
       <c r="S13" t="n">
-        <v>1.560247823337495</v>
+        <v>1.56</v>
       </c>
       <c r="T13" t="n">
-        <v>1.590188220677513</v>
+        <v>1.59</v>
       </c>
       <c r="U13" t="n">
         <v>0</v>
@@ -2887,61 +2887,61 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.2603983836945576</v>
+        <v>0.26</v>
       </c>
       <c r="C14" t="n">
-        <v>1.297446865396556</v>
+        <v>1.297</v>
       </c>
       <c r="D14" t="n">
-        <v>1.280442605500997</v>
+        <v>1.28</v>
       </c>
       <c r="E14" t="n">
-        <v>1.314676941625743</v>
+        <v>1.315</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0.119512354673235</v>
+        <v>0.12</v>
       </c>
       <c r="H14" t="n">
-        <v>1.126947167045201</v>
+        <v>1.127</v>
       </c>
       <c r="I14" t="n">
-        <v>1.108433190378347</v>
+        <v>1.108</v>
       </c>
       <c r="J14" t="n">
-        <v>1.145770379609171</v>
+        <v>1.146</v>
       </c>
       <c r="K14" t="n">
-        <v>2.129782635885435e-45</v>
+        <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>0.4121663588041479</v>
+        <v>0.412</v>
       </c>
       <c r="M14" t="n">
-        <v>1.510085631473717</v>
+        <v>1.51</v>
       </c>
       <c r="N14" t="n">
-        <v>1.474629264545173</v>
+        <v>1.475</v>
       </c>
       <c r="O14" t="n">
-        <v>1.546394520446951</v>
+        <v>1.546</v>
       </c>
       <c r="P14" t="n">
-        <v>2.228333975367533e-253</v>
+        <v>0</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.5173739872843396</v>
+        <v>0.517</v>
       </c>
       <c r="R14" t="n">
-        <v>1.677616418212638</v>
+        <v>1.678</v>
       </c>
       <c r="S14" t="n">
-        <v>1.66098844955852</v>
+        <v>1.661</v>
       </c>
       <c r="T14" t="n">
-        <v>1.694410847591776</v>
+        <v>1.694</v>
       </c>
       <c r="U14" t="n">
         <v>0</v>
@@ -2954,61 +2954,61 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.8717504375519924</v>
+        <v>0.872</v>
       </c>
       <c r="C15" t="n">
-        <v>2.391092650835305</v>
+        <v>2.391</v>
       </c>
       <c r="D15" t="n">
-        <v>2.328536195490225</v>
+        <v>2.329</v>
       </c>
       <c r="E15" t="n">
-        <v>2.455329694230903</v>
+        <v>2.455</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>0.4741880183605694</v>
+        <v>0.474</v>
       </c>
       <c r="H15" t="n">
-        <v>1.606709049431318</v>
+        <v>1.607</v>
       </c>
       <c r="I15" t="n">
-        <v>1.561454371390804</v>
+        <v>1.561</v>
       </c>
       <c r="J15" t="n">
-        <v>1.653275316156121</v>
+        <v>1.653</v>
       </c>
       <c r="K15" t="n">
-        <v>4.024633522998455e-232</v>
+        <v>0</v>
       </c>
       <c r="L15" t="n">
-        <v>0.4448918650236607</v>
+        <v>0.445</v>
       </c>
       <c r="M15" t="n">
-        <v>1.560321461385475</v>
+        <v>1.56</v>
       </c>
       <c r="N15" t="n">
-        <v>1.499721185466518</v>
+        <v>1.5</v>
       </c>
       <c r="O15" t="n">
-        <v>1.62337045475741</v>
+        <v>1.623</v>
       </c>
       <c r="P15" t="n">
-        <v>2.187747226763028e-107</v>
+        <v>0</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.6370943669946674</v>
+        <v>0.637</v>
       </c>
       <c r="R15" t="n">
-        <v>1.89097839983236</v>
+        <v>1.891</v>
       </c>
       <c r="S15" t="n">
-        <v>1.847210629613227</v>
+        <v>1.847</v>
       </c>
       <c r="T15" t="n">
-        <v>1.935783202688295</v>
+        <v>1.936</v>
       </c>
       <c r="U15" t="n">
         <v>0</v>
@@ -3021,61 +3021,61 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.8640548186055549</v>
+        <v>0.864</v>
       </c>
       <c r="C16" t="n">
-        <v>2.372762334955853</v>
+        <v>2.373</v>
       </c>
       <c r="D16" t="n">
-        <v>2.325924233270744</v>
+        <v>2.326</v>
       </c>
       <c r="E16" t="n">
-        <v>2.420543634935251</v>
+        <v>2.421</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>0.4574747951759584</v>
+        <v>0.457</v>
       </c>
       <c r="H16" t="n">
-        <v>1.580078920027529</v>
+        <v>1.58</v>
       </c>
       <c r="I16" t="n">
-        <v>1.54638432518592</v>
+        <v>1.546</v>
       </c>
       <c r="J16" t="n">
-        <v>1.614507695695372</v>
+        <v>1.615</v>
       </c>
       <c r="K16" t="n">
         <v>0</v>
       </c>
       <c r="L16" t="n">
-        <v>0.5067039036015962</v>
+        <v>0.507</v>
       </c>
       <c r="M16" t="n">
-        <v>1.659811270776363</v>
+        <v>1.66</v>
       </c>
       <c r="N16" t="n">
-        <v>1.600389125342325</v>
+        <v>1.6</v>
       </c>
       <c r="O16" t="n">
-        <v>1.721439749227834</v>
+        <v>1.721</v>
       </c>
       <c r="P16" t="n">
-        <v>2.134680169971962e-163</v>
+        <v>0</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.6502369331049204</v>
+        <v>0.65</v>
       </c>
       <c r="R16" t="n">
-        <v>1.915994737821004</v>
+        <v>1.916</v>
       </c>
       <c r="S16" t="n">
-        <v>1.879898880353713</v>
+        <v>1.88</v>
       </c>
       <c r="T16" t="n">
-        <v>1.952783670293507</v>
+        <v>1.953</v>
       </c>
       <c r="U16" t="n">
         <v>0</v>
@@ -3088,61 +3088,61 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.6349610133173633</v>
+        <v>0.635</v>
       </c>
       <c r="C17" t="n">
-        <v>1.886948574159462</v>
+        <v>1.887</v>
       </c>
       <c r="D17" t="n">
-        <v>1.850458027814983</v>
+        <v>1.85</v>
       </c>
       <c r="E17" t="n">
-        <v>1.924158704494771</v>
+        <v>1.924</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>0.3255971124211982</v>
+        <v>0.326</v>
       </c>
       <c r="H17" t="n">
-        <v>1.38485731465329</v>
+        <v>1.385</v>
       </c>
       <c r="I17" t="n">
-        <v>1.357250703595541</v>
+        <v>1.357</v>
       </c>
       <c r="J17" t="n">
-        <v>1.413025446859693</v>
+        <v>1.413</v>
       </c>
       <c r="K17" t="n">
-        <v>1.975963774801285e-220</v>
+        <v>0</v>
       </c>
       <c r="L17" t="n">
-        <v>0.4158423848672683</v>
+        <v>0.416</v>
       </c>
       <c r="M17" t="n">
-        <v>1.515646961146372</v>
+        <v>1.516</v>
       </c>
       <c r="N17" t="n">
-        <v>1.461952456758607</v>
+        <v>1.462</v>
       </c>
       <c r="O17" t="n">
-        <v>1.571313554153105</v>
+        <v>1.571</v>
       </c>
       <c r="P17" t="n">
-        <v>4.718714182631291e-113</v>
+        <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.5013183229232583</v>
+        <v>0.501</v>
       </c>
       <c r="R17" t="n">
-        <v>1.650896251093606</v>
+        <v>1.651</v>
       </c>
       <c r="S17" t="n">
-        <v>1.619950925990362</v>
+        <v>1.62</v>
       </c>
       <c r="T17" t="n">
-        <v>1.682432713329697</v>
+        <v>1.682</v>
       </c>
       <c r="U17" t="n">
         <v>0</v>
@@ -3155,64 +3155,64 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.3692192260218948</v>
+        <v>0.369</v>
       </c>
       <c r="C18" t="n">
-        <v>1.446604702309475</v>
+        <v>1.447</v>
       </c>
       <c r="D18" t="n">
-        <v>1.415418039188463</v>
+        <v>1.415</v>
       </c>
       <c r="E18" t="n">
-        <v>1.478478517868633</v>
+        <v>1.478</v>
       </c>
       <c r="F18" t="n">
-        <v>9.449975653836508e-242</v>
+        <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>0.04956812229564296</v>
+        <v>0.05</v>
       </c>
       <c r="H18" t="n">
-        <v>1.050817173854828</v>
+        <v>1.051</v>
       </c>
       <c r="I18" t="n">
-        <v>1.028196511516977</v>
+        <v>1.028</v>
       </c>
       <c r="J18" t="n">
-        <v>1.073935498224082</v>
+        <v>1.074</v>
       </c>
       <c r="K18" t="n">
-        <v>8.032290906367971e-06</v>
+        <v>0</v>
       </c>
       <c r="L18" t="n">
-        <v>0.1546459836107598</v>
+        <v>0.155</v>
       </c>
       <c r="M18" t="n">
-        <v>1.167244664211121</v>
+        <v>1.167</v>
       </c>
       <c r="N18" t="n">
-        <v>1.123882052451021</v>
+        <v>1.124</v>
       </c>
       <c r="O18" t="n">
-        <v>1.212280330625449</v>
+        <v>1.212</v>
       </c>
       <c r="P18" t="n">
-        <v>1.180926237162219e-15</v>
+        <v>0</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.3005192481228063</v>
+        <v>0.301</v>
       </c>
       <c r="R18" t="n">
-        <v>1.350559901232921</v>
+        <v>1.351</v>
       </c>
       <c r="S18" t="n">
-        <v>1.321418738087785</v>
+        <v>1.321</v>
       </c>
       <c r="T18" t="n">
-        <v>1.380343712590145</v>
+        <v>1.38</v>
       </c>
       <c r="U18" t="n">
-        <v>1.392270681037907e-160</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -3222,61 +3222,61 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.8923333567973833</v>
+        <v>0.892</v>
       </c>
       <c r="C19" t="n">
-        <v>2.440818311870621</v>
+        <v>2.441</v>
       </c>
       <c r="D19" t="n">
-        <v>2.389134712314726</v>
+        <v>2.389</v>
       </c>
       <c r="E19" t="n">
-        <v>2.493619970801437</v>
+        <v>2.494</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>0.409444679495961</v>
+        <v>0.409</v>
       </c>
       <c r="H19" t="n">
-        <v>1.505981250594812</v>
+        <v>1.506</v>
       </c>
       <c r="I19" t="n">
-        <v>1.474393776410867</v>
+        <v>1.474</v>
       </c>
       <c r="J19" t="n">
-        <v>1.538245456152211</v>
+        <v>1.538</v>
       </c>
       <c r="K19" t="n">
         <v>0</v>
       </c>
       <c r="L19" t="n">
-        <v>0.4863679009000634</v>
+        <v>0.486</v>
       </c>
       <c r="M19" t="n">
-        <v>1.626398239533651</v>
+        <v>1.626</v>
       </c>
       <c r="N19" t="n">
-        <v>1.567086367391125</v>
+        <v>1.567</v>
       </c>
       <c r="O19" t="n">
-        <v>1.687954977211514</v>
+        <v>1.688</v>
       </c>
       <c r="P19" t="n">
-        <v>3.272026872140047e-145</v>
+        <v>0</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.7349902471026686</v>
+        <v>0.735</v>
       </c>
       <c r="R19" t="n">
-        <v>2.085461653112453</v>
+        <v>2.085</v>
       </c>
       <c r="S19" t="n">
-        <v>2.0439974965356</v>
+        <v>2.044</v>
       </c>
       <c r="T19" t="n">
-        <v>2.127766943929217</v>
+        <v>2.128</v>
       </c>
       <c r="U19" t="n">
         <v>0</v>
@@ -3289,61 +3289,61 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.1959643287994745</v>
+        <v>0.196</v>
       </c>
       <c r="C20" t="n">
-        <v>1.216483511133098</v>
+        <v>1.216</v>
       </c>
       <c r="D20" t="n">
-        <v>1.194722997448667</v>
+        <v>1.195</v>
       </c>
       <c r="E20" t="n">
-        <v>1.238640367699369</v>
+        <v>1.239</v>
       </c>
       <c r="F20" t="n">
-        <v>1.781792304579433e-100</v>
+        <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>0.610558857960902</v>
+        <v>0.611</v>
       </c>
       <c r="H20" t="n">
-        <v>1.841460225977698</v>
+        <v>1.841</v>
       </c>
       <c r="I20" t="n">
-        <v>1.804203163638946</v>
+        <v>1.804</v>
       </c>
       <c r="J20" t="n">
-        <v>1.879486652167533</v>
+        <v>1.879</v>
       </c>
       <c r="K20" t="n">
         <v>0</v>
       </c>
       <c r="L20" t="n">
-        <v>-0.009424285493698194</v>
+        <v>-0.008999999999999999</v>
       </c>
       <c r="M20" t="n">
-        <v>0.9906199839065294</v>
+        <v>0.991</v>
       </c>
       <c r="N20" t="n">
-        <v>0.9711735511369559</v>
+        <v>0.971</v>
       </c>
       <c r="O20" t="n">
-        <v>1.010455805109323</v>
+        <v>1.01</v>
       </c>
       <c r="P20" t="n">
-        <v>0.3515031631673116</v>
+        <v>0.352</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.5940403188138854</v>
+        <v>0.594</v>
       </c>
       <c r="R20" t="n">
-        <v>1.811291847895276</v>
+        <v>1.811</v>
       </c>
       <c r="S20" t="n">
-        <v>1.780626828848865</v>
+        <v>1.781</v>
       </c>
       <c r="T20" t="n">
-        <v>1.842484963776959</v>
+        <v>1.842</v>
       </c>
       <c r="U20" t="n">
         <v>0</v>
@@ -3356,61 +3356,61 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.5116283490096447</v>
+        <v>0.512</v>
       </c>
       <c r="C21" t="n">
-        <v>1.668005079189647</v>
+        <v>1.668</v>
       </c>
       <c r="D21" t="n">
-        <v>1.642830633430301</v>
+        <v>1.643</v>
       </c>
       <c r="E21" t="n">
-        <v>1.693565293698609</v>
+        <v>1.694</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>0.4806473634864291</v>
+        <v>0.481</v>
       </c>
       <c r="H21" t="n">
-        <v>1.617120928457123</v>
+        <v>1.617</v>
       </c>
       <c r="I21" t="n">
-        <v>1.595645303848527</v>
+        <v>1.596</v>
       </c>
       <c r="J21" t="n">
-        <v>1.638885591269396</v>
+        <v>1.639</v>
       </c>
       <c r="K21" t="n">
         <v>0</v>
       </c>
       <c r="L21" t="n">
-        <v>0.2100274559687103</v>
+        <v>0.21</v>
       </c>
       <c r="M21" t="n">
-        <v>1.233711932247952</v>
+        <v>1.234</v>
       </c>
       <c r="N21" t="n">
-        <v>1.210867695431645</v>
+        <v>1.211</v>
       </c>
       <c r="O21" t="n">
-        <v>1.256987148565726</v>
+        <v>1.257</v>
       </c>
       <c r="P21" t="n">
-        <v>1.671877867162879e-107</v>
+        <v>0</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.4239058132736783</v>
+        <v>0.424</v>
       </c>
       <c r="R21" t="n">
-        <v>1.527917677442532</v>
+        <v>1.528</v>
       </c>
       <c r="S21" t="n">
-        <v>1.507852653571316</v>
+        <v>1.508</v>
       </c>
       <c r="T21" t="n">
-        <v>1.548249706967117</v>
+        <v>1.548</v>
       </c>
       <c r="U21" t="n">
         <v>0</v>
@@ -3423,61 +3423,61 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.4359309841668835</v>
+        <v>0.436</v>
       </c>
       <c r="C22" t="n">
-        <v>1.546402064839555</v>
+        <v>1.546</v>
       </c>
       <c r="D22" t="n">
-        <v>1.535089956947886</v>
+        <v>1.535</v>
       </c>
       <c r="E22" t="n">
-        <v>1.55779753187534</v>
+        <v>1.558</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>0.1608721137566858</v>
+        <v>0.161</v>
       </c>
       <c r="H22" t="n">
-        <v>1.174534752371645</v>
+        <v>1.175</v>
       </c>
       <c r="I22" t="n">
-        <v>1.164602947177257</v>
+        <v>1.165</v>
       </c>
       <c r="J22" t="n">
-        <v>1.184551256608448</v>
+        <v>1.185</v>
       </c>
       <c r="K22" t="n">
-        <v>9.251637420810133e-302</v>
+        <v>0</v>
       </c>
       <c r="L22" t="n">
-        <v>0.4519370166336235</v>
+        <v>0.452</v>
       </c>
       <c r="M22" t="n">
-        <v>1.571352976360663</v>
+        <v>1.571</v>
       </c>
       <c r="N22" t="n">
-        <v>1.553910983625445</v>
+        <v>1.554</v>
       </c>
       <c r="O22" t="n">
-        <v>1.588990748077934</v>
+        <v>1.589</v>
       </c>
       <c r="P22" t="n">
         <v>0</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.2964648864466646</v>
+        <v>0.296</v>
       </c>
       <c r="R22" t="n">
-        <v>1.345095328091472</v>
+        <v>1.345</v>
       </c>
       <c r="S22" t="n">
-        <v>1.333247405673996</v>
+        <v>1.333</v>
       </c>
       <c r="T22" t="n">
-        <v>1.357048537243439</v>
+        <v>1.357</v>
       </c>
       <c r="U22" t="n">
         <v>0</v>
@@ -3490,61 +3490,61 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.1786937304378252</v>
+        <v>0.179</v>
       </c>
       <c r="C23" t="n">
-        <v>1.195654495506487</v>
+        <v>1.196</v>
       </c>
       <c r="D23" t="n">
-        <v>1.174939250700343</v>
+        <v>1.175</v>
       </c>
       <c r="E23" t="n">
-        <v>1.216734968869871</v>
+        <v>1.217</v>
       </c>
       <c r="F23" t="n">
-        <v>2.500597716905403e-89</v>
+        <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.1055921953037176</v>
+        <v>-0.106</v>
       </c>
       <c r="H23" t="n">
-        <v>0.8997915124707888</v>
+        <v>0.9</v>
       </c>
       <c r="I23" t="n">
-        <v>0.8799213119534667</v>
+        <v>0.88</v>
       </c>
       <c r="J23" t="n">
-        <v>0.9201104177339048</v>
+        <v>0.92</v>
       </c>
       <c r="K23" t="n">
-        <v>1.899147908553644e-20</v>
+        <v>0</v>
       </c>
       <c r="L23" t="n">
-        <v>0.03060543748280943</v>
+        <v>0.031</v>
       </c>
       <c r="M23" t="n">
-        <v>1.03107859864972</v>
+        <v>1.031</v>
       </c>
       <c r="N23" t="n">
-        <v>1.014097349253362</v>
+        <v>1.014</v>
       </c>
       <c r="O23" t="n">
-        <v>1.0483442022368</v>
+        <v>1.048</v>
       </c>
       <c r="P23" t="n">
-        <v>0.000303649662831825</v>
+        <v>0</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.4909972047807827</v>
+        <v>0.491</v>
       </c>
       <c r="R23" t="n">
-        <v>1.633944785365318</v>
+        <v>1.634</v>
       </c>
       <c r="S23" t="n">
-        <v>1.608848978173048</v>
+        <v>1.609</v>
       </c>
       <c r="T23" t="n">
-        <v>1.659432052257769</v>
+        <v>1.659</v>
       </c>
       <c r="U23" t="n">
         <v>0</v>
@@ -3610,16 +3610,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.4691055946554749</v>
+        <v>0.4691</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5892046467577909</v>
+        <v>0.5891999999999999</v>
       </c>
       <c r="E2" t="n">
-        <v>2825877.609096161</v>
+        <v>2825877.6091</v>
       </c>
       <c r="F2" t="n">
-        <v>2826076.809213218</v>
+        <v>2826076.8092</v>
       </c>
     </row>
     <row r="3">
@@ -3630,32 +3630,36 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.4735024248024569</v>
+        <v>0.4735</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5833762761602982</v>
+        <v>0.5834</v>
       </c>
       <c r="E3"/>
       <c r="F3"/>
     </row>
     <row r="4">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Rice</t>
+        </is>
+      </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
           <t>Calibration</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.4691055946554749</v>
+        <v>0.4086</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5892046467577909</v>
+        <v>0.4949</v>
       </c>
       <c r="E4" t="n">
-        <v>2825877.609096161</v>
+        <v>1330173.2186</v>
       </c>
       <c r="F4" t="n">
-        <v>2826076.809213218</v>
+        <v>1330357.7948</v>
       </c>
     </row>
     <row r="5">
@@ -3666,10 +3670,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.4735024248024569</v>
+        <v>0.4048</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5833762761602982</v>
+        <v>0.4977</v>
       </c>
       <c r="E5"/>
       <c r="F5"/>
@@ -3677,7 +3681,7 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Rice</t>
+          <t>Soybean</t>
         </is>
       </c>
       <c r="B6" s="1" t="inlineStr">
@@ -3686,16 +3690,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.4086396766888927</v>
+        <v>0.3125</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4948846247822669</v>
+        <v>0.3926</v>
       </c>
       <c r="E6" t="n">
-        <v>1330173.218601608</v>
+        <v>1011746.8437</v>
       </c>
       <c r="F6" t="n">
-        <v>1330357.794808741</v>
+        <v>1011927.6329</v>
       </c>
     </row>
     <row r="7">
@@ -3706,32 +3710,36 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.4047994053055386</v>
+        <v>0.3223</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4976633148876741</v>
+        <v>0.3904</v>
       </c>
       <c r="E7"/>
       <c r="F7"/>
     </row>
     <row r="8">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
           <t>Calibration</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.4086396766888927</v>
+        <v>0.3681</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4948846247822669</v>
+        <v>0.5241</v>
       </c>
       <c r="E8" t="n">
-        <v>1330173.218601608</v>
+        <v>2882944.5953</v>
       </c>
       <c r="F8" t="n">
-        <v>1330357.794808741</v>
+        <v>2883145.2709</v>
       </c>
     </row>
     <row r="9">
@@ -3742,172 +3750,20 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.4047994053055386</v>
+        <v>0.3641</v>
       </c>
       <c r="D9" t="n">
-        <v>0.4976633148876741</v>
+        <v>0.5243</v>
       </c>
       <c r="E9"/>
       <c r="F9"/>
     </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>Soybean</t>
-        </is>
-      </c>
-      <c r="B10" s="1" t="inlineStr">
-        <is>
-          <t>Calibration</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>0.3125345491357727</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.3926494020479137</v>
-      </c>
-      <c r="E10" t="n">
-        <v>1011746.843656312</v>
-      </c>
-      <c r="F10" t="n">
-        <v>1011927.632853311</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="inlineStr">
-        <is>
-          <t>Validation</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>0.3223258184124012</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.390429794899244</v>
-      </c>
-      <c r="E11"/>
-      <c r="F11"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1" t="inlineStr">
-        <is>
-          <t>Calibration</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>0.3125345491357727</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.3926494020479137</v>
-      </c>
-      <c r="E12" t="n">
-        <v>1011746.843656312</v>
-      </c>
-      <c r="F12" t="n">
-        <v>1011927.632853311</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1" t="inlineStr">
-        <is>
-          <t>Validation</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>0.3223258184124012</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.390429794899244</v>
-      </c>
-      <c r="E13"/>
-      <c r="F13"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>Wheat</t>
-        </is>
-      </c>
-      <c r="B14" s="1" t="inlineStr">
-        <is>
-          <t>Calibration</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>0.3680774688245015</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0.5240906756102784</v>
-      </c>
-      <c r="E14" t="n">
-        <v>2882944.595284296</v>
-      </c>
-      <c r="F14" t="n">
-        <v>2883145.270936384</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1" t="inlineStr">
-        <is>
-          <t>Validation</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>0.364135129460144</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0.5242647678344248</v>
-      </c>
-      <c r="E15"/>
-      <c r="F15"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1" t="inlineStr">
-        <is>
-          <t>Calibration</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>0.3680774688245015</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0.5240906756102784</v>
-      </c>
-      <c r="E16" t="n">
-        <v>2882944.595284296</v>
-      </c>
-      <c r="F16" t="n">
-        <v>2883145.270936384</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1" t="inlineStr">
-        <is>
-          <t>Validation</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>0.364135129460144</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0.5242647678344248</v>
-      </c>
-      <c r="E17"/>
-      <c r="F17"/>
-    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -3957,16 +3813,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.1779584426355613</v>
+        <v>-0.178</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.4569527020493327</v>
+        <v>-0.457</v>
       </c>
       <c r="D2" t="n">
-        <v>0.009468833908120144</v>
+        <v>0.0095</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.4479078558422933</v>
+        <v>-0.4479</v>
       </c>
     </row>
     <row r="3">
@@ -3976,16 +3832,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.1636382669825838</v>
+        <v>-0.1636</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1113687804412284</v>
+        <v>0.1114</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.03014509379986741</v>
+        <v>-0.0301</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.3879849722653365</v>
+        <v>-0.388</v>
       </c>
     </row>
     <row r="4">
@@ -3995,16 +3851,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.4004814418875564</v>
+        <v>-0.4005</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.381617056335942</v>
+        <v>-0.3816</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.1894380090999936</v>
+        <v>-0.1894</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.345514477145242</v>
+        <v>-0.3455</v>
       </c>
     </row>
     <row r="5">
@@ -4014,16 +3870,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.3533376456634922</v>
+        <v>-0.3533</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.148599053386214</v>
+        <v>-0.1486</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.363605749284884</v>
+        <v>-0.3636</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.2565582683133087</v>
+        <v>-0.2566</v>
       </c>
     </row>
   </sheetData>
@@ -4101,49 +3957,49 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>2.71193498786088</v>
+        <v>2.71</v>
       </c>
       <c r="D2" t="n">
-        <v>1.64679536915212</v>
+        <v>1.65</v>
       </c>
       <c r="E2" t="n">
-        <v>2.71193498786088</v>
+        <v>2.71</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>2.61672967511951</v>
+        <v>2.62</v>
       </c>
       <c r="H2" t="n">
-        <v>1.61763088345874</v>
+        <v>1.62</v>
       </c>
       <c r="I2" t="n">
-        <v>2.61672967511951</v>
+        <v>2.62</v>
       </c>
       <c r="J2" t="n">
         <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>2.89312973704457</v>
+        <v>2.89</v>
       </c>
       <c r="L2" t="n">
-        <v>1.70092026181258</v>
+        <v>1.7</v>
       </c>
       <c r="M2" t="n">
-        <v>2.89312973704457</v>
+        <v>2.89</v>
       </c>
       <c r="N2" t="n">
         <v>1</v>
       </c>
       <c r="O2" t="n">
-        <v>2.50661923033399</v>
+        <v>2.51</v>
       </c>
       <c r="P2" t="n">
-        <v>1.58323063080967</v>
+        <v>1.58</v>
       </c>
       <c r="Q2" t="n">
-        <v>2.50661923033399</v>
+        <v>2.51</v>
       </c>
     </row>
     <row r="3">
@@ -4154,49 +4010,49 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>2.30550444759329</v>
+        <v>2.31</v>
       </c>
       <c r="D3" t="n">
-        <v>1.51838876694781</v>
+        <v>1.52</v>
       </c>
       <c r="E3" t="n">
-        <v>2.30550444759329</v>
+        <v>2.31</v>
       </c>
       <c r="F3" t="n">
         <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>2.00153437629713</v>
+        <v>2</v>
       </c>
       <c r="H3" t="n">
-        <v>1.41475594230847</v>
+        <v>1.41</v>
       </c>
       <c r="I3" t="n">
-        <v>2.00153437629713</v>
+        <v>2</v>
       </c>
       <c r="J3" t="n">
         <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>2.24715452220963</v>
+        <v>2.25</v>
       </c>
       <c r="L3" t="n">
-        <v>1.49905120733403</v>
+        <v>1.5</v>
       </c>
       <c r="M3" t="n">
-        <v>2.24715452220963</v>
+        <v>2.25</v>
       </c>
       <c r="N3" t="n">
         <v>1</v>
       </c>
       <c r="O3" t="n">
-        <v>2.6996832382275</v>
+        <v>2.7</v>
       </c>
       <c r="P3" t="n">
-        <v>1.64307128215044</v>
+        <v>1.64</v>
       </c>
       <c r="Q3" t="n">
-        <v>2.6996832382275</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="4">
@@ -4207,49 +4063,49 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>1.63259989417477</v>
+        <v>1.63</v>
       </c>
       <c r="D4" t="n">
-        <v>1.27773232493147</v>
+        <v>1.28</v>
       </c>
       <c r="E4" t="n">
-        <v>1.63259989417477</v>
+        <v>1.63</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>1.30530027241378</v>
+        <v>1.31</v>
       </c>
       <c r="H4" t="n">
-        <v>1.14249738398553</v>
+        <v>1.14</v>
       </c>
       <c r="I4" t="n">
-        <v>1.30530027241378</v>
+        <v>1.31</v>
       </c>
       <c r="J4" t="n">
         <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>2.54876180317693</v>
+        <v>2.55</v>
       </c>
       <c r="L4" t="n">
-        <v>1.59648420072888</v>
+        <v>1.6</v>
       </c>
       <c r="M4" t="n">
-        <v>2.54876180317693</v>
+        <v>2.55</v>
       </c>
       <c r="N4" t="n">
         <v>1</v>
       </c>
       <c r="O4" t="n">
-        <v>2.24898951816017</v>
+        <v>2.25</v>
       </c>
       <c r="P4" t="n">
-        <v>1.49966313489402</v>
+        <v>1.5</v>
       </c>
       <c r="Q4" t="n">
-        <v>2.24898951816017</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="5">
@@ -4260,49 +4116,49 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>2.44843296523841</v>
+        <v>2.45</v>
       </c>
       <c r="D5" t="n">
-        <v>1.56474693328934</v>
+        <v>1.56</v>
       </c>
       <c r="E5" t="n">
-        <v>2.44843296523841</v>
+        <v>2.45</v>
       </c>
       <c r="F5" t="n">
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>2.69073780298122</v>
+        <v>2.69</v>
       </c>
       <c r="H5" t="n">
-        <v>1.64034685447353</v>
+        <v>1.64</v>
       </c>
       <c r="I5" t="n">
-        <v>2.69073780298122</v>
+        <v>2.69</v>
       </c>
       <c r="J5" t="n">
         <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>1.99082991607438</v>
+        <v>1.99</v>
       </c>
       <c r="L5" t="n">
-        <v>1.41096772325748</v>
+        <v>1.41</v>
       </c>
       <c r="M5" t="n">
-        <v>1.99082991607438</v>
+        <v>1.99</v>
       </c>
       <c r="N5" t="n">
         <v>1</v>
       </c>
       <c r="O5" t="n">
-        <v>1.9384353948108</v>
+        <v>1.94</v>
       </c>
       <c r="P5" t="n">
-        <v>1.39227705389797</v>
+        <v>1.39</v>
       </c>
       <c r="Q5" t="n">
-        <v>1.9384353948108</v>
+        <v>1.94</v>
       </c>
     </row>
     <row r="6">
@@ -4313,49 +4169,49 @@
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>3.42576057199118</v>
+        <v>3.43</v>
       </c>
       <c r="D6" t="n">
-        <v>1.1080595059969</v>
+        <v>1.11</v>
       </c>
       <c r="E6" t="n">
-        <v>1.2277958688301</v>
+        <v>1.23</v>
       </c>
       <c r="F6" t="n">
         <v>6</v>
       </c>
       <c r="G6" t="n">
-        <v>4.04119753548385</v>
+        <v>4.04</v>
       </c>
       <c r="H6" t="n">
-        <v>1.12342091924423</v>
+        <v>1.12</v>
       </c>
       <c r="I6" t="n">
-        <v>1.26207456179555</v>
+        <v>1.26</v>
       </c>
       <c r="J6" t="n">
         <v>6</v>
       </c>
       <c r="K6" t="n">
-        <v>4.31297626968293</v>
+        <v>4.31</v>
       </c>
       <c r="L6" t="n">
-        <v>1.12953082941685</v>
+        <v>1.13</v>
       </c>
       <c r="M6" t="n">
-        <v>1.27583989460311</v>
+        <v>1.28</v>
       </c>
       <c r="N6" t="n">
         <v>6</v>
       </c>
       <c r="O6" t="n">
-        <v>3.4890316678403</v>
+        <v>3.49</v>
       </c>
       <c r="P6" t="n">
-        <v>1.1097506530751</v>
+        <v>1.11</v>
       </c>
       <c r="Q6" t="n">
-        <v>1.23154651200062</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="7">
@@ -4366,49 +4222,49 @@
         <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>1.61104397300311</v>
+        <v>1.61</v>
       </c>
       <c r="D7" t="n">
-        <v>1.06142282936737</v>
+        <v>1.06</v>
       </c>
       <c r="E7" t="n">
-        <v>1.12661842270222</v>
+        <v>1.13</v>
       </c>
       <c r="F7" t="n">
         <v>4</v>
       </c>
       <c r="G7" t="n">
-        <v>2.05823775922541</v>
+        <v>2.06</v>
       </c>
       <c r="H7" t="n">
-        <v>1.09442736265586</v>
+        <v>1.09</v>
       </c>
       <c r="I7" t="n">
-        <v>1.19777125212986</v>
+        <v>1.2</v>
       </c>
       <c r="J7" t="n">
         <v>4</v>
       </c>
       <c r="K7" t="n">
-        <v>2.09336761144225</v>
+        <v>2.09</v>
       </c>
       <c r="L7" t="n">
-        <v>1.0967450616279</v>
+        <v>1.1</v>
       </c>
       <c r="M7" t="n">
-        <v>1.20284973020519</v>
+        <v>1.2</v>
       </c>
       <c r="N7" t="n">
         <v>4</v>
       </c>
       <c r="O7" t="n">
-        <v>1.79670947393228</v>
+        <v>1.8</v>
       </c>
       <c r="P7" t="n">
-        <v>1.07599370918285</v>
+        <v>1.08</v>
       </c>
       <c r="Q7" t="n">
-        <v>1.15776246220107</v>
+        <v>1.16</v>
       </c>
     </row>
     <row r="8">
@@ -4419,49 +4275,49 @@
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>3.15985652488177</v>
+        <v>3.16</v>
       </c>
       <c r="D8" t="n">
-        <v>1.12193251956872</v>
+        <v>1.12</v>
       </c>
       <c r="E8" t="n">
-        <v>1.25873257846582</v>
+        <v>1.26</v>
       </c>
       <c r="F8" t="n">
         <v>5</v>
       </c>
       <c r="G8" t="n">
-        <v>2.62021299999999</v>
+        <v>2.62</v>
       </c>
       <c r="H8" t="n">
-        <v>1.10111748679652</v>
+        <v>1.1</v>
       </c>
       <c r="I8" t="n">
-        <v>1.21245971972909</v>
+        <v>1.21</v>
       </c>
       <c r="J8" t="n">
         <v>5</v>
       </c>
       <c r="K8" t="n">
-        <v>4.22480137765604</v>
+        <v>4.22</v>
       </c>
       <c r="L8" t="n">
-        <v>1.1549963974175</v>
+        <v>1.15</v>
       </c>
       <c r="M8" t="n">
-        <v>1.33401667804739</v>
+        <v>1.33</v>
       </c>
       <c r="N8" t="n">
         <v>5</v>
       </c>
       <c r="O8" t="n">
-        <v>3.42427757256006</v>
+        <v>3.42</v>
       </c>
       <c r="P8" t="n">
-        <v>1.13098513314866</v>
+        <v>1.13</v>
       </c>
       <c r="Q8" t="n">
-        <v>1.2791273714033</v>
+        <v>1.28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>